<commit_message>
Digitized hood et al 2020 up to density
</commit_message>
<xml_diff>
--- a/data/web_plot_digitizer_data.xlsx
+++ b/data/web_plot_digitizer_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramR\dnr_report\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramR\fuels_longevity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E74A79D-87A6-4EDB-A800-DBCBE950608C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE5132A-9960-4FF4-8339-A8A7A0340A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6245A06B-15CE-492B-AD18-D354A95DB25A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="36">
   <si>
     <t>variable</t>
   </si>
@@ -127,6 +127,27 @@
   <si>
     <t>interior_pnw</t>
   </si>
+  <si>
+    <t>wet burn</t>
+  </si>
+  <si>
+    <t>dry burn</t>
+  </si>
+  <si>
+    <t>shelterwood</t>
+  </si>
+  <si>
+    <t>cwd</t>
+  </si>
+  <si>
+    <t>litterduff</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>trees/ha</t>
+  </si>
 </sst>
 </file>
 
@@ -188,6 +209,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>422019</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>149624</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D12E4CD-9B7F-4DA4-BAEE-4AE263FEA281}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13310577" y="1113692"/>
+          <a:ext cx="1657143" cy="323810"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -487,15 +557,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A8627B-2386-4DAF-99DA-19F1EA4382AF}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.21875" customWidth="1"/>
+    <col min="1" max="1" width="34" customWidth="1"/>
     <col min="2" max="2" width="13.88671875" customWidth="1"/>
     <col min="3" max="3" width="13.109375" customWidth="1"/>
     <col min="4" max="8" width="12.6640625" customWidth="1"/>
@@ -923,9 +993,2788 @@
         <v>24</v>
       </c>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>0.56679389312977002</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>0.52671755725190805</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>26</v>
+      </c>
+      <c r="H15" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>0.85877862595419796</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>0.55534351145038097</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>22</v>
+      </c>
+      <c r="E17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>0.95038167938931295</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" t="s">
+        <v>28</v>
+      </c>
+      <c r="I18" t="s">
+        <v>14</v>
+      </c>
+      <c r="J18" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>0.44083969465648798</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" t="s">
+        <v>28</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>0.58396946564885399</v>
+      </c>
+      <c r="B20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G20" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" t="s">
+        <v>28</v>
+      </c>
+      <c r="I20" t="s">
+        <v>14</v>
+      </c>
+      <c r="J20" t="s">
+        <v>31</v>
+      </c>
+      <c r="K20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>0.30916030534351102</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+      <c r="H21" t="s">
+        <v>28</v>
+      </c>
+      <c r="I21" t="s">
+        <v>14</v>
+      </c>
+      <c r="J21" t="s">
+        <v>31</v>
+      </c>
+      <c r="K21" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>1.1393129770992301</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" t="s">
+        <v>26</v>
+      </c>
+      <c r="H22" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" t="s">
+        <v>31</v>
+      </c>
+      <c r="K22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>0.61545801526717503</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H23" t="s">
+        <v>28</v>
+      </c>
+      <c r="I23" t="s">
+        <v>14</v>
+      </c>
+      <c r="J23" t="s">
+        <v>31</v>
+      </c>
+      <c r="K23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>0.48377862595419802</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" t="s">
+        <v>16</v>
+      </c>
+      <c r="G24" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" t="s">
+        <v>31</v>
+      </c>
+      <c r="K24" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>0.41507633587786202</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25">
+        <v>22</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" t="s">
+        <v>26</v>
+      </c>
+      <c r="H25" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" t="s">
+        <v>14</v>
+      </c>
+      <c r="J25" t="s">
+        <v>31</v>
+      </c>
+      <c r="K25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>0.86283185840707899</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26">
+        <v>12</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" t="s">
+        <v>26</v>
+      </c>
+      <c r="H26" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" t="s">
+        <v>13</v>
+      </c>
+      <c r="J26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>0.428097345132744</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" t="s">
+        <v>13</v>
+      </c>
+      <c r="J27" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>1.4269911504424699</v>
+      </c>
+      <c r="B28" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" t="s">
+        <v>26</v>
+      </c>
+      <c r="H28" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" t="s">
+        <v>13</v>
+      </c>
+      <c r="J28" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>0.51769911504424804</v>
+      </c>
+      <c r="B29" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>22</v>
+      </c>
+      <c r="E29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" t="s">
+        <v>13</v>
+      </c>
+      <c r="J29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>1.31747787610619</v>
+      </c>
+      <c r="B30" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>0.44800884955752202</v>
+      </c>
+      <c r="B31" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" t="s">
+        <v>16</v>
+      </c>
+      <c r="G31" t="s">
+        <v>26</v>
+      </c>
+      <c r="H31" t="s">
+        <v>28</v>
+      </c>
+      <c r="I31" t="s">
+        <v>14</v>
+      </c>
+      <c r="J31" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>0.46792035398230097</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G32" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" t="s">
+        <v>14</v>
+      </c>
+      <c r="J32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>0.31194690265486802</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>22</v>
+      </c>
+      <c r="E33" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" t="s">
+        <v>26</v>
+      </c>
+      <c r="H33" t="s">
+        <v>28</v>
+      </c>
+      <c r="I33" t="s">
+        <v>14</v>
+      </c>
+      <c r="J33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>0.87610619469026496</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" t="s">
+        <v>16</v>
+      </c>
+      <c r="G34" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" t="s">
+        <v>28</v>
+      </c>
+      <c r="I34" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>0.10951327433628399</v>
+      </c>
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" t="s">
+        <v>16</v>
+      </c>
+      <c r="G35" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" t="s">
+        <v>28</v>
+      </c>
+      <c r="I35" t="s">
+        <v>15</v>
+      </c>
+      <c r="J35" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>0.50442477876106195</v>
+      </c>
+      <c r="B36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" t="s">
+        <v>16</v>
+      </c>
+      <c r="G36" t="s">
+        <v>26</v>
+      </c>
+      <c r="H36" t="s">
+        <v>28</v>
+      </c>
+      <c r="I36" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>0.47455752212389402</v>
+      </c>
+      <c r="B37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>22</v>
+      </c>
+      <c r="E37" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" t="s">
+        <v>26</v>
+      </c>
+      <c r="H37" t="s">
+        <v>28</v>
+      </c>
+      <c r="I37" t="s">
+        <v>15</v>
+      </c>
+      <c r="J37" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>1.4869888475836399</v>
+      </c>
+      <c r="B38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" t="s">
+        <v>26</v>
+      </c>
+      <c r="H38" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" t="s">
+        <v>13</v>
+      </c>
+      <c r="J38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>1.4721189591078001</v>
+      </c>
+      <c r="B39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39">
+        <v>22</v>
+      </c>
+      <c r="E39" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" t="s">
+        <v>16</v>
+      </c>
+      <c r="G39" t="s">
+        <v>26</v>
+      </c>
+      <c r="H39" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" t="s">
+        <v>13</v>
+      </c>
+      <c r="J39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>1.0855018587360501</v>
+      </c>
+      <c r="B40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>12</v>
+      </c>
+      <c r="E40" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" t="s">
+        <v>16</v>
+      </c>
+      <c r="G40" t="s">
+        <v>26</v>
+      </c>
+      <c r="H40" t="s">
+        <v>28</v>
+      </c>
+      <c r="I40" t="s">
+        <v>13</v>
+      </c>
+      <c r="J40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>1.62825278810408</v>
+      </c>
+      <c r="B41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41">
+        <v>22</v>
+      </c>
+      <c r="E41" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" t="s">
+        <v>16</v>
+      </c>
+      <c r="G41" t="s">
+        <v>26</v>
+      </c>
+      <c r="H41" t="s">
+        <v>28</v>
+      </c>
+      <c r="I41" t="s">
+        <v>13</v>
+      </c>
+      <c r="J41" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>0.40892193308550101</v>
+      </c>
+      <c r="B42" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" t="s">
+        <v>26</v>
+      </c>
+      <c r="H42" t="s">
+        <v>28</v>
+      </c>
+      <c r="I42" t="s">
+        <v>14</v>
+      </c>
+      <c r="J42" t="s">
+        <v>31</v>
+      </c>
+      <c r="K42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>0.12639405204460899</v>
+      </c>
+      <c r="B43" t="s">
+        <v>32</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" t="s">
+        <v>16</v>
+      </c>
+      <c r="G43" t="s">
+        <v>26</v>
+      </c>
+      <c r="H43" t="s">
+        <v>28</v>
+      </c>
+      <c r="I43" t="s">
+        <v>14</v>
+      </c>
+      <c r="J43" t="s">
+        <v>31</v>
+      </c>
+      <c r="K43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>1.4646840148698801</v>
+      </c>
+      <c r="B44" t="s">
+        <v>32</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44">
+        <v>12</v>
+      </c>
+      <c r="E44" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" t="s">
+        <v>16</v>
+      </c>
+      <c r="G44" t="s">
+        <v>26</v>
+      </c>
+      <c r="H44" t="s">
+        <v>28</v>
+      </c>
+      <c r="I44" t="s">
+        <v>14</v>
+      </c>
+      <c r="J44" t="s">
+        <v>31</v>
+      </c>
+      <c r="K44" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>0.67657992565055702</v>
+      </c>
+      <c r="B45" t="s">
+        <v>32</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45">
+        <v>22</v>
+      </c>
+      <c r="E45" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" t="s">
+        <v>26</v>
+      </c>
+      <c r="H45" t="s">
+        <v>28</v>
+      </c>
+      <c r="I45" t="s">
+        <v>14</v>
+      </c>
+      <c r="J45" t="s">
+        <v>31</v>
+      </c>
+      <c r="K45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>0.70631970260222998</v>
+      </c>
+      <c r="B46" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" t="s">
+        <v>16</v>
+      </c>
+      <c r="G46" t="s">
+        <v>26</v>
+      </c>
+      <c r="H46" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" t="s">
+        <v>31</v>
+      </c>
+      <c r="K46" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>0.13382899628252801</v>
+      </c>
+      <c r="B47" t="s">
+        <v>32</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
+        <v>11</v>
+      </c>
+      <c r="F47" t="s">
+        <v>16</v>
+      </c>
+      <c r="G47" t="s">
+        <v>26</v>
+      </c>
+      <c r="H47" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" t="s">
+        <v>14</v>
+      </c>
+      <c r="J47" t="s">
+        <v>31</v>
+      </c>
+      <c r="K47" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>1.13011152416356</v>
+      </c>
+      <c r="B48" t="s">
+        <v>32</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48">
+        <v>12</v>
+      </c>
+      <c r="E48" t="s">
+        <v>11</v>
+      </c>
+      <c r="F48" t="s">
+        <v>16</v>
+      </c>
+      <c r="G48" t="s">
+        <v>26</v>
+      </c>
+      <c r="H48" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" t="s">
+        <v>14</v>
+      </c>
+      <c r="J48" t="s">
+        <v>31</v>
+      </c>
+      <c r="K48" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>0.77323420074349403</v>
+      </c>
+      <c r="B49" t="s">
+        <v>32</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49">
+        <v>22</v>
+      </c>
+      <c r="E49" t="s">
+        <v>11</v>
+      </c>
+      <c r="F49" t="s">
+        <v>16</v>
+      </c>
+      <c r="G49" t="s">
+        <v>26</v>
+      </c>
+      <c r="H49" t="s">
+        <v>28</v>
+      </c>
+      <c r="I49" t="s">
+        <v>14</v>
+      </c>
+      <c r="J49" t="s">
+        <v>31</v>
+      </c>
+      <c r="K49" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>4.1652892561983403</v>
+      </c>
+      <c r="B50" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50">
+        <v>12</v>
+      </c>
+      <c r="E50" t="s">
+        <v>9</v>
+      </c>
+      <c r="F50" t="s">
+        <v>16</v>
+      </c>
+      <c r="G50" t="s">
+        <v>26</v>
+      </c>
+      <c r="H50" t="s">
+        <v>28</v>
+      </c>
+      <c r="I50" t="s">
+        <v>13</v>
+      </c>
+      <c r="J50" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>2.0826446280991702</v>
+      </c>
+      <c r="B51" t="s">
+        <v>33</v>
+      </c>
+      <c r="C51" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51">
+        <v>22</v>
+      </c>
+      <c r="E51" t="s">
+        <v>9</v>
+      </c>
+      <c r="F51" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" t="s">
+        <v>26</v>
+      </c>
+      <c r="H51" t="s">
+        <v>28</v>
+      </c>
+      <c r="I51" t="s">
+        <v>13</v>
+      </c>
+      <c r="J51" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>2.4628099173553699</v>
+      </c>
+      <c r="B52" t="s">
+        <v>33</v>
+      </c>
+      <c r="C52" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52">
+        <v>12</v>
+      </c>
+      <c r="E52" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" t="s">
+        <v>16</v>
+      </c>
+      <c r="G52" t="s">
+        <v>26</v>
+      </c>
+      <c r="H52" t="s">
+        <v>28</v>
+      </c>
+      <c r="I52" t="s">
+        <v>13</v>
+      </c>
+      <c r="J52" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>1.5702479338842901</v>
+      </c>
+      <c r="B53" t="s">
+        <v>33</v>
+      </c>
+      <c r="C53" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53">
+        <v>22</v>
+      </c>
+      <c r="E53" t="s">
+        <v>10</v>
+      </c>
+      <c r="F53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" t="s">
+        <v>26</v>
+      </c>
+      <c r="H53" t="s">
+        <v>28</v>
+      </c>
+      <c r="I53" t="s">
+        <v>13</v>
+      </c>
+      <c r="J53" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>2.2644628099173501</v>
+      </c>
+      <c r="B54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" t="s">
+        <v>16</v>
+      </c>
+      <c r="G54" t="s">
+        <v>26</v>
+      </c>
+      <c r="H54" t="s">
+        <v>28</v>
+      </c>
+      <c r="I54" t="s">
+        <v>14</v>
+      </c>
+      <c r="J54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>1.32231404958677</v>
+      </c>
+      <c r="B55" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="s">
+        <v>11</v>
+      </c>
+      <c r="F55" t="s">
+        <v>16</v>
+      </c>
+      <c r="G55" t="s">
+        <v>26</v>
+      </c>
+      <c r="H55" t="s">
+        <v>28</v>
+      </c>
+      <c r="I55" t="s">
+        <v>14</v>
+      </c>
+      <c r="J55" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>1.63636363636363</v>
+      </c>
+      <c r="B56" t="s">
+        <v>33</v>
+      </c>
+      <c r="C56" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56">
+        <v>12</v>
+      </c>
+      <c r="E56" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" t="s">
+        <v>16</v>
+      </c>
+      <c r="G56" t="s">
+        <v>26</v>
+      </c>
+      <c r="H56" t="s">
+        <v>28</v>
+      </c>
+      <c r="I56" t="s">
+        <v>14</v>
+      </c>
+      <c r="J56" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>1.1735537190082601</v>
+      </c>
+      <c r="B57" t="s">
+        <v>33</v>
+      </c>
+      <c r="C57" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57">
+        <v>22</v>
+      </c>
+      <c r="E57" t="s">
+        <v>11</v>
+      </c>
+      <c r="F57" t="s">
+        <v>16</v>
+      </c>
+      <c r="G57" t="s">
+        <v>26</v>
+      </c>
+      <c r="H57" t="s">
+        <v>28</v>
+      </c>
+      <c r="I57" t="s">
+        <v>14</v>
+      </c>
+      <c r="J57" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>3.02479338842975</v>
+      </c>
+      <c r="B58" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58" t="s">
+        <v>11</v>
+      </c>
+      <c r="F58" t="s">
+        <v>16</v>
+      </c>
+      <c r="G58" t="s">
+        <v>26</v>
+      </c>
+      <c r="H58" t="s">
+        <v>28</v>
+      </c>
+      <c r="I58" t="s">
+        <v>15</v>
+      </c>
+      <c r="J58" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>0.92561983471074305</v>
+      </c>
+      <c r="B59" t="s">
+        <v>33</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59" t="s">
+        <v>16</v>
+      </c>
+      <c r="G59" t="s">
+        <v>26</v>
+      </c>
+      <c r="H59" t="s">
+        <v>28</v>
+      </c>
+      <c r="I59" t="s">
+        <v>15</v>
+      </c>
+      <c r="J59" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>1.38842975206611</v>
+      </c>
+      <c r="B60" t="s">
+        <v>33</v>
+      </c>
+      <c r="C60" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60">
+        <v>12</v>
+      </c>
+      <c r="E60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60" t="s">
+        <v>16</v>
+      </c>
+      <c r="G60" t="s">
+        <v>26</v>
+      </c>
+      <c r="H60" t="s">
+        <v>28</v>
+      </c>
+      <c r="I60" t="s">
+        <v>15</v>
+      </c>
+      <c r="J60" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>1.2066115702479301</v>
+      </c>
+      <c r="B61" t="s">
+        <v>33</v>
+      </c>
+      <c r="C61" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61">
+        <v>22</v>
+      </c>
+      <c r="E61" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61" t="s">
+        <v>16</v>
+      </c>
+      <c r="G61" t="s">
+        <v>26</v>
+      </c>
+      <c r="H61" t="s">
+        <v>28</v>
+      </c>
+      <c r="I61" t="s">
+        <v>15</v>
+      </c>
+      <c r="J61" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>3.3934426229508099</v>
+      </c>
+      <c r="B62" t="s">
+        <v>33</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62">
+        <v>12</v>
+      </c>
+      <c r="E62" t="s">
+        <v>9</v>
+      </c>
+      <c r="F62" t="s">
+        <v>16</v>
+      </c>
+      <c r="G62" t="s">
+        <v>26</v>
+      </c>
+      <c r="H62" t="s">
+        <v>28</v>
+      </c>
+      <c r="I62" t="s">
+        <v>13</v>
+      </c>
+      <c r="J62" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>1.9672131147540901</v>
+      </c>
+      <c r="B63" t="s">
+        <v>33</v>
+      </c>
+      <c r="C63" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63">
+        <v>22</v>
+      </c>
+      <c r="E63" t="s">
+        <v>9</v>
+      </c>
+      <c r="F63" t="s">
+        <v>16</v>
+      </c>
+      <c r="G63" t="s">
+        <v>26</v>
+      </c>
+      <c r="H63" t="s">
+        <v>28</v>
+      </c>
+      <c r="I63" t="s">
+        <v>13</v>
+      </c>
+      <c r="J63" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>2.9016393442622901</v>
+      </c>
+      <c r="B64" t="s">
+        <v>33</v>
+      </c>
+      <c r="C64" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64">
+        <v>12</v>
+      </c>
+      <c r="E64" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" t="s">
+        <v>16</v>
+      </c>
+      <c r="G64" t="s">
+        <v>26</v>
+      </c>
+      <c r="H64" t="s">
+        <v>28</v>
+      </c>
+      <c r="I64" t="s">
+        <v>13</v>
+      </c>
+      <c r="J64" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>2.0655737704917998</v>
+      </c>
+      <c r="B65" t="s">
+        <v>33</v>
+      </c>
+      <c r="C65" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65">
+        <v>22</v>
+      </c>
+      <c r="E65" t="s">
+        <v>10</v>
+      </c>
+      <c r="F65" t="s">
+        <v>16</v>
+      </c>
+      <c r="G65" t="s">
+        <v>26</v>
+      </c>
+      <c r="H65" t="s">
+        <v>28</v>
+      </c>
+      <c r="I65" t="s">
+        <v>13</v>
+      </c>
+      <c r="J65" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>2.7704918032786798</v>
+      </c>
+      <c r="B66" t="s">
+        <v>33</v>
+      </c>
+      <c r="C66" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66" t="s">
+        <v>11</v>
+      </c>
+      <c r="F66" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" t="s">
+        <v>26</v>
+      </c>
+      <c r="H66" t="s">
+        <v>28</v>
+      </c>
+      <c r="I66" t="s">
+        <v>14</v>
+      </c>
+      <c r="J66" t="s">
+        <v>31</v>
+      </c>
+      <c r="K66" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>2.2950819672131102</v>
+      </c>
+      <c r="B67" t="s">
+        <v>33</v>
+      </c>
+      <c r="C67" t="s">
+        <v>6</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>11</v>
+      </c>
+      <c r="F67" t="s">
+        <v>16</v>
+      </c>
+      <c r="G67" t="s">
+        <v>26</v>
+      </c>
+      <c r="H67" t="s">
+        <v>28</v>
+      </c>
+      <c r="I67" t="s">
+        <v>14</v>
+      </c>
+      <c r="J67" t="s">
+        <v>31</v>
+      </c>
+      <c r="K67" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>1.9016393442622901</v>
+      </c>
+      <c r="B68" t="s">
+        <v>33</v>
+      </c>
+      <c r="C68" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68">
+        <v>12</v>
+      </c>
+      <c r="E68" t="s">
+        <v>11</v>
+      </c>
+      <c r="F68" t="s">
+        <v>16</v>
+      </c>
+      <c r="G68" t="s">
+        <v>26</v>
+      </c>
+      <c r="H68" t="s">
+        <v>28</v>
+      </c>
+      <c r="I68" t="s">
+        <v>14</v>
+      </c>
+      <c r="J68" t="s">
+        <v>31</v>
+      </c>
+      <c r="K68" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A69" s="2">
+        <v>1.3114754098360599</v>
+      </c>
+      <c r="B69" t="s">
+        <v>33</v>
+      </c>
+      <c r="C69" t="s">
+        <v>6</v>
+      </c>
+      <c r="D69">
+        <v>22</v>
+      </c>
+      <c r="E69" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" t="s">
+        <v>16</v>
+      </c>
+      <c r="G69" t="s">
+        <v>26</v>
+      </c>
+      <c r="H69" t="s">
+        <v>28</v>
+      </c>
+      <c r="I69" t="s">
+        <v>14</v>
+      </c>
+      <c r="J69" t="s">
+        <v>31</v>
+      </c>
+      <c r="K69" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A70" s="2">
+        <v>3.5409836065573699</v>
+      </c>
+      <c r="B70" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70" t="s">
+        <v>11</v>
+      </c>
+      <c r="F70" t="s">
+        <v>16</v>
+      </c>
+      <c r="G70" t="s">
+        <v>26</v>
+      </c>
+      <c r="H70" t="s">
+        <v>28</v>
+      </c>
+      <c r="I70" t="s">
+        <v>14</v>
+      </c>
+      <c r="J70" t="s">
+        <v>31</v>
+      </c>
+      <c r="K70" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A71" s="2">
+        <v>2.1967213114753998</v>
+      </c>
+      <c r="B71" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+      <c r="E71" t="s">
+        <v>11</v>
+      </c>
+      <c r="F71" t="s">
+        <v>16</v>
+      </c>
+      <c r="G71" t="s">
+        <v>26</v>
+      </c>
+      <c r="H71" t="s">
+        <v>28</v>
+      </c>
+      <c r="I71" t="s">
+        <v>14</v>
+      </c>
+      <c r="J71" t="s">
+        <v>31</v>
+      </c>
+      <c r="K71" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A72" s="2">
+        <v>1.6065573770491799</v>
+      </c>
+      <c r="B72" t="s">
+        <v>33</v>
+      </c>
+      <c r="C72" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72">
+        <v>12</v>
+      </c>
+      <c r="E72" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" t="s">
+        <v>16</v>
+      </c>
+      <c r="G72" t="s">
+        <v>26</v>
+      </c>
+      <c r="H72" t="s">
+        <v>28</v>
+      </c>
+      <c r="I72" t="s">
+        <v>14</v>
+      </c>
+      <c r="J72" t="s">
+        <v>31</v>
+      </c>
+      <c r="K72" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A73" s="2">
+        <v>1.3934426229508099</v>
+      </c>
+      <c r="B73" t="s">
+        <v>33</v>
+      </c>
+      <c r="C73" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73">
+        <v>22</v>
+      </c>
+      <c r="E73" t="s">
+        <v>11</v>
+      </c>
+      <c r="F73" t="s">
+        <v>16</v>
+      </c>
+      <c r="G73" t="s">
+        <v>26</v>
+      </c>
+      <c r="H73" t="s">
+        <v>28</v>
+      </c>
+      <c r="I73" t="s">
+        <v>14</v>
+      </c>
+      <c r="J73" t="s">
+        <v>31</v>
+      </c>
+      <c r="K73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>348</v>
+      </c>
+      <c r="B74" t="s">
+        <v>34</v>
+      </c>
+      <c r="C74" t="s">
+        <v>35</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
+        <v>9</v>
+      </c>
+      <c r="F74" t="s">
+        <v>16</v>
+      </c>
+      <c r="G74" t="s">
+        <v>26</v>
+      </c>
+      <c r="H74" t="s">
+        <v>28</v>
+      </c>
+      <c r="I74" t="s">
+        <v>13</v>
+      </c>
+      <c r="J74" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>358</v>
+      </c>
+      <c r="B75" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75" t="s">
+        <v>35</v>
+      </c>
+      <c r="D75">
+        <v>12</v>
+      </c>
+      <c r="E75" t="s">
+        <v>9</v>
+      </c>
+      <c r="F75" t="s">
+        <v>16</v>
+      </c>
+      <c r="G75" t="s">
+        <v>26</v>
+      </c>
+      <c r="H75" t="s">
+        <v>28</v>
+      </c>
+      <c r="I75" t="s">
+        <v>13</v>
+      </c>
+      <c r="J75" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>304</v>
+      </c>
+      <c r="B76" t="s">
+        <v>34</v>
+      </c>
+      <c r="C76" t="s">
+        <v>35</v>
+      </c>
+      <c r="D76">
+        <v>22</v>
+      </c>
+      <c r="E76" t="s">
+        <v>9</v>
+      </c>
+      <c r="F76" t="s">
+        <v>16</v>
+      </c>
+      <c r="G76" t="s">
+        <v>26</v>
+      </c>
+      <c r="H76" t="s">
+        <v>28</v>
+      </c>
+      <c r="I76" t="s">
+        <v>13</v>
+      </c>
+      <c r="J76" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>177</v>
+      </c>
+      <c r="B77" t="s">
+        <v>34</v>
+      </c>
+      <c r="C77" t="s">
+        <v>35</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+      <c r="E77" t="s">
+        <v>10</v>
+      </c>
+      <c r="F77" t="s">
+        <v>16</v>
+      </c>
+      <c r="G77" t="s">
+        <v>26</v>
+      </c>
+      <c r="H77" t="s">
+        <v>28</v>
+      </c>
+      <c r="I77" t="s">
+        <v>13</v>
+      </c>
+      <c r="J77" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>186</v>
+      </c>
+      <c r="B78" t="s">
+        <v>34</v>
+      </c>
+      <c r="C78" t="s">
+        <v>35</v>
+      </c>
+      <c r="D78">
+        <v>12</v>
+      </c>
+      <c r="E78" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" t="s">
+        <v>16</v>
+      </c>
+      <c r="G78" t="s">
+        <v>26</v>
+      </c>
+      <c r="H78" t="s">
+        <v>28</v>
+      </c>
+      <c r="I78" t="s">
+        <v>13</v>
+      </c>
+      <c r="J78" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>189</v>
+      </c>
+      <c r="B79" t="s">
+        <v>34</v>
+      </c>
+      <c r="C79" t="s">
+        <v>35</v>
+      </c>
+      <c r="D79">
+        <v>22</v>
+      </c>
+      <c r="E79" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" t="s">
+        <v>16</v>
+      </c>
+      <c r="G79" t="s">
+        <v>26</v>
+      </c>
+      <c r="H79" t="s">
+        <v>28</v>
+      </c>
+      <c r="I79" t="s">
+        <v>13</v>
+      </c>
+      <c r="J79" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>199</v>
+      </c>
+      <c r="B80" t="s">
+        <v>34</v>
+      </c>
+      <c r="C80" t="s">
+        <v>35</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80" t="s">
+        <v>11</v>
+      </c>
+      <c r="F80" t="s">
+        <v>16</v>
+      </c>
+      <c r="G80" t="s">
+        <v>26</v>
+      </c>
+      <c r="H80" t="s">
+        <v>28</v>
+      </c>
+      <c r="I80" t="s">
+        <v>14</v>
+      </c>
+      <c r="J80" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>199</v>
+      </c>
+      <c r="B81" t="s">
+        <v>34</v>
+      </c>
+      <c r="C81" t="s">
+        <v>35</v>
+      </c>
+      <c r="D81">
+        <v>12</v>
+      </c>
+      <c r="E81" t="s">
+        <v>11</v>
+      </c>
+      <c r="F81" t="s">
+        <v>16</v>
+      </c>
+      <c r="G81" t="s">
+        <v>26</v>
+      </c>
+      <c r="H81" t="s">
+        <v>28</v>
+      </c>
+      <c r="I81" t="s">
+        <v>14</v>
+      </c>
+      <c r="J81" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>208</v>
+      </c>
+      <c r="B82" t="s">
+        <v>34</v>
+      </c>
+      <c r="C82" t="s">
+        <v>35</v>
+      </c>
+      <c r="D82">
+        <v>22</v>
+      </c>
+      <c r="E82" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" t="s">
+        <v>16</v>
+      </c>
+      <c r="G82" t="s">
+        <v>26</v>
+      </c>
+      <c r="H82" t="s">
+        <v>28</v>
+      </c>
+      <c r="I82" t="s">
+        <v>14</v>
+      </c>
+      <c r="J82" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>202</v>
+      </c>
+      <c r="B83" t="s">
+        <v>34</v>
+      </c>
+      <c r="C83" t="s">
+        <v>35</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" t="s">
+        <v>16</v>
+      </c>
+      <c r="G83" t="s">
+        <v>26</v>
+      </c>
+      <c r="H83" t="s">
+        <v>28</v>
+      </c>
+      <c r="I83" t="s">
+        <v>15</v>
+      </c>
+      <c r="J83" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>213</v>
+      </c>
+      <c r="B84" t="s">
+        <v>34</v>
+      </c>
+      <c r="C84" t="s">
+        <v>35</v>
+      </c>
+      <c r="D84">
+        <v>12</v>
+      </c>
+      <c r="E84" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" t="s">
+        <v>16</v>
+      </c>
+      <c r="G84" t="s">
+        <v>26</v>
+      </c>
+      <c r="H84" t="s">
+        <v>28</v>
+      </c>
+      <c r="I84" t="s">
+        <v>15</v>
+      </c>
+      <c r="J84" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>202</v>
+      </c>
+      <c r="B85" t="s">
+        <v>34</v>
+      </c>
+      <c r="C85" t="s">
+        <v>35</v>
+      </c>
+      <c r="D85">
+        <v>22</v>
+      </c>
+      <c r="E85" t="s">
+        <v>11</v>
+      </c>
+      <c r="F85" t="s">
+        <v>16</v>
+      </c>
+      <c r="G85" t="s">
+        <v>26</v>
+      </c>
+      <c r="H85" t="s">
+        <v>28</v>
+      </c>
+      <c r="I85" t="s">
+        <v>15</v>
+      </c>
+      <c r="J85" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>325</v>
+      </c>
+      <c r="B86" t="s">
+        <v>34</v>
+      </c>
+      <c r="C86" t="s">
+        <v>35</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>9</v>
+      </c>
+      <c r="F86" t="s">
+        <v>16</v>
+      </c>
+      <c r="G86" t="s">
+        <v>26</v>
+      </c>
+      <c r="H86" t="s">
+        <v>28</v>
+      </c>
+      <c r="I86" t="s">
+        <v>13</v>
+      </c>
+      <c r="J86" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>306</v>
+      </c>
+      <c r="B87" t="s">
+        <v>34</v>
+      </c>
+      <c r="C87" t="s">
+        <v>35</v>
+      </c>
+      <c r="D87">
+        <v>12</v>
+      </c>
+      <c r="E87" t="s">
+        <v>9</v>
+      </c>
+      <c r="F87" t="s">
+        <v>16</v>
+      </c>
+      <c r="G87" t="s">
+        <v>26</v>
+      </c>
+      <c r="H87" t="s">
+        <v>28</v>
+      </c>
+      <c r="I87" t="s">
+        <v>13</v>
+      </c>
+      <c r="J87" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>275</v>
+      </c>
+      <c r="B88" t="s">
+        <v>34</v>
+      </c>
+      <c r="C88" t="s">
+        <v>35</v>
+      </c>
+      <c r="D88">
+        <v>22</v>
+      </c>
+      <c r="E88" t="s">
+        <v>9</v>
+      </c>
+      <c r="F88" t="s">
+        <v>16</v>
+      </c>
+      <c r="G88" t="s">
+        <v>26</v>
+      </c>
+      <c r="H88" t="s">
+        <v>28</v>
+      </c>
+      <c r="I88" t="s">
+        <v>13</v>
+      </c>
+      <c r="J88" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>140</v>
+      </c>
+      <c r="B89" t="s">
+        <v>34</v>
+      </c>
+      <c r="C89" t="s">
+        <v>35</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89" t="s">
+        <v>10</v>
+      </c>
+      <c r="F89" t="s">
+        <v>16</v>
+      </c>
+      <c r="G89" t="s">
+        <v>26</v>
+      </c>
+      <c r="H89" t="s">
+        <v>28</v>
+      </c>
+      <c r="I89" t="s">
+        <v>13</v>
+      </c>
+      <c r="J89" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>133</v>
+      </c>
+      <c r="B90" t="s">
+        <v>34</v>
+      </c>
+      <c r="C90" t="s">
+        <v>35</v>
+      </c>
+      <c r="D90">
+        <v>12</v>
+      </c>
+      <c r="E90" t="s">
+        <v>10</v>
+      </c>
+      <c r="F90" t="s">
+        <v>16</v>
+      </c>
+      <c r="G90" t="s">
+        <v>26</v>
+      </c>
+      <c r="H90" t="s">
+        <v>28</v>
+      </c>
+      <c r="I90" t="s">
+        <v>13</v>
+      </c>
+      <c r="J90" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>140</v>
+      </c>
+      <c r="B91" t="s">
+        <v>34</v>
+      </c>
+      <c r="C91" t="s">
+        <v>35</v>
+      </c>
+      <c r="D91">
+        <v>22</v>
+      </c>
+      <c r="E91" t="s">
+        <v>10</v>
+      </c>
+      <c r="F91" t="s">
+        <v>16</v>
+      </c>
+      <c r="G91" t="s">
+        <v>26</v>
+      </c>
+      <c r="H91" t="s">
+        <v>28</v>
+      </c>
+      <c r="I91" t="s">
+        <v>13</v>
+      </c>
+      <c r="J91" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>118</v>
+      </c>
+      <c r="B92" t="s">
+        <v>34</v>
+      </c>
+      <c r="C92" t="s">
+        <v>35</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+      <c r="E92" t="s">
+        <v>11</v>
+      </c>
+      <c r="F92" t="s">
+        <v>16</v>
+      </c>
+      <c r="G92" t="s">
+        <v>26</v>
+      </c>
+      <c r="H92" t="s">
+        <v>28</v>
+      </c>
+      <c r="I92" t="s">
+        <v>14</v>
+      </c>
+      <c r="J92" t="s">
+        <v>31</v>
+      </c>
+      <c r="K92" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>115</v>
+      </c>
+      <c r="B93" t="s">
+        <v>34</v>
+      </c>
+      <c r="C93" t="s">
+        <v>35</v>
+      </c>
+      <c r="D93">
+        <v>12</v>
+      </c>
+      <c r="E93" t="s">
+        <v>11</v>
+      </c>
+      <c r="F93" t="s">
+        <v>16</v>
+      </c>
+      <c r="G93" t="s">
+        <v>26</v>
+      </c>
+      <c r="H93" t="s">
+        <v>28</v>
+      </c>
+      <c r="I93" t="s">
+        <v>14</v>
+      </c>
+      <c r="J93" t="s">
+        <v>31</v>
+      </c>
+      <c r="K93" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>122</v>
+      </c>
+      <c r="B94" t="s">
+        <v>34</v>
+      </c>
+      <c r="C94" t="s">
+        <v>35</v>
+      </c>
+      <c r="D94">
+        <v>22</v>
+      </c>
+      <c r="E94" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94" t="s">
+        <v>16</v>
+      </c>
+      <c r="G94" t="s">
+        <v>26</v>
+      </c>
+      <c r="H94" t="s">
+        <v>28</v>
+      </c>
+      <c r="I94" t="s">
+        <v>14</v>
+      </c>
+      <c r="J94" t="s">
+        <v>31</v>
+      </c>
+      <c r="K94" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>148</v>
+      </c>
+      <c r="B95" t="s">
+        <v>34</v>
+      </c>
+      <c r="C95" t="s">
+        <v>35</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+      <c r="E95" t="s">
+        <v>11</v>
+      </c>
+      <c r="F95" t="s">
+        <v>16</v>
+      </c>
+      <c r="G95" t="s">
+        <v>26</v>
+      </c>
+      <c r="H95" t="s">
+        <v>28</v>
+      </c>
+      <c r="I95" t="s">
+        <v>14</v>
+      </c>
+      <c r="J95" t="s">
+        <v>31</v>
+      </c>
+      <c r="K95" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>131</v>
+      </c>
+      <c r="B96" t="s">
+        <v>34</v>
+      </c>
+      <c r="C96" t="s">
+        <v>35</v>
+      </c>
+      <c r="D96">
+        <v>12</v>
+      </c>
+      <c r="E96" t="s">
+        <v>11</v>
+      </c>
+      <c r="F96" t="s">
+        <v>16</v>
+      </c>
+      <c r="G96" t="s">
+        <v>26</v>
+      </c>
+      <c r="H96" t="s">
+        <v>28</v>
+      </c>
+      <c r="I96" t="s">
+        <v>14</v>
+      </c>
+      <c r="J96" t="s">
+        <v>31</v>
+      </c>
+      <c r="K96" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>133</v>
+      </c>
+      <c r="B97" t="s">
+        <v>34</v>
+      </c>
+      <c r="C97" t="s">
+        <v>35</v>
+      </c>
+      <c r="D97">
+        <v>22</v>
+      </c>
+      <c r="E97" t="s">
+        <v>11</v>
+      </c>
+      <c r="F97" t="s">
+        <v>16</v>
+      </c>
+      <c r="G97" t="s">
+        <v>26</v>
+      </c>
+      <c r="H97" t="s">
+        <v>28</v>
+      </c>
+      <c r="I97" t="s">
+        <v>14</v>
+      </c>
+      <c r="J97" t="s">
+        <v>31</v>
+      </c>
+      <c r="K97" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
finished digitizing hood et al 2020
</commit_message>
<xml_diff>
--- a/data/web_plot_digitizer_data.xlsx
+++ b/data/web_plot_digitizer_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramR\fuels_longevity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE5132A-9960-4FF4-8339-A8A7A0340A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4844266-17CE-4DCB-A378-939ACEC90944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6245A06B-15CE-492B-AD18-D354A95DB25A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="44">
   <si>
     <t>variable</t>
   </si>
@@ -148,11 +148,38 @@
   <si>
     <t>trees/ha</t>
   </si>
+  <si>
+    <t>basal_area</t>
+  </si>
+  <si>
+    <t>m2/ha</t>
+  </si>
+  <si>
+    <t>qmd</t>
+  </si>
+  <si>
+    <t>cm</t>
+  </si>
+  <si>
+    <t>sapling_density</t>
+  </si>
+  <si>
+    <t>saps/ha</t>
+  </si>
+  <si>
+    <t>seedling_density</t>
+  </si>
+  <si>
+    <t>seedlings/ha</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.0"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -188,12 +215,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,16 +589,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A8627B-2386-4DAF-99DA-19F1EA4382AF}">
-  <dimension ref="A1:K97"/>
+  <dimension ref="A1:K185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F83" sqref="F83"/>
+    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I160" sqref="I160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
     <col min="3" max="3" width="13.109375" customWidth="1"/>
     <col min="4" max="8" width="12.6640625" customWidth="1"/>
     <col min="9" max="9" width="15.33203125" customWidth="1"/>
@@ -3768,6 +3800,2888 @@
         <v>31</v>
       </c>
       <c r="K97" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A98" s="3">
+        <v>23.690476190476101</v>
+      </c>
+      <c r="B98" t="s">
+        <v>36</v>
+      </c>
+      <c r="C98" t="s">
+        <v>37</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+      <c r="E98" t="s">
+        <v>9</v>
+      </c>
+      <c r="F98" t="s">
+        <v>16</v>
+      </c>
+      <c r="G98" t="s">
+        <v>26</v>
+      </c>
+      <c r="H98" t="s">
+        <v>28</v>
+      </c>
+      <c r="I98" t="s">
+        <v>13</v>
+      </c>
+      <c r="J98" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A99" s="4">
+        <v>30</v>
+      </c>
+      <c r="B99" t="s">
+        <v>36</v>
+      </c>
+      <c r="C99" t="s">
+        <v>37</v>
+      </c>
+      <c r="D99">
+        <v>12</v>
+      </c>
+      <c r="E99" t="s">
+        <v>9</v>
+      </c>
+      <c r="F99" t="s">
+        <v>16</v>
+      </c>
+      <c r="G99" t="s">
+        <v>26</v>
+      </c>
+      <c r="H99" t="s">
+        <v>28</v>
+      </c>
+      <c r="I99" t="s">
+        <v>13</v>
+      </c>
+      <c r="J99" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A100" s="4">
+        <v>29.047619047619001</v>
+      </c>
+      <c r="B100" t="s">
+        <v>36</v>
+      </c>
+      <c r="C100" t="s">
+        <v>37</v>
+      </c>
+      <c r="D100">
+        <v>22</v>
+      </c>
+      <c r="E100" t="s">
+        <v>9</v>
+      </c>
+      <c r="F100" t="s">
+        <v>16</v>
+      </c>
+      <c r="G100" t="s">
+        <v>26</v>
+      </c>
+      <c r="H100" t="s">
+        <v>28</v>
+      </c>
+      <c r="I100" t="s">
+        <v>13</v>
+      </c>
+      <c r="J100" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A101" s="4">
+        <v>12.857142857142801</v>
+      </c>
+      <c r="B101" t="s">
+        <v>36</v>
+      </c>
+      <c r="C101" t="s">
+        <v>37</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+      <c r="E101" t="s">
+        <v>10</v>
+      </c>
+      <c r="F101" t="s">
+        <v>16</v>
+      </c>
+      <c r="G101" t="s">
+        <v>26</v>
+      </c>
+      <c r="H101" t="s">
+        <v>28</v>
+      </c>
+      <c r="I101" t="s">
+        <v>13</v>
+      </c>
+      <c r="J101" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A102" s="4">
+        <v>17.380952380952301</v>
+      </c>
+      <c r="B102" t="s">
+        <v>36</v>
+      </c>
+      <c r="C102" t="s">
+        <v>37</v>
+      </c>
+      <c r="D102">
+        <v>12</v>
+      </c>
+      <c r="E102" t="s">
+        <v>10</v>
+      </c>
+      <c r="F102" t="s">
+        <v>16</v>
+      </c>
+      <c r="G102" t="s">
+        <v>26</v>
+      </c>
+      <c r="H102" t="s">
+        <v>28</v>
+      </c>
+      <c r="I102" t="s">
+        <v>13</v>
+      </c>
+      <c r="J102" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A103" s="4">
+        <v>20.952380952380899</v>
+      </c>
+      <c r="B103" t="s">
+        <v>36</v>
+      </c>
+      <c r="C103" t="s">
+        <v>37</v>
+      </c>
+      <c r="D103">
+        <v>22</v>
+      </c>
+      <c r="E103" t="s">
+        <v>10</v>
+      </c>
+      <c r="F103" t="s">
+        <v>16</v>
+      </c>
+      <c r="G103" t="s">
+        <v>26</v>
+      </c>
+      <c r="H103" t="s">
+        <v>28</v>
+      </c>
+      <c r="I103" t="s">
+        <v>13</v>
+      </c>
+      <c r="J103" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A104" s="4">
+        <v>12.857142857142801</v>
+      </c>
+      <c r="B104" t="s">
+        <v>36</v>
+      </c>
+      <c r="C104" t="s">
+        <v>37</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104" t="s">
+        <v>11</v>
+      </c>
+      <c r="F104" t="s">
+        <v>16</v>
+      </c>
+      <c r="G104" t="s">
+        <v>26</v>
+      </c>
+      <c r="H104" t="s">
+        <v>28</v>
+      </c>
+      <c r="I104" t="s">
+        <v>14</v>
+      </c>
+      <c r="J104" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A105" s="4">
+        <v>16.6666666666666</v>
+      </c>
+      <c r="B105" t="s">
+        <v>36</v>
+      </c>
+      <c r="C105" t="s">
+        <v>37</v>
+      </c>
+      <c r="D105">
+        <v>12</v>
+      </c>
+      <c r="E105" t="s">
+        <v>11</v>
+      </c>
+      <c r="F105" t="s">
+        <v>16</v>
+      </c>
+      <c r="G105" t="s">
+        <v>26</v>
+      </c>
+      <c r="H105" t="s">
+        <v>28</v>
+      </c>
+      <c r="I105" t="s">
+        <v>14</v>
+      </c>
+      <c r="J105" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A106" s="4">
+        <v>20.8333333333333</v>
+      </c>
+      <c r="B106" t="s">
+        <v>36</v>
+      </c>
+      <c r="C106" t="s">
+        <v>37</v>
+      </c>
+      <c r="D106">
+        <v>22</v>
+      </c>
+      <c r="E106" t="s">
+        <v>11</v>
+      </c>
+      <c r="F106" t="s">
+        <v>16</v>
+      </c>
+      <c r="G106" t="s">
+        <v>26</v>
+      </c>
+      <c r="H106" t="s">
+        <v>28</v>
+      </c>
+      <c r="I106" t="s">
+        <v>14</v>
+      </c>
+      <c r="J106" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A107" s="4">
+        <v>14.4047619047619</v>
+      </c>
+      <c r="B107" t="s">
+        <v>36</v>
+      </c>
+      <c r="C107" t="s">
+        <v>37</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+      <c r="E107" t="s">
+        <v>11</v>
+      </c>
+      <c r="F107" t="s">
+        <v>16</v>
+      </c>
+      <c r="G107" t="s">
+        <v>26</v>
+      </c>
+      <c r="H107" t="s">
+        <v>28</v>
+      </c>
+      <c r="I107" t="s">
+        <v>15</v>
+      </c>
+      <c r="J107" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A108" s="4">
+        <v>18.928571428571399</v>
+      </c>
+      <c r="B108" t="s">
+        <v>36</v>
+      </c>
+      <c r="C108" t="s">
+        <v>37</v>
+      </c>
+      <c r="D108">
+        <v>12</v>
+      </c>
+      <c r="E108" t="s">
+        <v>11</v>
+      </c>
+      <c r="F108" t="s">
+        <v>16</v>
+      </c>
+      <c r="G108" t="s">
+        <v>26</v>
+      </c>
+      <c r="H108" t="s">
+        <v>28</v>
+      </c>
+      <c r="I108" t="s">
+        <v>15</v>
+      </c>
+      <c r="J108" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A109" s="4">
+        <v>21.6666666666666</v>
+      </c>
+      <c r="B109" t="s">
+        <v>36</v>
+      </c>
+      <c r="C109" t="s">
+        <v>37</v>
+      </c>
+      <c r="D109">
+        <v>22</v>
+      </c>
+      <c r="E109" t="s">
+        <v>11</v>
+      </c>
+      <c r="F109" t="s">
+        <v>16</v>
+      </c>
+      <c r="G109" t="s">
+        <v>26</v>
+      </c>
+      <c r="H109" t="s">
+        <v>28</v>
+      </c>
+      <c r="I109" t="s">
+        <v>15</v>
+      </c>
+      <c r="J109" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>25.5</v>
+      </c>
+      <c r="B110" t="s">
+        <v>36</v>
+      </c>
+      <c r="C110" t="s">
+        <v>37</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110" t="s">
+        <v>9</v>
+      </c>
+      <c r="F110" t="s">
+        <v>16</v>
+      </c>
+      <c r="G110" t="s">
+        <v>26</v>
+      </c>
+      <c r="H110" t="s">
+        <v>28</v>
+      </c>
+      <c r="I110" t="s">
+        <v>13</v>
+      </c>
+      <c r="J110" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <v>28.3</v>
+      </c>
+      <c r="B111" t="s">
+        <v>36</v>
+      </c>
+      <c r="C111" t="s">
+        <v>37</v>
+      </c>
+      <c r="D111">
+        <v>12</v>
+      </c>
+      <c r="E111" t="s">
+        <v>9</v>
+      </c>
+      <c r="F111" t="s">
+        <v>16</v>
+      </c>
+      <c r="G111" t="s">
+        <v>26</v>
+      </c>
+      <c r="H111" t="s">
+        <v>28</v>
+      </c>
+      <c r="I111" t="s">
+        <v>13</v>
+      </c>
+      <c r="J111" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <v>29.2</v>
+      </c>
+      <c r="B112" t="s">
+        <v>36</v>
+      </c>
+      <c r="C112" t="s">
+        <v>37</v>
+      </c>
+      <c r="D112">
+        <v>22</v>
+      </c>
+      <c r="E112" t="s">
+        <v>9</v>
+      </c>
+      <c r="F112" t="s">
+        <v>16</v>
+      </c>
+      <c r="G112" t="s">
+        <v>26</v>
+      </c>
+      <c r="H112" t="s">
+        <v>28</v>
+      </c>
+      <c r="I112" t="s">
+        <v>13</v>
+      </c>
+      <c r="J112" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <v>11.9</v>
+      </c>
+      <c r="B113" t="s">
+        <v>36</v>
+      </c>
+      <c r="C113" t="s">
+        <v>37</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+      <c r="E113" t="s">
+        <v>10</v>
+      </c>
+      <c r="F113" t="s">
+        <v>16</v>
+      </c>
+      <c r="G113" t="s">
+        <v>26</v>
+      </c>
+      <c r="H113" t="s">
+        <v>28</v>
+      </c>
+      <c r="I113" t="s">
+        <v>13</v>
+      </c>
+      <c r="J113" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A114" s="4">
+        <v>15</v>
+      </c>
+      <c r="B114" t="s">
+        <v>36</v>
+      </c>
+      <c r="C114" t="s">
+        <v>37</v>
+      </c>
+      <c r="D114">
+        <v>12</v>
+      </c>
+      <c r="E114" t="s">
+        <v>10</v>
+      </c>
+      <c r="F114" t="s">
+        <v>16</v>
+      </c>
+      <c r="G114" t="s">
+        <v>26</v>
+      </c>
+      <c r="H114" t="s">
+        <v>28</v>
+      </c>
+      <c r="I114" t="s">
+        <v>13</v>
+      </c>
+      <c r="J114" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A115" s="4">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="B115" t="s">
+        <v>36</v>
+      </c>
+      <c r="C115" t="s">
+        <v>37</v>
+      </c>
+      <c r="D115">
+        <v>22</v>
+      </c>
+      <c r="E115" t="s">
+        <v>10</v>
+      </c>
+      <c r="F115" t="s">
+        <v>16</v>
+      </c>
+      <c r="G115" t="s">
+        <v>26</v>
+      </c>
+      <c r="H115" t="s">
+        <v>28</v>
+      </c>
+      <c r="I115" t="s">
+        <v>13</v>
+      </c>
+      <c r="J115" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A116" s="4">
+        <v>10</v>
+      </c>
+      <c r="B116" t="s">
+        <v>36</v>
+      </c>
+      <c r="C116" t="s">
+        <v>37</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+      <c r="E116" t="s">
+        <v>11</v>
+      </c>
+      <c r="F116" t="s">
+        <v>16</v>
+      </c>
+      <c r="G116" t="s">
+        <v>26</v>
+      </c>
+      <c r="H116" t="s">
+        <v>28</v>
+      </c>
+      <c r="I116" t="s">
+        <v>14</v>
+      </c>
+      <c r="J116" t="s">
+        <v>31</v>
+      </c>
+      <c r="K116" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A117" s="4">
+        <v>12.5</v>
+      </c>
+      <c r="B117" t="s">
+        <v>36</v>
+      </c>
+      <c r="C117" t="s">
+        <v>37</v>
+      </c>
+      <c r="D117">
+        <v>12</v>
+      </c>
+      <c r="E117" t="s">
+        <v>11</v>
+      </c>
+      <c r="F117" t="s">
+        <v>16</v>
+      </c>
+      <c r="G117" t="s">
+        <v>26</v>
+      </c>
+      <c r="H117" t="s">
+        <v>28</v>
+      </c>
+      <c r="I117" t="s">
+        <v>14</v>
+      </c>
+      <c r="J117" t="s">
+        <v>31</v>
+      </c>
+      <c r="K117" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A118" s="4">
+        <v>15.5</v>
+      </c>
+      <c r="B118" t="s">
+        <v>36</v>
+      </c>
+      <c r="C118" t="s">
+        <v>37</v>
+      </c>
+      <c r="D118">
+        <v>22</v>
+      </c>
+      <c r="E118" t="s">
+        <v>11</v>
+      </c>
+      <c r="F118" t="s">
+        <v>16</v>
+      </c>
+      <c r="G118" t="s">
+        <v>26</v>
+      </c>
+      <c r="H118" t="s">
+        <v>28</v>
+      </c>
+      <c r="I118" t="s">
+        <v>14</v>
+      </c>
+      <c r="J118" t="s">
+        <v>31</v>
+      </c>
+      <c r="K118" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A119" s="4">
+        <v>11.6</v>
+      </c>
+      <c r="B119" t="s">
+        <v>36</v>
+      </c>
+      <c r="C119" t="s">
+        <v>37</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+      <c r="E119" t="s">
+        <v>11</v>
+      </c>
+      <c r="F119" t="s">
+        <v>16</v>
+      </c>
+      <c r="G119" t="s">
+        <v>26</v>
+      </c>
+      <c r="H119" t="s">
+        <v>28</v>
+      </c>
+      <c r="I119" t="s">
+        <v>14</v>
+      </c>
+      <c r="J119" t="s">
+        <v>31</v>
+      </c>
+      <c r="K119" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A120" s="4">
+        <v>13.2</v>
+      </c>
+      <c r="B120" t="s">
+        <v>36</v>
+      </c>
+      <c r="C120" t="s">
+        <v>37</v>
+      </c>
+      <c r="D120">
+        <v>12</v>
+      </c>
+      <c r="E120" t="s">
+        <v>11</v>
+      </c>
+      <c r="F120" t="s">
+        <v>16</v>
+      </c>
+      <c r="G120" t="s">
+        <v>26</v>
+      </c>
+      <c r="H120" t="s">
+        <v>28</v>
+      </c>
+      <c r="I120" t="s">
+        <v>14</v>
+      </c>
+      <c r="J120" t="s">
+        <v>31</v>
+      </c>
+      <c r="K120" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A121" s="4">
+        <v>16</v>
+      </c>
+      <c r="B121" t="s">
+        <v>36</v>
+      </c>
+      <c r="C121" t="s">
+        <v>37</v>
+      </c>
+      <c r="D121">
+        <v>22</v>
+      </c>
+      <c r="E121" t="s">
+        <v>11</v>
+      </c>
+      <c r="F121" t="s">
+        <v>16</v>
+      </c>
+      <c r="G121" t="s">
+        <v>26</v>
+      </c>
+      <c r="H121" t="s">
+        <v>28</v>
+      </c>
+      <c r="I121" t="s">
+        <v>14</v>
+      </c>
+      <c r="J121" t="s">
+        <v>31</v>
+      </c>
+      <c r="K121" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <v>30.1</v>
+      </c>
+      <c r="B122" t="s">
+        <v>38</v>
+      </c>
+      <c r="C122" t="s">
+        <v>39</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+      <c r="E122" t="s">
+        <v>9</v>
+      </c>
+      <c r="F122" t="s">
+        <v>16</v>
+      </c>
+      <c r="G122" t="s">
+        <v>26</v>
+      </c>
+      <c r="H122" t="s">
+        <v>28</v>
+      </c>
+      <c r="I122" t="s">
+        <v>13</v>
+      </c>
+      <c r="J122" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <v>33.1</v>
+      </c>
+      <c r="B123" t="s">
+        <v>38</v>
+      </c>
+      <c r="C123" t="s">
+        <v>39</v>
+      </c>
+      <c r="D123">
+        <v>12</v>
+      </c>
+      <c r="E123" t="s">
+        <v>9</v>
+      </c>
+      <c r="F123" t="s">
+        <v>16</v>
+      </c>
+      <c r="G123" t="s">
+        <v>26</v>
+      </c>
+      <c r="H123" t="s">
+        <v>28</v>
+      </c>
+      <c r="I123" t="s">
+        <v>13</v>
+      </c>
+      <c r="J123" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <v>35.5</v>
+      </c>
+      <c r="B124" t="s">
+        <v>38</v>
+      </c>
+      <c r="C124" t="s">
+        <v>39</v>
+      </c>
+      <c r="D124">
+        <v>22</v>
+      </c>
+      <c r="E124" t="s">
+        <v>9</v>
+      </c>
+      <c r="F124" t="s">
+        <v>16</v>
+      </c>
+      <c r="G124" t="s">
+        <v>26</v>
+      </c>
+      <c r="H124" t="s">
+        <v>28</v>
+      </c>
+      <c r="I124" t="s">
+        <v>13</v>
+      </c>
+      <c r="J124" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <v>31.2</v>
+      </c>
+      <c r="B125" t="s">
+        <v>38</v>
+      </c>
+      <c r="C125" t="s">
+        <v>39</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+      <c r="E125" t="s">
+        <v>10</v>
+      </c>
+      <c r="F125" t="s">
+        <v>16</v>
+      </c>
+      <c r="G125" t="s">
+        <v>26</v>
+      </c>
+      <c r="H125" t="s">
+        <v>28</v>
+      </c>
+      <c r="I125" t="s">
+        <v>13</v>
+      </c>
+      <c r="J125" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <v>35.4</v>
+      </c>
+      <c r="B126" t="s">
+        <v>38</v>
+      </c>
+      <c r="C126" t="s">
+        <v>39</v>
+      </c>
+      <c r="D126">
+        <v>12</v>
+      </c>
+      <c r="E126" t="s">
+        <v>10</v>
+      </c>
+      <c r="F126" t="s">
+        <v>16</v>
+      </c>
+      <c r="G126" t="s">
+        <v>26</v>
+      </c>
+      <c r="H126" t="s">
+        <v>28</v>
+      </c>
+      <c r="I126" t="s">
+        <v>13</v>
+      </c>
+      <c r="J126" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <v>38.6</v>
+      </c>
+      <c r="B127" t="s">
+        <v>38</v>
+      </c>
+      <c r="C127" t="s">
+        <v>39</v>
+      </c>
+      <c r="D127">
+        <v>22</v>
+      </c>
+      <c r="E127" t="s">
+        <v>10</v>
+      </c>
+      <c r="F127" t="s">
+        <v>16</v>
+      </c>
+      <c r="G127" t="s">
+        <v>26</v>
+      </c>
+      <c r="H127" t="s">
+        <v>28</v>
+      </c>
+      <c r="I127" t="s">
+        <v>13</v>
+      </c>
+      <c r="J127" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <v>29.4</v>
+      </c>
+      <c r="B128" t="s">
+        <v>38</v>
+      </c>
+      <c r="C128" t="s">
+        <v>39</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+      <c r="E128" t="s">
+        <v>11</v>
+      </c>
+      <c r="F128" t="s">
+        <v>16</v>
+      </c>
+      <c r="G128" t="s">
+        <v>26</v>
+      </c>
+      <c r="H128" t="s">
+        <v>28</v>
+      </c>
+      <c r="I128" t="s">
+        <v>14</v>
+      </c>
+      <c r="J128" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <v>33.6</v>
+      </c>
+      <c r="B129" t="s">
+        <v>38</v>
+      </c>
+      <c r="C129" t="s">
+        <v>39</v>
+      </c>
+      <c r="D129">
+        <v>12</v>
+      </c>
+      <c r="E129" t="s">
+        <v>11</v>
+      </c>
+      <c r="F129" t="s">
+        <v>16</v>
+      </c>
+      <c r="G129" t="s">
+        <v>26</v>
+      </c>
+      <c r="H129" t="s">
+        <v>28</v>
+      </c>
+      <c r="I129" t="s">
+        <v>14</v>
+      </c>
+      <c r="J129" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <v>36.9</v>
+      </c>
+      <c r="B130" t="s">
+        <v>38</v>
+      </c>
+      <c r="C130" t="s">
+        <v>39</v>
+      </c>
+      <c r="D130">
+        <v>22</v>
+      </c>
+      <c r="E130" t="s">
+        <v>11</v>
+      </c>
+      <c r="F130" t="s">
+        <v>16</v>
+      </c>
+      <c r="G130" t="s">
+        <v>26</v>
+      </c>
+      <c r="H130" t="s">
+        <v>28</v>
+      </c>
+      <c r="I130" t="s">
+        <v>14</v>
+      </c>
+      <c r="J130" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <v>30.4</v>
+      </c>
+      <c r="B131" t="s">
+        <v>38</v>
+      </c>
+      <c r="C131" t="s">
+        <v>39</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+      <c r="E131" t="s">
+        <v>11</v>
+      </c>
+      <c r="F131" t="s">
+        <v>16</v>
+      </c>
+      <c r="G131" t="s">
+        <v>26</v>
+      </c>
+      <c r="H131" t="s">
+        <v>28</v>
+      </c>
+      <c r="I131" t="s">
+        <v>15</v>
+      </c>
+      <c r="J131" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <v>34</v>
+      </c>
+      <c r="B132" t="s">
+        <v>38</v>
+      </c>
+      <c r="C132" t="s">
+        <v>39</v>
+      </c>
+      <c r="D132">
+        <v>12</v>
+      </c>
+      <c r="E132" t="s">
+        <v>11</v>
+      </c>
+      <c r="F132" t="s">
+        <v>16</v>
+      </c>
+      <c r="G132" t="s">
+        <v>26</v>
+      </c>
+      <c r="H132" t="s">
+        <v>28</v>
+      </c>
+      <c r="I132" t="s">
+        <v>15</v>
+      </c>
+      <c r="J132" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <v>37.6</v>
+      </c>
+      <c r="B133" t="s">
+        <v>38</v>
+      </c>
+      <c r="C133" t="s">
+        <v>39</v>
+      </c>
+      <c r="D133">
+        <v>22</v>
+      </c>
+      <c r="E133" t="s">
+        <v>11</v>
+      </c>
+      <c r="F133" t="s">
+        <v>16</v>
+      </c>
+      <c r="G133" t="s">
+        <v>26</v>
+      </c>
+      <c r="H133" t="s">
+        <v>28</v>
+      </c>
+      <c r="I133" t="s">
+        <v>15</v>
+      </c>
+      <c r="J133" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="B134" t="s">
+        <v>38</v>
+      </c>
+      <c r="C134" t="s">
+        <v>39</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+      <c r="E134" t="s">
+        <v>9</v>
+      </c>
+      <c r="F134" t="s">
+        <v>16</v>
+      </c>
+      <c r="G134" t="s">
+        <v>26</v>
+      </c>
+      <c r="H134" t="s">
+        <v>28</v>
+      </c>
+      <c r="I134" t="s">
+        <v>13</v>
+      </c>
+      <c r="J134" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <v>34.9</v>
+      </c>
+      <c r="B135" t="s">
+        <v>38</v>
+      </c>
+      <c r="C135" t="s">
+        <v>39</v>
+      </c>
+      <c r="D135">
+        <v>12</v>
+      </c>
+      <c r="E135" t="s">
+        <v>9</v>
+      </c>
+      <c r="F135" t="s">
+        <v>16</v>
+      </c>
+      <c r="G135" t="s">
+        <v>26</v>
+      </c>
+      <c r="H135" t="s">
+        <v>28</v>
+      </c>
+      <c r="I135" t="s">
+        <v>13</v>
+      </c>
+      <c r="J135" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <v>36.6</v>
+      </c>
+      <c r="B136" t="s">
+        <v>38</v>
+      </c>
+      <c r="C136" t="s">
+        <v>39</v>
+      </c>
+      <c r="D136">
+        <v>22</v>
+      </c>
+      <c r="E136" t="s">
+        <v>9</v>
+      </c>
+      <c r="F136" t="s">
+        <v>16</v>
+      </c>
+      <c r="G136" t="s">
+        <v>26</v>
+      </c>
+      <c r="H136" t="s">
+        <v>28</v>
+      </c>
+      <c r="I136" t="s">
+        <v>13</v>
+      </c>
+      <c r="J136" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <v>34.5</v>
+      </c>
+      <c r="B137" t="s">
+        <v>38</v>
+      </c>
+      <c r="C137" t="s">
+        <v>39</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+      <c r="E137" t="s">
+        <v>10</v>
+      </c>
+      <c r="F137" t="s">
+        <v>16</v>
+      </c>
+      <c r="G137" t="s">
+        <v>26</v>
+      </c>
+      <c r="H137" t="s">
+        <v>28</v>
+      </c>
+      <c r="I137" t="s">
+        <v>13</v>
+      </c>
+      <c r="J137" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="B138" t="s">
+        <v>38</v>
+      </c>
+      <c r="C138" t="s">
+        <v>39</v>
+      </c>
+      <c r="D138">
+        <v>12</v>
+      </c>
+      <c r="E138" t="s">
+        <v>10</v>
+      </c>
+      <c r="F138" t="s">
+        <v>16</v>
+      </c>
+      <c r="G138" t="s">
+        <v>26</v>
+      </c>
+      <c r="H138" t="s">
+        <v>28</v>
+      </c>
+      <c r="I138" t="s">
+        <v>13</v>
+      </c>
+      <c r="J138" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <v>41.9</v>
+      </c>
+      <c r="B139" t="s">
+        <v>38</v>
+      </c>
+      <c r="C139" t="s">
+        <v>39</v>
+      </c>
+      <c r="D139">
+        <v>22</v>
+      </c>
+      <c r="E139" t="s">
+        <v>10</v>
+      </c>
+      <c r="F139" t="s">
+        <v>16</v>
+      </c>
+      <c r="G139" t="s">
+        <v>26</v>
+      </c>
+      <c r="H139" t="s">
+        <v>28</v>
+      </c>
+      <c r="I139" t="s">
+        <v>13</v>
+      </c>
+      <c r="J139" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <v>34.5</v>
+      </c>
+      <c r="B140" t="s">
+        <v>38</v>
+      </c>
+      <c r="C140" t="s">
+        <v>39</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+      <c r="E140" t="s">
+        <v>11</v>
+      </c>
+      <c r="F140" t="s">
+        <v>16</v>
+      </c>
+      <c r="G140" t="s">
+        <v>26</v>
+      </c>
+      <c r="H140" t="s">
+        <v>28</v>
+      </c>
+      <c r="I140" t="s">
+        <v>14</v>
+      </c>
+      <c r="J140" t="s">
+        <v>31</v>
+      </c>
+      <c r="K140" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <v>39</v>
+      </c>
+      <c r="B141" t="s">
+        <v>38</v>
+      </c>
+      <c r="C141" t="s">
+        <v>39</v>
+      </c>
+      <c r="D141">
+        <v>12</v>
+      </c>
+      <c r="E141" t="s">
+        <v>11</v>
+      </c>
+      <c r="F141" t="s">
+        <v>16</v>
+      </c>
+      <c r="G141" t="s">
+        <v>26</v>
+      </c>
+      <c r="H141" t="s">
+        <v>28</v>
+      </c>
+      <c r="I141" t="s">
+        <v>14</v>
+      </c>
+      <c r="J141" t="s">
+        <v>31</v>
+      </c>
+      <c r="K141" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <v>42.6</v>
+      </c>
+      <c r="B142" t="s">
+        <v>38</v>
+      </c>
+      <c r="C142" t="s">
+        <v>39</v>
+      </c>
+      <c r="D142">
+        <v>22</v>
+      </c>
+      <c r="E142" t="s">
+        <v>11</v>
+      </c>
+      <c r="F142" t="s">
+        <v>16</v>
+      </c>
+      <c r="G142" t="s">
+        <v>26</v>
+      </c>
+      <c r="H142" t="s">
+        <v>28</v>
+      </c>
+      <c r="I142" t="s">
+        <v>14</v>
+      </c>
+      <c r="J142" t="s">
+        <v>31</v>
+      </c>
+      <c r="K142" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="B143" t="s">
+        <v>38</v>
+      </c>
+      <c r="C143" t="s">
+        <v>39</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+      <c r="E143" t="s">
+        <v>11</v>
+      </c>
+      <c r="F143" t="s">
+        <v>16</v>
+      </c>
+      <c r="G143" t="s">
+        <v>26</v>
+      </c>
+      <c r="H143" t="s">
+        <v>28</v>
+      </c>
+      <c r="I143" t="s">
+        <v>14</v>
+      </c>
+      <c r="J143" t="s">
+        <v>31</v>
+      </c>
+      <c r="K143" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <v>38.1</v>
+      </c>
+      <c r="B144" t="s">
+        <v>38</v>
+      </c>
+      <c r="C144" t="s">
+        <v>39</v>
+      </c>
+      <c r="D144">
+        <v>12</v>
+      </c>
+      <c r="E144" t="s">
+        <v>11</v>
+      </c>
+      <c r="F144" t="s">
+        <v>16</v>
+      </c>
+      <c r="G144" t="s">
+        <v>26</v>
+      </c>
+      <c r="H144" t="s">
+        <v>28</v>
+      </c>
+      <c r="I144" t="s">
+        <v>14</v>
+      </c>
+      <c r="J144" t="s">
+        <v>31</v>
+      </c>
+      <c r="K144" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <v>41</v>
+      </c>
+      <c r="B145" t="s">
+        <v>38</v>
+      </c>
+      <c r="C145" t="s">
+        <v>39</v>
+      </c>
+      <c r="D145">
+        <v>22</v>
+      </c>
+      <c r="E145" t="s">
+        <v>11</v>
+      </c>
+      <c r="F145" t="s">
+        <v>16</v>
+      </c>
+      <c r="G145" t="s">
+        <v>26</v>
+      </c>
+      <c r="H145" t="s">
+        <v>28</v>
+      </c>
+      <c r="I145" t="s">
+        <v>14</v>
+      </c>
+      <c r="J145" t="s">
+        <v>31</v>
+      </c>
+      <c r="K145" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A146" s="5">
+        <v>103.6</v>
+      </c>
+      <c r="B146" t="s">
+        <v>40</v>
+      </c>
+      <c r="C146" t="s">
+        <v>41</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+      <c r="E146" t="s">
+        <v>9</v>
+      </c>
+      <c r="F146" t="s">
+        <v>16</v>
+      </c>
+      <c r="G146" t="s">
+        <v>26</v>
+      </c>
+      <c r="H146" t="s">
+        <v>28</v>
+      </c>
+      <c r="I146" t="s">
+        <v>13</v>
+      </c>
+      <c r="J146" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A147" s="5">
+        <v>174.5</v>
+      </c>
+      <c r="B147" t="s">
+        <v>40</v>
+      </c>
+      <c r="C147" t="s">
+        <v>41</v>
+      </c>
+      <c r="D147">
+        <v>12</v>
+      </c>
+      <c r="E147" t="s">
+        <v>9</v>
+      </c>
+      <c r="F147" t="s">
+        <v>16</v>
+      </c>
+      <c r="G147" t="s">
+        <v>26</v>
+      </c>
+      <c r="H147" t="s">
+        <v>28</v>
+      </c>
+      <c r="I147" t="s">
+        <v>13</v>
+      </c>
+      <c r="J147" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A148" s="5">
+        <v>237.3</v>
+      </c>
+      <c r="B148" t="s">
+        <v>40</v>
+      </c>
+      <c r="C148" t="s">
+        <v>41</v>
+      </c>
+      <c r="D148">
+        <v>22</v>
+      </c>
+      <c r="E148" t="s">
+        <v>9</v>
+      </c>
+      <c r="F148" t="s">
+        <v>16</v>
+      </c>
+      <c r="G148" t="s">
+        <v>26</v>
+      </c>
+      <c r="H148" t="s">
+        <v>28</v>
+      </c>
+      <c r="I148" t="s">
+        <v>13</v>
+      </c>
+      <c r="J148" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A149" s="5">
+        <v>58.6</v>
+      </c>
+      <c r="B149" t="s">
+        <v>40</v>
+      </c>
+      <c r="C149" t="s">
+        <v>41</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+      <c r="E149" t="s">
+        <v>10</v>
+      </c>
+      <c r="F149" t="s">
+        <v>16</v>
+      </c>
+      <c r="G149" t="s">
+        <v>26</v>
+      </c>
+      <c r="H149" t="s">
+        <v>28</v>
+      </c>
+      <c r="I149" t="s">
+        <v>13</v>
+      </c>
+      <c r="J149" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A150" s="5">
+        <v>104.3</v>
+      </c>
+      <c r="B150" t="s">
+        <v>40</v>
+      </c>
+      <c r="C150" t="s">
+        <v>41</v>
+      </c>
+      <c r="D150">
+        <v>12</v>
+      </c>
+      <c r="E150" t="s">
+        <v>10</v>
+      </c>
+      <c r="F150" t="s">
+        <v>16</v>
+      </c>
+      <c r="G150" t="s">
+        <v>26</v>
+      </c>
+      <c r="H150" t="s">
+        <v>28</v>
+      </c>
+      <c r="I150" t="s">
+        <v>13</v>
+      </c>
+      <c r="J150" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A151" s="5">
+        <v>174.5</v>
+      </c>
+      <c r="B151" t="s">
+        <v>40</v>
+      </c>
+      <c r="C151" t="s">
+        <v>41</v>
+      </c>
+      <c r="D151">
+        <v>22</v>
+      </c>
+      <c r="E151" t="s">
+        <v>10</v>
+      </c>
+      <c r="F151" t="s">
+        <v>16</v>
+      </c>
+      <c r="G151" t="s">
+        <v>26</v>
+      </c>
+      <c r="H151" t="s">
+        <v>28</v>
+      </c>
+      <c r="I151" t="s">
+        <v>13</v>
+      </c>
+      <c r="J151" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A152" s="5">
+        <v>73</v>
+      </c>
+      <c r="B152" t="s">
+        <v>40</v>
+      </c>
+      <c r="C152" t="s">
+        <v>41</v>
+      </c>
+      <c r="D152">
+        <v>1</v>
+      </c>
+      <c r="E152" t="s">
+        <v>11</v>
+      </c>
+      <c r="F152" t="s">
+        <v>16</v>
+      </c>
+      <c r="G152" t="s">
+        <v>26</v>
+      </c>
+      <c r="H152" t="s">
+        <v>28</v>
+      </c>
+      <c r="I152" t="s">
+        <v>14</v>
+      </c>
+      <c r="J152" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A153" s="5">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="B153" t="s">
+        <v>40</v>
+      </c>
+      <c r="C153" t="s">
+        <v>41</v>
+      </c>
+      <c r="D153">
+        <v>12</v>
+      </c>
+      <c r="E153" t="s">
+        <v>11</v>
+      </c>
+      <c r="F153" t="s">
+        <v>16</v>
+      </c>
+      <c r="G153" t="s">
+        <v>26</v>
+      </c>
+      <c r="H153" t="s">
+        <v>28</v>
+      </c>
+      <c r="I153" t="s">
+        <v>14</v>
+      </c>
+      <c r="J153" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A154" s="5">
+        <v>135.69999999999999</v>
+      </c>
+      <c r="B154" t="s">
+        <v>40</v>
+      </c>
+      <c r="C154" t="s">
+        <v>41</v>
+      </c>
+      <c r="D154">
+        <v>22</v>
+      </c>
+      <c r="E154" t="s">
+        <v>11</v>
+      </c>
+      <c r="F154" t="s">
+        <v>16</v>
+      </c>
+      <c r="G154" t="s">
+        <v>26</v>
+      </c>
+      <c r="H154" t="s">
+        <v>28</v>
+      </c>
+      <c r="I154" t="s">
+        <v>14</v>
+      </c>
+      <c r="J154" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A155" s="5">
+        <v>47.7</v>
+      </c>
+      <c r="B155" t="s">
+        <v>40</v>
+      </c>
+      <c r="C155" t="s">
+        <v>41</v>
+      </c>
+      <c r="D155">
+        <v>1</v>
+      </c>
+      <c r="E155" t="s">
+        <v>11</v>
+      </c>
+      <c r="F155" t="s">
+        <v>16</v>
+      </c>
+      <c r="G155" t="s">
+        <v>26</v>
+      </c>
+      <c r="H155" t="s">
+        <v>28</v>
+      </c>
+      <c r="I155" t="s">
+        <v>15</v>
+      </c>
+      <c r="J155" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A156" s="5">
+        <v>22.5</v>
+      </c>
+      <c r="B156" t="s">
+        <v>40</v>
+      </c>
+      <c r="C156" t="s">
+        <v>41</v>
+      </c>
+      <c r="D156">
+        <v>12</v>
+      </c>
+      <c r="E156" t="s">
+        <v>11</v>
+      </c>
+      <c r="F156" t="s">
+        <v>16</v>
+      </c>
+      <c r="G156" t="s">
+        <v>26</v>
+      </c>
+      <c r="H156" t="s">
+        <v>28</v>
+      </c>
+      <c r="I156" t="s">
+        <v>15</v>
+      </c>
+      <c r="J156" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A157" s="5">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="B157" t="s">
+        <v>40</v>
+      </c>
+      <c r="C157" t="s">
+        <v>41</v>
+      </c>
+      <c r="D157">
+        <v>22</v>
+      </c>
+      <c r="E157" t="s">
+        <v>11</v>
+      </c>
+      <c r="F157" t="s">
+        <v>16</v>
+      </c>
+      <c r="G157" t="s">
+        <v>26</v>
+      </c>
+      <c r="H157" t="s">
+        <v>28</v>
+      </c>
+      <c r="I157" t="s">
+        <v>15</v>
+      </c>
+      <c r="J157" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A158" s="5">
+        <v>382.9</v>
+      </c>
+      <c r="B158" t="s">
+        <v>40</v>
+      </c>
+      <c r="C158" t="s">
+        <v>41</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
+      </c>
+      <c r="E158" t="s">
+        <v>9</v>
+      </c>
+      <c r="F158" t="s">
+        <v>16</v>
+      </c>
+      <c r="G158" t="s">
+        <v>26</v>
+      </c>
+      <c r="H158" t="s">
+        <v>28</v>
+      </c>
+      <c r="I158" t="s">
+        <v>13</v>
+      </c>
+      <c r="J158" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A159" s="5">
+        <v>461.7</v>
+      </c>
+      <c r="B159" t="s">
+        <v>40</v>
+      </c>
+      <c r="C159" t="s">
+        <v>41</v>
+      </c>
+      <c r="D159">
+        <v>12</v>
+      </c>
+      <c r="E159" t="s">
+        <v>9</v>
+      </c>
+      <c r="F159" t="s">
+        <v>16</v>
+      </c>
+      <c r="G159" t="s">
+        <v>26</v>
+      </c>
+      <c r="H159" t="s">
+        <v>28</v>
+      </c>
+      <c r="I159" t="s">
+        <v>13</v>
+      </c>
+      <c r="J159" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A160" s="5">
+        <v>613.70000000000005</v>
+      </c>
+      <c r="B160" t="s">
+        <v>40</v>
+      </c>
+      <c r="C160" t="s">
+        <v>41</v>
+      </c>
+      <c r="D160">
+        <v>22</v>
+      </c>
+      <c r="E160" t="s">
+        <v>9</v>
+      </c>
+      <c r="F160" t="s">
+        <v>16</v>
+      </c>
+      <c r="G160" t="s">
+        <v>26</v>
+      </c>
+      <c r="H160" t="s">
+        <v>28</v>
+      </c>
+      <c r="I160" t="s">
+        <v>13</v>
+      </c>
+      <c r="J160" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A161" s="5">
+        <v>101.4</v>
+      </c>
+      <c r="B161" t="s">
+        <v>40</v>
+      </c>
+      <c r="C161" t="s">
+        <v>41</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+      <c r="E161" t="s">
+        <v>10</v>
+      </c>
+      <c r="F161" t="s">
+        <v>16</v>
+      </c>
+      <c r="G161" t="s">
+        <v>26</v>
+      </c>
+      <c r="H161" t="s">
+        <v>28</v>
+      </c>
+      <c r="I161" t="s">
+        <v>13</v>
+      </c>
+      <c r="J161" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A162" s="5">
+        <v>692.6</v>
+      </c>
+      <c r="B162" t="s">
+        <v>40</v>
+      </c>
+      <c r="C162" t="s">
+        <v>41</v>
+      </c>
+      <c r="D162">
+        <v>12</v>
+      </c>
+      <c r="E162" t="s">
+        <v>10</v>
+      </c>
+      <c r="F162" t="s">
+        <v>16</v>
+      </c>
+      <c r="G162" t="s">
+        <v>26</v>
+      </c>
+      <c r="H162" t="s">
+        <v>28</v>
+      </c>
+      <c r="I162" t="s">
+        <v>13</v>
+      </c>
+      <c r="J162" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A163" s="5">
+        <v>1525.9</v>
+      </c>
+      <c r="B163" t="s">
+        <v>40</v>
+      </c>
+      <c r="C163" t="s">
+        <v>41</v>
+      </c>
+      <c r="D163">
+        <v>22</v>
+      </c>
+      <c r="E163" t="s">
+        <v>10</v>
+      </c>
+      <c r="F163" t="s">
+        <v>16</v>
+      </c>
+      <c r="G163" t="s">
+        <v>26</v>
+      </c>
+      <c r="H163" t="s">
+        <v>28</v>
+      </c>
+      <c r="I163" t="s">
+        <v>13</v>
+      </c>
+      <c r="J163" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A164" s="5">
+        <v>16.899999999999999</v>
+      </c>
+      <c r="B164" t="s">
+        <v>40</v>
+      </c>
+      <c r="C164" t="s">
+        <v>41</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+      <c r="E164" t="s">
+        <v>11</v>
+      </c>
+      <c r="F164" t="s">
+        <v>16</v>
+      </c>
+      <c r="G164" t="s">
+        <v>26</v>
+      </c>
+      <c r="H164" t="s">
+        <v>28</v>
+      </c>
+      <c r="I164" t="s">
+        <v>14</v>
+      </c>
+      <c r="J164" t="s">
+        <v>31</v>
+      </c>
+      <c r="K164" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A165" s="5">
+        <v>28.2</v>
+      </c>
+      <c r="B165" t="s">
+        <v>40</v>
+      </c>
+      <c r="C165" t="s">
+        <v>41</v>
+      </c>
+      <c r="D165">
+        <v>12</v>
+      </c>
+      <c r="E165" t="s">
+        <v>11</v>
+      </c>
+      <c r="F165" t="s">
+        <v>16</v>
+      </c>
+      <c r="G165" t="s">
+        <v>26</v>
+      </c>
+      <c r="H165" t="s">
+        <v>28</v>
+      </c>
+      <c r="I165" t="s">
+        <v>14</v>
+      </c>
+      <c r="J165" t="s">
+        <v>31</v>
+      </c>
+      <c r="K165" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A166" s="5">
+        <v>478.6</v>
+      </c>
+      <c r="B166" t="s">
+        <v>40</v>
+      </c>
+      <c r="C166" t="s">
+        <v>41</v>
+      </c>
+      <c r="D166">
+        <v>22</v>
+      </c>
+      <c r="E166" t="s">
+        <v>11</v>
+      </c>
+      <c r="F166" t="s">
+        <v>16</v>
+      </c>
+      <c r="G166" t="s">
+        <v>26</v>
+      </c>
+      <c r="H166" t="s">
+        <v>28</v>
+      </c>
+      <c r="I166" t="s">
+        <v>14</v>
+      </c>
+      <c r="J166" t="s">
+        <v>31</v>
+      </c>
+      <c r="K166" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A167" s="5">
+        <v>45</v>
+      </c>
+      <c r="B167" t="s">
+        <v>40</v>
+      </c>
+      <c r="C167" t="s">
+        <v>41</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+      <c r="E167" t="s">
+        <v>11</v>
+      </c>
+      <c r="F167" t="s">
+        <v>16</v>
+      </c>
+      <c r="G167" t="s">
+        <v>26</v>
+      </c>
+      <c r="H167" t="s">
+        <v>28</v>
+      </c>
+      <c r="I167" t="s">
+        <v>14</v>
+      </c>
+      <c r="J167" t="s">
+        <v>31</v>
+      </c>
+      <c r="K167" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A168" s="5">
+        <v>123.9</v>
+      </c>
+      <c r="B168" t="s">
+        <v>40</v>
+      </c>
+      <c r="C168" t="s">
+        <v>41</v>
+      </c>
+      <c r="D168">
+        <v>12</v>
+      </c>
+      <c r="E168" t="s">
+        <v>11</v>
+      </c>
+      <c r="F168" t="s">
+        <v>16</v>
+      </c>
+      <c r="G168" t="s">
+        <v>26</v>
+      </c>
+      <c r="H168" t="s">
+        <v>28</v>
+      </c>
+      <c r="I168" t="s">
+        <v>14</v>
+      </c>
+      <c r="J168" t="s">
+        <v>31</v>
+      </c>
+      <c r="K168" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A169" s="5">
+        <v>495.5</v>
+      </c>
+      <c r="B169" t="s">
+        <v>40</v>
+      </c>
+      <c r="C169" t="s">
+        <v>41</v>
+      </c>
+      <c r="D169">
+        <v>22</v>
+      </c>
+      <c r="E169" t="s">
+        <v>11</v>
+      </c>
+      <c r="F169" t="s">
+        <v>16</v>
+      </c>
+      <c r="G169" t="s">
+        <v>26</v>
+      </c>
+      <c r="H169" t="s">
+        <v>28</v>
+      </c>
+      <c r="I169" t="s">
+        <v>14</v>
+      </c>
+      <c r="J169" t="s">
+        <v>31</v>
+      </c>
+      <c r="K169" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A170" s="5">
+        <v>134.5</v>
+      </c>
+      <c r="B170" t="s">
+        <v>42</v>
+      </c>
+      <c r="C170" t="s">
+        <v>43</v>
+      </c>
+      <c r="D170">
+        <v>12</v>
+      </c>
+      <c r="E170" t="s">
+        <v>9</v>
+      </c>
+      <c r="F170" t="s">
+        <v>16</v>
+      </c>
+      <c r="G170" t="s">
+        <v>26</v>
+      </c>
+      <c r="H170" t="s">
+        <v>28</v>
+      </c>
+      <c r="I170" t="s">
+        <v>13</v>
+      </c>
+      <c r="J170" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A171" s="5">
+        <v>274.7</v>
+      </c>
+      <c r="B171" t="s">
+        <v>42</v>
+      </c>
+      <c r="C171" t="s">
+        <v>43</v>
+      </c>
+      <c r="D171">
+        <v>22</v>
+      </c>
+      <c r="E171" t="s">
+        <v>9</v>
+      </c>
+      <c r="F171" t="s">
+        <v>16</v>
+      </c>
+      <c r="G171" t="s">
+        <v>26</v>
+      </c>
+      <c r="H171" t="s">
+        <v>28</v>
+      </c>
+      <c r="I171" t="s">
+        <v>13</v>
+      </c>
+      <c r="J171" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A172" s="5">
+        <v>16.8</v>
+      </c>
+      <c r="B172" t="s">
+        <v>42</v>
+      </c>
+      <c r="C172" t="s">
+        <v>43</v>
+      </c>
+      <c r="D172">
+        <v>12</v>
+      </c>
+      <c r="E172" t="s">
+        <v>10</v>
+      </c>
+      <c r="F172" t="s">
+        <v>16</v>
+      </c>
+      <c r="G172" t="s">
+        <v>26</v>
+      </c>
+      <c r="H172" t="s">
+        <v>28</v>
+      </c>
+      <c r="I172" t="s">
+        <v>13</v>
+      </c>
+      <c r="J172" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A173" s="5">
+        <v>773.5</v>
+      </c>
+      <c r="B173" t="s">
+        <v>42</v>
+      </c>
+      <c r="C173" t="s">
+        <v>43</v>
+      </c>
+      <c r="D173">
+        <v>22</v>
+      </c>
+      <c r="E173" t="s">
+        <v>10</v>
+      </c>
+      <c r="F173" t="s">
+        <v>16</v>
+      </c>
+      <c r="G173" t="s">
+        <v>26</v>
+      </c>
+      <c r="H173" t="s">
+        <v>28</v>
+      </c>
+      <c r="I173" t="s">
+        <v>13</v>
+      </c>
+      <c r="J173" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A174" s="5">
+        <v>11.2</v>
+      </c>
+      <c r="B174" t="s">
+        <v>42</v>
+      </c>
+      <c r="C174" t="s">
+        <v>43</v>
+      </c>
+      <c r="D174">
+        <v>12</v>
+      </c>
+      <c r="E174" t="s">
+        <v>11</v>
+      </c>
+      <c r="F174" t="s">
+        <v>16</v>
+      </c>
+      <c r="G174" t="s">
+        <v>26</v>
+      </c>
+      <c r="H174" t="s">
+        <v>28</v>
+      </c>
+      <c r="I174" t="s">
+        <v>14</v>
+      </c>
+      <c r="J174" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A175" s="5">
+        <v>1603.1</v>
+      </c>
+      <c r="B175" t="s">
+        <v>42</v>
+      </c>
+      <c r="C175" t="s">
+        <v>43</v>
+      </c>
+      <c r="D175">
+        <v>22</v>
+      </c>
+      <c r="E175" t="s">
+        <v>11</v>
+      </c>
+      <c r="F175" t="s">
+        <v>16</v>
+      </c>
+      <c r="G175" t="s">
+        <v>26</v>
+      </c>
+      <c r="H175" t="s">
+        <v>28</v>
+      </c>
+      <c r="I175" t="s">
+        <v>14</v>
+      </c>
+      <c r="J175" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A176" s="5">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="B176" t="s">
+        <v>42</v>
+      </c>
+      <c r="C176" t="s">
+        <v>43</v>
+      </c>
+      <c r="D176">
+        <v>12</v>
+      </c>
+      <c r="E176" t="s">
+        <v>11</v>
+      </c>
+      <c r="F176" t="s">
+        <v>16</v>
+      </c>
+      <c r="G176" t="s">
+        <v>26</v>
+      </c>
+      <c r="H176" t="s">
+        <v>28</v>
+      </c>
+      <c r="I176" t="s">
+        <v>15</v>
+      </c>
+      <c r="J176" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A177" s="5">
+        <v>1872.2</v>
+      </c>
+      <c r="B177" t="s">
+        <v>42</v>
+      </c>
+      <c r="C177" t="s">
+        <v>43</v>
+      </c>
+      <c r="D177">
+        <v>22</v>
+      </c>
+      <c r="E177" t="s">
+        <v>11</v>
+      </c>
+      <c r="F177" t="s">
+        <v>16</v>
+      </c>
+      <c r="G177" t="s">
+        <v>26</v>
+      </c>
+      <c r="H177" t="s">
+        <v>28</v>
+      </c>
+      <c r="I177" t="s">
+        <v>15</v>
+      </c>
+      <c r="J177" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A178" s="5">
+        <v>864.9</v>
+      </c>
+      <c r="B178" t="s">
+        <v>42</v>
+      </c>
+      <c r="C178" t="s">
+        <v>43</v>
+      </c>
+      <c r="D178">
+        <v>12</v>
+      </c>
+      <c r="E178" t="s">
+        <v>9</v>
+      </c>
+      <c r="F178" t="s">
+        <v>16</v>
+      </c>
+      <c r="G178" t="s">
+        <v>26</v>
+      </c>
+      <c r="H178" t="s">
+        <v>28</v>
+      </c>
+      <c r="I178" t="s">
+        <v>13</v>
+      </c>
+      <c r="J178" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A179" s="5">
+        <v>4810.8</v>
+      </c>
+      <c r="B179" t="s">
+        <v>42</v>
+      </c>
+      <c r="C179" t="s">
+        <v>43</v>
+      </c>
+      <c r="D179">
+        <v>22</v>
+      </c>
+      <c r="E179" t="s">
+        <v>9</v>
+      </c>
+      <c r="F179" t="s">
+        <v>16</v>
+      </c>
+      <c r="G179" t="s">
+        <v>26</v>
+      </c>
+      <c r="H179" t="s">
+        <v>28</v>
+      </c>
+      <c r="I179" t="s">
+        <v>13</v>
+      </c>
+      <c r="J179" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A180" s="5">
+        <v>2000</v>
+      </c>
+      <c r="B180" t="s">
+        <v>42</v>
+      </c>
+      <c r="C180" t="s">
+        <v>43</v>
+      </c>
+      <c r="D180">
+        <v>12</v>
+      </c>
+      <c r="E180" t="s">
+        <v>10</v>
+      </c>
+      <c r="F180" t="s">
+        <v>16</v>
+      </c>
+      <c r="G180" t="s">
+        <v>26</v>
+      </c>
+      <c r="H180" t="s">
+        <v>28</v>
+      </c>
+      <c r="I180" t="s">
+        <v>13</v>
+      </c>
+      <c r="J180" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A181" s="5">
+        <v>3202.7</v>
+      </c>
+      <c r="B181" t="s">
+        <v>42</v>
+      </c>
+      <c r="C181" t="s">
+        <v>43</v>
+      </c>
+      <c r="D181">
+        <v>22</v>
+      </c>
+      <c r="E181" t="s">
+        <v>10</v>
+      </c>
+      <c r="F181" t="s">
+        <v>16</v>
+      </c>
+      <c r="G181" t="s">
+        <v>26</v>
+      </c>
+      <c r="H181" t="s">
+        <v>28</v>
+      </c>
+      <c r="I181" t="s">
+        <v>13</v>
+      </c>
+      <c r="J181" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A182" s="5">
+        <v>621.6</v>
+      </c>
+      <c r="B182" t="s">
+        <v>42</v>
+      </c>
+      <c r="C182" t="s">
+        <v>43</v>
+      </c>
+      <c r="D182">
+        <v>12</v>
+      </c>
+      <c r="E182" t="s">
+        <v>11</v>
+      </c>
+      <c r="F182" t="s">
+        <v>16</v>
+      </c>
+      <c r="G182" t="s">
+        <v>26</v>
+      </c>
+      <c r="H182" t="s">
+        <v>28</v>
+      </c>
+      <c r="I182" t="s">
+        <v>14</v>
+      </c>
+      <c r="J182" t="s">
+        <v>31</v>
+      </c>
+      <c r="K182" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A183" s="5">
+        <v>3878.4</v>
+      </c>
+      <c r="B183" t="s">
+        <v>42</v>
+      </c>
+      <c r="C183" t="s">
+        <v>43</v>
+      </c>
+      <c r="D183">
+        <v>22</v>
+      </c>
+      <c r="E183" t="s">
+        <v>11</v>
+      </c>
+      <c r="F183" t="s">
+        <v>16</v>
+      </c>
+      <c r="G183" t="s">
+        <v>26</v>
+      </c>
+      <c r="H183" t="s">
+        <v>28</v>
+      </c>
+      <c r="I183" t="s">
+        <v>14</v>
+      </c>
+      <c r="J183" t="s">
+        <v>31</v>
+      </c>
+      <c r="K183" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A184" s="5">
+        <v>567.6</v>
+      </c>
+      <c r="B184" t="s">
+        <v>42</v>
+      </c>
+      <c r="C184" t="s">
+        <v>43</v>
+      </c>
+      <c r="D184">
+        <v>12</v>
+      </c>
+      <c r="E184" t="s">
+        <v>11</v>
+      </c>
+      <c r="F184" t="s">
+        <v>16</v>
+      </c>
+      <c r="G184" t="s">
+        <v>26</v>
+      </c>
+      <c r="H184" t="s">
+        <v>28</v>
+      </c>
+      <c r="I184" t="s">
+        <v>14</v>
+      </c>
+      <c r="J184" t="s">
+        <v>31</v>
+      </c>
+      <c r="K184" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A185" s="5">
+        <v>2094.6</v>
+      </c>
+      <c r="B185" t="s">
+        <v>42</v>
+      </c>
+      <c r="C185" t="s">
+        <v>43</v>
+      </c>
+      <c r="D185">
+        <v>22</v>
+      </c>
+      <c r="E185" t="s">
+        <v>11</v>
+      </c>
+      <c r="F185" t="s">
+        <v>16</v>
+      </c>
+      <c r="G185" t="s">
+        <v>26</v>
+      </c>
+      <c r="H185" t="s">
+        <v>28</v>
+      </c>
+      <c r="I185" t="s">
+        <v>14</v>
+      </c>
+      <c r="J185" t="s">
+        <v>31</v>
+      </c>
+      <c r="K185" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
started digitizing Morici data
</commit_message>
<xml_diff>
--- a/data/web_plot_digitizer_data.xlsx
+++ b/data/web_plot_digitizer_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramR\fuels_longevity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4844266-17CE-4DCB-A378-939ACEC90944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B54422B-014D-4F78-B33C-D063C378C4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6245A06B-15CE-492B-AD18-D354A95DB25A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1541" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="52">
   <si>
     <t>variable</t>
   </si>
@@ -172,13 +172,37 @@
   <si>
     <t>seedlings/ha</t>
   </si>
+  <si>
+    <t>all_woody</t>
+  </si>
+  <si>
+    <t>cwd_sound</t>
+  </si>
+  <si>
+    <t>cwd_rotten</t>
+  </si>
+  <si>
+    <t>hundred_hour</t>
+  </si>
+  <si>
+    <t>ten_hour</t>
+  </si>
+  <si>
+    <t>one_hour</t>
+  </si>
+  <si>
+    <t>Mg/ha</t>
+  </si>
+  <si>
+    <t>morici</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -221,10 +245,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -589,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A8627B-2386-4DAF-99DA-19F1EA4382AF}">
-  <dimension ref="A1:K185"/>
+  <dimension ref="A1:K209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A144" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I160" sqref="I160"/>
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G180" sqref="G180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1054,7 +1078,7 @@
         <v>13</v>
       </c>
       <c r="J14" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -1086,7 +1110,7 @@
         <v>13</v>
       </c>
       <c r="J15" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -1462,7 +1486,7 @@
         <v>13</v>
       </c>
       <c r="J26" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -1494,7 +1518,7 @@
         <v>13</v>
       </c>
       <c r="J27" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -1846,7 +1870,7 @@
         <v>13</v>
       </c>
       <c r="J38" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -1878,7 +1902,7 @@
         <v>13</v>
       </c>
       <c r="J39" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -2254,7 +2278,7 @@
         <v>13</v>
       </c>
       <c r="J50" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
@@ -2286,7 +2310,7 @@
         <v>13</v>
       </c>
       <c r="J51" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
@@ -2638,7 +2662,7 @@
         <v>13</v>
       </c>
       <c r="J62" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
@@ -2670,7 +2694,7 @@
         <v>13</v>
       </c>
       <c r="J63" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
@@ -3046,7 +3070,7 @@
         <v>13</v>
       </c>
       <c r="J74" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
@@ -3078,7 +3102,7 @@
         <v>13</v>
       </c>
       <c r="J75" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
@@ -3110,7 +3134,7 @@
         <v>13</v>
       </c>
       <c r="J76" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
@@ -3430,7 +3454,7 @@
         <v>13</v>
       </c>
       <c r="J86" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
@@ -3462,7 +3486,7 @@
         <v>13</v>
       </c>
       <c r="J87" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.3">
@@ -3494,7 +3518,7 @@
         <v>13</v>
       </c>
       <c r="J88" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.3">
@@ -3832,7 +3856,7 @@
         <v>13</v>
       </c>
       <c r="J98" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.3">
@@ -3864,7 +3888,7 @@
         <v>13</v>
       </c>
       <c r="J99" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.3">
@@ -3896,7 +3920,7 @@
         <v>13</v>
       </c>
       <c r="J100" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.3">
@@ -4216,7 +4240,7 @@
         <v>13</v>
       </c>
       <c r="J110" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.3">
@@ -4248,7 +4272,7 @@
         <v>13</v>
       </c>
       <c r="J111" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.3">
@@ -4280,7 +4304,7 @@
         <v>13</v>
       </c>
       <c r="J112" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.3">
@@ -4618,7 +4642,7 @@
         <v>13</v>
       </c>
       <c r="J122" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.3">
@@ -4650,7 +4674,7 @@
         <v>13</v>
       </c>
       <c r="J123" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.3">
@@ -4682,7 +4706,7 @@
         <v>13</v>
       </c>
       <c r="J124" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.3">
@@ -5002,7 +5026,7 @@
         <v>13</v>
       </c>
       <c r="J134" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.3">
@@ -5034,7 +5058,7 @@
         <v>13</v>
       </c>
       <c r="J135" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.3">
@@ -5066,7 +5090,7 @@
         <v>13</v>
       </c>
       <c r="J136" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.3">
@@ -5404,7 +5428,7 @@
         <v>13</v>
       </c>
       <c r="J146" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.3">
@@ -5436,7 +5460,7 @@
         <v>13</v>
       </c>
       <c r="J147" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.3">
@@ -5468,7 +5492,7 @@
         <v>13</v>
       </c>
       <c r="J148" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.3">
@@ -5788,7 +5812,7 @@
         <v>13</v>
       </c>
       <c r="J158" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.3">
@@ -5820,7 +5844,7 @@
         <v>13</v>
       </c>
       <c r="J159" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.3">
@@ -5852,7 +5876,7 @@
         <v>13</v>
       </c>
       <c r="J160" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.3">
@@ -6190,7 +6214,7 @@
         <v>13</v>
       </c>
       <c r="J170" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.3">
@@ -6222,7 +6246,7 @@
         <v>13</v>
       </c>
       <c r="J171" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.3">
@@ -6446,7 +6470,7 @@
         <v>13</v>
       </c>
       <c r="J178" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.3">
@@ -6478,7 +6502,7 @@
         <v>13</v>
       </c>
       <c r="J179" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.3">
@@ -6683,6 +6707,846 @@
       </c>
       <c r="K185" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A186">
+        <v>23.9</v>
+      </c>
+      <c r="B186" t="s">
+        <v>44</v>
+      </c>
+      <c r="C186" t="s">
+        <v>50</v>
+      </c>
+      <c r="D186">
+        <v>0</v>
+      </c>
+      <c r="E186" t="s">
+        <v>9</v>
+      </c>
+      <c r="F186" t="s">
+        <v>51</v>
+      </c>
+      <c r="G186" t="s">
+        <v>26</v>
+      </c>
+      <c r="H186" t="s">
+        <v>28</v>
+      </c>
+      <c r="I186" t="s">
+        <v>13</v>
+      </c>
+      <c r="J186" t="s">
+        <v>13</v>
+      </c>
+      <c r="K186" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A187">
+        <v>19.3</v>
+      </c>
+      <c r="B187" t="s">
+        <v>44</v>
+      </c>
+      <c r="C187" t="s">
+        <v>50</v>
+      </c>
+      <c r="D187">
+        <v>8</v>
+      </c>
+      <c r="E187" t="s">
+        <v>9</v>
+      </c>
+      <c r="F187" t="s">
+        <v>51</v>
+      </c>
+      <c r="G187" t="s">
+        <v>26</v>
+      </c>
+      <c r="H187" t="s">
+        <v>28</v>
+      </c>
+      <c r="I187" t="s">
+        <v>13</v>
+      </c>
+      <c r="J187" t="s">
+        <v>13</v>
+      </c>
+      <c r="K187" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A188">
+        <v>25</v>
+      </c>
+      <c r="B188" t="s">
+        <v>44</v>
+      </c>
+      <c r="C188" t="s">
+        <v>50</v>
+      </c>
+      <c r="D188">
+        <v>17</v>
+      </c>
+      <c r="E188" t="s">
+        <v>9</v>
+      </c>
+      <c r="F188" t="s">
+        <v>51</v>
+      </c>
+      <c r="G188" t="s">
+        <v>26</v>
+      </c>
+      <c r="H188" t="s">
+        <v>28</v>
+      </c>
+      <c r="I188" t="s">
+        <v>13</v>
+      </c>
+      <c r="J188" t="s">
+        <v>13</v>
+      </c>
+      <c r="K188" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A189">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="B189" t="s">
+        <v>32</v>
+      </c>
+      <c r="C189" t="s">
+        <v>50</v>
+      </c>
+      <c r="D189">
+        <v>0</v>
+      </c>
+      <c r="E189" t="s">
+        <v>9</v>
+      </c>
+      <c r="F189" t="s">
+        <v>51</v>
+      </c>
+      <c r="G189" t="s">
+        <v>26</v>
+      </c>
+      <c r="H189" t="s">
+        <v>28</v>
+      </c>
+      <c r="I189" t="s">
+        <v>13</v>
+      </c>
+      <c r="J189" t="s">
+        <v>13</v>
+      </c>
+      <c r="K189" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A190">
+        <v>15.3</v>
+      </c>
+      <c r="B190" t="s">
+        <v>32</v>
+      </c>
+      <c r="C190" t="s">
+        <v>50</v>
+      </c>
+      <c r="D190">
+        <v>8</v>
+      </c>
+      <c r="E190" t="s">
+        <v>9</v>
+      </c>
+      <c r="F190" t="s">
+        <v>51</v>
+      </c>
+      <c r="G190" t="s">
+        <v>26</v>
+      </c>
+      <c r="H190" t="s">
+        <v>28</v>
+      </c>
+      <c r="I190" t="s">
+        <v>13</v>
+      </c>
+      <c r="J190" t="s">
+        <v>13</v>
+      </c>
+      <c r="K190" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A191">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="B191" t="s">
+        <v>32</v>
+      </c>
+      <c r="C191" t="s">
+        <v>50</v>
+      </c>
+      <c r="D191">
+        <v>17</v>
+      </c>
+      <c r="E191" t="s">
+        <v>9</v>
+      </c>
+      <c r="F191" t="s">
+        <v>51</v>
+      </c>
+      <c r="G191" t="s">
+        <v>26</v>
+      </c>
+      <c r="H191" t="s">
+        <v>28</v>
+      </c>
+      <c r="I191" t="s">
+        <v>13</v>
+      </c>
+      <c r="J191" t="s">
+        <v>13</v>
+      </c>
+      <c r="K191" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A192">
+        <v>10</v>
+      </c>
+      <c r="B192" t="s">
+        <v>45</v>
+      </c>
+      <c r="C192" t="s">
+        <v>50</v>
+      </c>
+      <c r="D192">
+        <v>0</v>
+      </c>
+      <c r="E192" t="s">
+        <v>9</v>
+      </c>
+      <c r="F192" t="s">
+        <v>51</v>
+      </c>
+      <c r="G192" t="s">
+        <v>26</v>
+      </c>
+      <c r="H192" t="s">
+        <v>28</v>
+      </c>
+      <c r="I192" t="s">
+        <v>13</v>
+      </c>
+      <c r="J192" t="s">
+        <v>13</v>
+      </c>
+      <c r="K192" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A193">
+        <v>8.4</v>
+      </c>
+      <c r="B193" t="s">
+        <v>45</v>
+      </c>
+      <c r="C193" t="s">
+        <v>50</v>
+      </c>
+      <c r="D193">
+        <v>8</v>
+      </c>
+      <c r="E193" t="s">
+        <v>9</v>
+      </c>
+      <c r="F193" t="s">
+        <v>51</v>
+      </c>
+      <c r="G193" t="s">
+        <v>26</v>
+      </c>
+      <c r="H193" t="s">
+        <v>28</v>
+      </c>
+      <c r="I193" t="s">
+        <v>13</v>
+      </c>
+      <c r="J193" t="s">
+        <v>13</v>
+      </c>
+      <c r="K193" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A194">
+        <v>3.7</v>
+      </c>
+      <c r="B194" t="s">
+        <v>45</v>
+      </c>
+      <c r="C194" t="s">
+        <v>50</v>
+      </c>
+      <c r="D194">
+        <v>17</v>
+      </c>
+      <c r="E194" t="s">
+        <v>9</v>
+      </c>
+      <c r="F194" t="s">
+        <v>51</v>
+      </c>
+      <c r="G194" t="s">
+        <v>26</v>
+      </c>
+      <c r="H194" t="s">
+        <v>28</v>
+      </c>
+      <c r="I194" t="s">
+        <v>13</v>
+      </c>
+      <c r="J194" t="s">
+        <v>13</v>
+      </c>
+      <c r="K194" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A195">
+        <v>7.4</v>
+      </c>
+      <c r="B195" t="s">
+        <v>46</v>
+      </c>
+      <c r="C195" t="s">
+        <v>50</v>
+      </c>
+      <c r="D195">
+        <v>0</v>
+      </c>
+      <c r="E195" t="s">
+        <v>9</v>
+      </c>
+      <c r="F195" t="s">
+        <v>51</v>
+      </c>
+      <c r="G195" t="s">
+        <v>26</v>
+      </c>
+      <c r="H195" t="s">
+        <v>28</v>
+      </c>
+      <c r="I195" t="s">
+        <v>13</v>
+      </c>
+      <c r="J195" t="s">
+        <v>13</v>
+      </c>
+      <c r="K195" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A196">
+        <v>6.9</v>
+      </c>
+      <c r="B196" t="s">
+        <v>46</v>
+      </c>
+      <c r="C196" t="s">
+        <v>50</v>
+      </c>
+      <c r="D196">
+        <v>8</v>
+      </c>
+      <c r="E196" t="s">
+        <v>9</v>
+      </c>
+      <c r="F196" t="s">
+        <v>51</v>
+      </c>
+      <c r="G196" t="s">
+        <v>26</v>
+      </c>
+      <c r="H196" t="s">
+        <v>28</v>
+      </c>
+      <c r="I196" t="s">
+        <v>13</v>
+      </c>
+      <c r="J196" t="s">
+        <v>13</v>
+      </c>
+      <c r="K196" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A197">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="B197" t="s">
+        <v>46</v>
+      </c>
+      <c r="C197" t="s">
+        <v>50</v>
+      </c>
+      <c r="D197">
+        <v>17</v>
+      </c>
+      <c r="E197" t="s">
+        <v>9</v>
+      </c>
+      <c r="F197" t="s">
+        <v>51</v>
+      </c>
+      <c r="G197" t="s">
+        <v>26</v>
+      </c>
+      <c r="H197" t="s">
+        <v>28</v>
+      </c>
+      <c r="I197" t="s">
+        <v>13</v>
+      </c>
+      <c r="J197" t="s">
+        <v>13</v>
+      </c>
+      <c r="K197" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A198">
+        <v>6.7</v>
+      </c>
+      <c r="B198" t="s">
+        <v>5</v>
+      </c>
+      <c r="C198" t="s">
+        <v>50</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198" t="s">
+        <v>9</v>
+      </c>
+      <c r="F198" t="s">
+        <v>51</v>
+      </c>
+      <c r="G198" t="s">
+        <v>26</v>
+      </c>
+      <c r="H198" t="s">
+        <v>28</v>
+      </c>
+      <c r="I198" t="s">
+        <v>13</v>
+      </c>
+      <c r="J198" t="s">
+        <v>13</v>
+      </c>
+      <c r="K198" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A199">
+        <v>3.9</v>
+      </c>
+      <c r="B199" t="s">
+        <v>5</v>
+      </c>
+      <c r="C199" t="s">
+        <v>50</v>
+      </c>
+      <c r="D199">
+        <v>8</v>
+      </c>
+      <c r="E199" t="s">
+        <v>9</v>
+      </c>
+      <c r="F199" t="s">
+        <v>51</v>
+      </c>
+      <c r="G199" t="s">
+        <v>26</v>
+      </c>
+      <c r="H199" t="s">
+        <v>28</v>
+      </c>
+      <c r="I199" t="s">
+        <v>13</v>
+      </c>
+      <c r="J199" t="s">
+        <v>13</v>
+      </c>
+      <c r="K199" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A200">
+        <v>4.8</v>
+      </c>
+      <c r="B200" t="s">
+        <v>5</v>
+      </c>
+      <c r="C200" t="s">
+        <v>50</v>
+      </c>
+      <c r="D200">
+        <v>17</v>
+      </c>
+      <c r="E200" t="s">
+        <v>9</v>
+      </c>
+      <c r="F200" t="s">
+        <v>51</v>
+      </c>
+      <c r="G200" t="s">
+        <v>26</v>
+      </c>
+      <c r="H200" t="s">
+        <v>28</v>
+      </c>
+      <c r="I200" t="s">
+        <v>13</v>
+      </c>
+      <c r="J200" t="s">
+        <v>13</v>
+      </c>
+      <c r="K200" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A201">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="B201" t="s">
+        <v>47</v>
+      </c>
+      <c r="C201" t="s">
+        <v>50</v>
+      </c>
+      <c r="D201">
+        <v>0</v>
+      </c>
+      <c r="E201" t="s">
+        <v>9</v>
+      </c>
+      <c r="F201" t="s">
+        <v>51</v>
+      </c>
+      <c r="G201" t="s">
+        <v>26</v>
+      </c>
+      <c r="H201" t="s">
+        <v>28</v>
+      </c>
+      <c r="I201" t="s">
+        <v>13</v>
+      </c>
+      <c r="J201" t="s">
+        <v>13</v>
+      </c>
+      <c r="K201" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A202">
+        <v>3.1</v>
+      </c>
+      <c r="B202" t="s">
+        <v>47</v>
+      </c>
+      <c r="C202" t="s">
+        <v>50</v>
+      </c>
+      <c r="D202">
+        <v>8</v>
+      </c>
+      <c r="E202" t="s">
+        <v>9</v>
+      </c>
+      <c r="F202" t="s">
+        <v>51</v>
+      </c>
+      <c r="G202" t="s">
+        <v>26</v>
+      </c>
+      <c r="H202" t="s">
+        <v>28</v>
+      </c>
+      <c r="I202" t="s">
+        <v>13</v>
+      </c>
+      <c r="J202" t="s">
+        <v>13</v>
+      </c>
+      <c r="K202" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A203">
+        <v>3.2</v>
+      </c>
+      <c r="B203" t="s">
+        <v>47</v>
+      </c>
+      <c r="C203" t="s">
+        <v>50</v>
+      </c>
+      <c r="D203">
+        <v>17</v>
+      </c>
+      <c r="E203" t="s">
+        <v>9</v>
+      </c>
+      <c r="F203" t="s">
+        <v>51</v>
+      </c>
+      <c r="G203" t="s">
+        <v>26</v>
+      </c>
+      <c r="H203" t="s">
+        <v>28</v>
+      </c>
+      <c r="I203" t="s">
+        <v>13</v>
+      </c>
+      <c r="J203" t="s">
+        <v>13</v>
+      </c>
+      <c r="K203" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A204">
+        <v>1.96</v>
+      </c>
+      <c r="B204" t="s">
+        <v>48</v>
+      </c>
+      <c r="C204" t="s">
+        <v>50</v>
+      </c>
+      <c r="D204">
+        <v>0</v>
+      </c>
+      <c r="E204" t="s">
+        <v>9</v>
+      </c>
+      <c r="F204" t="s">
+        <v>51</v>
+      </c>
+      <c r="G204" t="s">
+        <v>26</v>
+      </c>
+      <c r="H204" t="s">
+        <v>28</v>
+      </c>
+      <c r="I204" t="s">
+        <v>13</v>
+      </c>
+      <c r="J204" t="s">
+        <v>13</v>
+      </c>
+      <c r="K204" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A205">
+        <v>0.76</v>
+      </c>
+      <c r="B205" t="s">
+        <v>48</v>
+      </c>
+      <c r="C205" t="s">
+        <v>50</v>
+      </c>
+      <c r="D205">
+        <v>8</v>
+      </c>
+      <c r="E205" t="s">
+        <v>9</v>
+      </c>
+      <c r="F205" t="s">
+        <v>51</v>
+      </c>
+      <c r="G205" t="s">
+        <v>26</v>
+      </c>
+      <c r="H205" t="s">
+        <v>28</v>
+      </c>
+      <c r="I205" t="s">
+        <v>13</v>
+      </c>
+      <c r="J205" t="s">
+        <v>13</v>
+      </c>
+      <c r="K205" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A206">
+        <v>1.31</v>
+      </c>
+      <c r="B206" t="s">
+        <v>48</v>
+      </c>
+      <c r="C206" t="s">
+        <v>50</v>
+      </c>
+      <c r="D206">
+        <v>17</v>
+      </c>
+      <c r="E206" t="s">
+        <v>9</v>
+      </c>
+      <c r="F206" t="s">
+        <v>51</v>
+      </c>
+      <c r="G206" t="s">
+        <v>26</v>
+      </c>
+      <c r="H206" t="s">
+        <v>28</v>
+      </c>
+      <c r="I206" t="s">
+        <v>13</v>
+      </c>
+      <c r="J206" t="s">
+        <v>13</v>
+      </c>
+      <c r="K206" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A207">
+        <v>0.27</v>
+      </c>
+      <c r="B207" t="s">
+        <v>49</v>
+      </c>
+      <c r="C207" t="s">
+        <v>50</v>
+      </c>
+      <c r="D207">
+        <v>0</v>
+      </c>
+      <c r="E207" t="s">
+        <v>9</v>
+      </c>
+      <c r="F207" t="s">
+        <v>51</v>
+      </c>
+      <c r="G207" t="s">
+        <v>26</v>
+      </c>
+      <c r="H207" t="s">
+        <v>28</v>
+      </c>
+      <c r="I207" t="s">
+        <v>13</v>
+      </c>
+      <c r="J207" t="s">
+        <v>13</v>
+      </c>
+      <c r="K207" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A208">
+        <v>0.05</v>
+      </c>
+      <c r="B208" t="s">
+        <v>49</v>
+      </c>
+      <c r="C208" t="s">
+        <v>50</v>
+      </c>
+      <c r="D208">
+        <v>8</v>
+      </c>
+      <c r="E208" t="s">
+        <v>9</v>
+      </c>
+      <c r="F208" t="s">
+        <v>51</v>
+      </c>
+      <c r="G208" t="s">
+        <v>26</v>
+      </c>
+      <c r="H208" t="s">
+        <v>28</v>
+      </c>
+      <c r="I208" t="s">
+        <v>13</v>
+      </c>
+      <c r="J208" t="s">
+        <v>13</v>
+      </c>
+      <c r="K208" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A209">
+        <v>0.27</v>
+      </c>
+      <c r="B209" t="s">
+        <v>49</v>
+      </c>
+      <c r="C209" t="s">
+        <v>50</v>
+      </c>
+      <c r="D209">
+        <v>17</v>
+      </c>
+      <c r="E209" t="s">
+        <v>9</v>
+      </c>
+      <c r="F209" t="s">
+        <v>51</v>
+      </c>
+      <c r="G209" t="s">
+        <v>26</v>
+      </c>
+      <c r="H209" t="s">
+        <v>28</v>
+      </c>
+      <c r="I209" t="s">
+        <v>13</v>
+      </c>
+      <c r="J209" t="s">
+        <v>13</v>
+      </c>
+      <c r="K209" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
One more piece of the Morici thesis digitized
</commit_message>
<xml_diff>
--- a/data/web_plot_digitizer_data.xlsx
+++ b/data/web_plot_digitizer_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramR\fuels_longevity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B54422B-014D-4F78-B33C-D063C378C4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A855DD2F-2A2D-4C4E-B3B6-BE69FE2D7149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6245A06B-15CE-492B-AD18-D354A95DB25A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1757" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1997" uniqueCount="77">
   <si>
     <t>variable</t>
   </si>
@@ -195,6 +195,81 @@
   </si>
   <si>
     <t>morici</t>
+  </si>
+  <si>
+    <t>1998.09, 10.02</t>
+  </si>
+  <si>
+    <t>2006.64, 4.14</t>
+  </si>
+  <si>
+    <t>2015.27, 8.82</t>
+  </si>
+  <si>
+    <t>1998.07, 7.52</t>
+  </si>
+  <si>
+    <t>2006.43, 2.45</t>
+  </si>
+  <si>
+    <t>2015.25, 6.75</t>
+  </si>
+  <si>
+    <t>1997.86, 5.07</t>
+  </si>
+  <si>
+    <t>2006.42, 0.44</t>
+  </si>
+  <si>
+    <t>2015.04, 4.08</t>
+  </si>
+  <si>
+    <t>1998.03, 2.61</t>
+  </si>
+  <si>
+    <t>2006.43, 1.63</t>
+  </si>
+  <si>
+    <t>2015.02, 2.07</t>
+  </si>
+  <si>
+    <t>1997.84, 2.40</t>
+  </si>
+  <si>
+    <t>2006.43, 2.07</t>
+  </si>
+  <si>
+    <t>2015.03, 2.61</t>
+  </si>
+  <si>
+    <t>1997.83, 1.91</t>
+  </si>
+  <si>
+    <t>2006.42, 1.09</t>
+  </si>
+  <si>
+    <t>2015.02, 1.20</t>
+  </si>
+  <si>
+    <t>1997.82, 0.60</t>
+  </si>
+  <si>
+    <t>2006.42, 0.38</t>
+  </si>
+  <si>
+    <t>2015.01, 0.76</t>
+  </si>
+  <si>
+    <t>1997.82, 0.05</t>
+  </si>
+  <si>
+    <t>2006.41, 0.00</t>
+  </si>
+  <si>
+    <t>2015.01, 0.11</t>
+  </si>
+  <si>
+    <t>burn</t>
   </si>
 </sst>
 </file>
@@ -613,10 +688,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A8627B-2386-4DAF-99DA-19F1EA4382AF}">
-  <dimension ref="A1:K209"/>
+  <dimension ref="A1:K233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G180" sqref="G180"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A202" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G229" sqref="G229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6755,7 +6831,7 @@
         <v>50</v>
       </c>
       <c r="D187">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E187" t="s">
         <v>9</v>
@@ -6860,7 +6936,7 @@
         <v>50</v>
       </c>
       <c r="D190">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E190" t="s">
         <v>9</v>
@@ -6965,7 +7041,7 @@
         <v>50</v>
       </c>
       <c r="D193">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E193" t="s">
         <v>9</v>
@@ -7070,7 +7146,7 @@
         <v>50</v>
       </c>
       <c r="D196">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E196" t="s">
         <v>9</v>
@@ -7175,7 +7251,7 @@
         <v>50</v>
       </c>
       <c r="D199">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E199" t="s">
         <v>9</v>
@@ -7280,7 +7356,7 @@
         <v>50</v>
       </c>
       <c r="D202">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E202" t="s">
         <v>9</v>
@@ -7385,7 +7461,7 @@
         <v>50</v>
       </c>
       <c r="D205">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E205" t="s">
         <v>9</v>
@@ -7490,7 +7566,7 @@
         <v>50</v>
       </c>
       <c r="D208">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E208" t="s">
         <v>9</v>
@@ -7546,6 +7622,846 @@
         <v>13</v>
       </c>
       <c r="K209" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A210" t="s">
+        <v>52</v>
+      </c>
+      <c r="B210" t="s">
+        <v>44</v>
+      </c>
+      <c r="C210" t="s">
+        <v>50</v>
+      </c>
+      <c r="D210">
+        <v>0</v>
+      </c>
+      <c r="E210" t="s">
+        <v>76</v>
+      </c>
+      <c r="F210" t="s">
+        <v>51</v>
+      </c>
+      <c r="G210" t="s">
+        <v>26</v>
+      </c>
+      <c r="H210" t="s">
+        <v>28</v>
+      </c>
+      <c r="I210" t="s">
+        <v>15</v>
+      </c>
+      <c r="J210" t="s">
+        <v>13</v>
+      </c>
+      <c r="K210" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A211" t="s">
+        <v>53</v>
+      </c>
+      <c r="B211" t="s">
+        <v>44</v>
+      </c>
+      <c r="C211" t="s">
+        <v>50</v>
+      </c>
+      <c r="D211">
+        <v>4</v>
+      </c>
+      <c r="E211" t="s">
+        <v>76</v>
+      </c>
+      <c r="F211" t="s">
+        <v>51</v>
+      </c>
+      <c r="G211" t="s">
+        <v>26</v>
+      </c>
+      <c r="H211" t="s">
+        <v>28</v>
+      </c>
+      <c r="I211" t="s">
+        <v>15</v>
+      </c>
+      <c r="J211" t="s">
+        <v>13</v>
+      </c>
+      <c r="K211" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A212" t="s">
+        <v>54</v>
+      </c>
+      <c r="B212" t="s">
+        <v>44</v>
+      </c>
+      <c r="C212" t="s">
+        <v>50</v>
+      </c>
+      <c r="D212">
+        <v>15</v>
+      </c>
+      <c r="E212" t="s">
+        <v>76</v>
+      </c>
+      <c r="F212" t="s">
+        <v>51</v>
+      </c>
+      <c r="G212" t="s">
+        <v>26</v>
+      </c>
+      <c r="H212" t="s">
+        <v>28</v>
+      </c>
+      <c r="I212" t="s">
+        <v>15</v>
+      </c>
+      <c r="J212" t="s">
+        <v>13</v>
+      </c>
+      <c r="K212" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="213" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
+        <v>55</v>
+      </c>
+      <c r="B213" t="s">
+        <v>32</v>
+      </c>
+      <c r="C213" t="s">
+        <v>50</v>
+      </c>
+      <c r="D213">
+        <v>0</v>
+      </c>
+      <c r="E213" t="s">
+        <v>76</v>
+      </c>
+      <c r="F213" t="s">
+        <v>51</v>
+      </c>
+      <c r="G213" t="s">
+        <v>26</v>
+      </c>
+      <c r="H213" t="s">
+        <v>28</v>
+      </c>
+      <c r="I213" t="s">
+        <v>15</v>
+      </c>
+      <c r="J213" t="s">
+        <v>13</v>
+      </c>
+      <c r="K213" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A214" t="s">
+        <v>56</v>
+      </c>
+      <c r="B214" t="s">
+        <v>32</v>
+      </c>
+      <c r="C214" t="s">
+        <v>50</v>
+      </c>
+      <c r="D214">
+        <v>4</v>
+      </c>
+      <c r="E214" t="s">
+        <v>76</v>
+      </c>
+      <c r="F214" t="s">
+        <v>51</v>
+      </c>
+      <c r="G214" t="s">
+        <v>26</v>
+      </c>
+      <c r="H214" t="s">
+        <v>28</v>
+      </c>
+      <c r="I214" t="s">
+        <v>15</v>
+      </c>
+      <c r="J214" t="s">
+        <v>13</v>
+      </c>
+      <c r="K214" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A215" t="s">
+        <v>57</v>
+      </c>
+      <c r="B215" t="s">
+        <v>32</v>
+      </c>
+      <c r="C215" t="s">
+        <v>50</v>
+      </c>
+      <c r="D215">
+        <v>15</v>
+      </c>
+      <c r="E215" t="s">
+        <v>76</v>
+      </c>
+      <c r="F215" t="s">
+        <v>51</v>
+      </c>
+      <c r="G215" t="s">
+        <v>26</v>
+      </c>
+      <c r="H215" t="s">
+        <v>28</v>
+      </c>
+      <c r="I215" t="s">
+        <v>15</v>
+      </c>
+      <c r="J215" t="s">
+        <v>13</v>
+      </c>
+      <c r="K215" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A216" t="s">
+        <v>58</v>
+      </c>
+      <c r="B216" t="s">
+        <v>46</v>
+      </c>
+      <c r="C216" t="s">
+        <v>50</v>
+      </c>
+      <c r="D216">
+        <v>0</v>
+      </c>
+      <c r="E216" t="s">
+        <v>76</v>
+      </c>
+      <c r="F216" t="s">
+        <v>51</v>
+      </c>
+      <c r="G216" t="s">
+        <v>26</v>
+      </c>
+      <c r="H216" t="s">
+        <v>28</v>
+      </c>
+      <c r="I216" t="s">
+        <v>15</v>
+      </c>
+      <c r="J216" t="s">
+        <v>13</v>
+      </c>
+      <c r="K216" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A217" t="s">
+        <v>59</v>
+      </c>
+      <c r="B217" t="s">
+        <v>46</v>
+      </c>
+      <c r="C217" t="s">
+        <v>50</v>
+      </c>
+      <c r="D217">
+        <v>4</v>
+      </c>
+      <c r="E217" t="s">
+        <v>76</v>
+      </c>
+      <c r="F217" t="s">
+        <v>51</v>
+      </c>
+      <c r="G217" t="s">
+        <v>26</v>
+      </c>
+      <c r="H217" t="s">
+        <v>28</v>
+      </c>
+      <c r="I217" t="s">
+        <v>15</v>
+      </c>
+      <c r="J217" t="s">
+        <v>13</v>
+      </c>
+      <c r="K217" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A218" t="s">
+        <v>60</v>
+      </c>
+      <c r="B218" t="s">
+        <v>46</v>
+      </c>
+      <c r="C218" t="s">
+        <v>50</v>
+      </c>
+      <c r="D218">
+        <v>15</v>
+      </c>
+      <c r="E218" t="s">
+        <v>76</v>
+      </c>
+      <c r="F218" t="s">
+        <v>51</v>
+      </c>
+      <c r="G218" t="s">
+        <v>26</v>
+      </c>
+      <c r="H218" t="s">
+        <v>28</v>
+      </c>
+      <c r="I218" t="s">
+        <v>15</v>
+      </c>
+      <c r="J218" t="s">
+        <v>13</v>
+      </c>
+      <c r="K218" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A219" t="s">
+        <v>61</v>
+      </c>
+      <c r="B219" t="s">
+        <v>5</v>
+      </c>
+      <c r="C219" t="s">
+        <v>50</v>
+      </c>
+      <c r="D219">
+        <v>0</v>
+      </c>
+      <c r="E219" t="s">
+        <v>76</v>
+      </c>
+      <c r="F219" t="s">
+        <v>51</v>
+      </c>
+      <c r="G219" t="s">
+        <v>26</v>
+      </c>
+      <c r="H219" t="s">
+        <v>28</v>
+      </c>
+      <c r="I219" t="s">
+        <v>15</v>
+      </c>
+      <c r="J219" t="s">
+        <v>13</v>
+      </c>
+      <c r="K219" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A220" t="s">
+        <v>62</v>
+      </c>
+      <c r="B220" t="s">
+        <v>5</v>
+      </c>
+      <c r="C220" t="s">
+        <v>50</v>
+      </c>
+      <c r="D220">
+        <v>4</v>
+      </c>
+      <c r="E220" t="s">
+        <v>76</v>
+      </c>
+      <c r="F220" t="s">
+        <v>51</v>
+      </c>
+      <c r="G220" t="s">
+        <v>26</v>
+      </c>
+      <c r="H220" t="s">
+        <v>28</v>
+      </c>
+      <c r="I220" t="s">
+        <v>15</v>
+      </c>
+      <c r="J220" t="s">
+        <v>13</v>
+      </c>
+      <c r="K220" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A221" t="s">
+        <v>63</v>
+      </c>
+      <c r="B221" t="s">
+        <v>5</v>
+      </c>
+      <c r="C221" t="s">
+        <v>50</v>
+      </c>
+      <c r="D221">
+        <v>15</v>
+      </c>
+      <c r="E221" t="s">
+        <v>76</v>
+      </c>
+      <c r="F221" t="s">
+        <v>51</v>
+      </c>
+      <c r="G221" t="s">
+        <v>26</v>
+      </c>
+      <c r="H221" t="s">
+        <v>28</v>
+      </c>
+      <c r="I221" t="s">
+        <v>15</v>
+      </c>
+      <c r="J221" t="s">
+        <v>13</v>
+      </c>
+      <c r="K221" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="222" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A222" t="s">
+        <v>64</v>
+      </c>
+      <c r="B222" t="s">
+        <v>45</v>
+      </c>
+      <c r="C222" t="s">
+        <v>50</v>
+      </c>
+      <c r="D222">
+        <v>0</v>
+      </c>
+      <c r="E222" t="s">
+        <v>76</v>
+      </c>
+      <c r="F222" t="s">
+        <v>51</v>
+      </c>
+      <c r="G222" t="s">
+        <v>26</v>
+      </c>
+      <c r="H222" t="s">
+        <v>28</v>
+      </c>
+      <c r="I222" t="s">
+        <v>15</v>
+      </c>
+      <c r="J222" t="s">
+        <v>13</v>
+      </c>
+      <c r="K222" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="223" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A223" t="s">
+        <v>65</v>
+      </c>
+      <c r="B223" t="s">
+        <v>45</v>
+      </c>
+      <c r="C223" t="s">
+        <v>50</v>
+      </c>
+      <c r="D223">
+        <v>4</v>
+      </c>
+      <c r="E223" t="s">
+        <v>76</v>
+      </c>
+      <c r="F223" t="s">
+        <v>51</v>
+      </c>
+      <c r="G223" t="s">
+        <v>26</v>
+      </c>
+      <c r="H223" t="s">
+        <v>28</v>
+      </c>
+      <c r="I223" t="s">
+        <v>15</v>
+      </c>
+      <c r="J223" t="s">
+        <v>13</v>
+      </c>
+      <c r="K223" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="224" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A224" t="s">
+        <v>66</v>
+      </c>
+      <c r="B224" t="s">
+        <v>45</v>
+      </c>
+      <c r="C224" t="s">
+        <v>50</v>
+      </c>
+      <c r="D224">
+        <v>15</v>
+      </c>
+      <c r="E224" t="s">
+        <v>76</v>
+      </c>
+      <c r="F224" t="s">
+        <v>51</v>
+      </c>
+      <c r="G224" t="s">
+        <v>26</v>
+      </c>
+      <c r="H224" t="s">
+        <v>28</v>
+      </c>
+      <c r="I224" t="s">
+        <v>15</v>
+      </c>
+      <c r="J224" t="s">
+        <v>13</v>
+      </c>
+      <c r="K224" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="225" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A225" t="s">
+        <v>67</v>
+      </c>
+      <c r="B225" t="s">
+        <v>47</v>
+      </c>
+      <c r="C225" t="s">
+        <v>50</v>
+      </c>
+      <c r="D225">
+        <v>0</v>
+      </c>
+      <c r="E225" t="s">
+        <v>76</v>
+      </c>
+      <c r="F225" t="s">
+        <v>51</v>
+      </c>
+      <c r="G225" t="s">
+        <v>26</v>
+      </c>
+      <c r="H225" t="s">
+        <v>28</v>
+      </c>
+      <c r="I225" t="s">
+        <v>15</v>
+      </c>
+      <c r="J225" t="s">
+        <v>13</v>
+      </c>
+      <c r="K225" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A226" t="s">
+        <v>68</v>
+      </c>
+      <c r="B226" t="s">
+        <v>47</v>
+      </c>
+      <c r="C226" t="s">
+        <v>50</v>
+      </c>
+      <c r="D226">
+        <v>4</v>
+      </c>
+      <c r="E226" t="s">
+        <v>76</v>
+      </c>
+      <c r="F226" t="s">
+        <v>51</v>
+      </c>
+      <c r="G226" t="s">
+        <v>26</v>
+      </c>
+      <c r="H226" t="s">
+        <v>28</v>
+      </c>
+      <c r="I226" t="s">
+        <v>15</v>
+      </c>
+      <c r="J226" t="s">
+        <v>13</v>
+      </c>
+      <c r="K226" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="227" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A227" t="s">
+        <v>69</v>
+      </c>
+      <c r="B227" t="s">
+        <v>47</v>
+      </c>
+      <c r="C227" t="s">
+        <v>50</v>
+      </c>
+      <c r="D227">
+        <v>15</v>
+      </c>
+      <c r="E227" t="s">
+        <v>76</v>
+      </c>
+      <c r="F227" t="s">
+        <v>51</v>
+      </c>
+      <c r="G227" t="s">
+        <v>26</v>
+      </c>
+      <c r="H227" t="s">
+        <v>28</v>
+      </c>
+      <c r="I227" t="s">
+        <v>15</v>
+      </c>
+      <c r="J227" t="s">
+        <v>13</v>
+      </c>
+      <c r="K227" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="228" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A228" t="s">
+        <v>70</v>
+      </c>
+      <c r="B228" t="s">
+        <v>48</v>
+      </c>
+      <c r="C228" t="s">
+        <v>50</v>
+      </c>
+      <c r="D228">
+        <v>0</v>
+      </c>
+      <c r="E228" t="s">
+        <v>76</v>
+      </c>
+      <c r="F228" t="s">
+        <v>51</v>
+      </c>
+      <c r="G228" t="s">
+        <v>26</v>
+      </c>
+      <c r="H228" t="s">
+        <v>28</v>
+      </c>
+      <c r="I228" t="s">
+        <v>15</v>
+      </c>
+      <c r="J228" t="s">
+        <v>13</v>
+      </c>
+      <c r="K228" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="229" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A229" t="s">
+        <v>71</v>
+      </c>
+      <c r="B229" t="s">
+        <v>48</v>
+      </c>
+      <c r="C229" t="s">
+        <v>50</v>
+      </c>
+      <c r="D229">
+        <v>4</v>
+      </c>
+      <c r="E229" t="s">
+        <v>76</v>
+      </c>
+      <c r="F229" t="s">
+        <v>51</v>
+      </c>
+      <c r="G229" t="s">
+        <v>26</v>
+      </c>
+      <c r="H229" t="s">
+        <v>28</v>
+      </c>
+      <c r="I229" t="s">
+        <v>15</v>
+      </c>
+      <c r="J229" t="s">
+        <v>13</v>
+      </c>
+      <c r="K229" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="230" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A230" t="s">
+        <v>72</v>
+      </c>
+      <c r="B230" t="s">
+        <v>48</v>
+      </c>
+      <c r="C230" t="s">
+        <v>50</v>
+      </c>
+      <c r="D230">
+        <v>15</v>
+      </c>
+      <c r="E230" t="s">
+        <v>76</v>
+      </c>
+      <c r="F230" t="s">
+        <v>51</v>
+      </c>
+      <c r="G230" t="s">
+        <v>26</v>
+      </c>
+      <c r="H230" t="s">
+        <v>28</v>
+      </c>
+      <c r="I230" t="s">
+        <v>15</v>
+      </c>
+      <c r="J230" t="s">
+        <v>13</v>
+      </c>
+      <c r="K230" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="231" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A231" t="s">
+        <v>73</v>
+      </c>
+      <c r="B231" t="s">
+        <v>49</v>
+      </c>
+      <c r="C231" t="s">
+        <v>50</v>
+      </c>
+      <c r="D231">
+        <v>0</v>
+      </c>
+      <c r="E231" t="s">
+        <v>76</v>
+      </c>
+      <c r="F231" t="s">
+        <v>51</v>
+      </c>
+      <c r="G231" t="s">
+        <v>26</v>
+      </c>
+      <c r="H231" t="s">
+        <v>28</v>
+      </c>
+      <c r="I231" t="s">
+        <v>15</v>
+      </c>
+      <c r="J231" t="s">
+        <v>13</v>
+      </c>
+      <c r="K231" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="232" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A232" t="s">
+        <v>74</v>
+      </c>
+      <c r="B232" t="s">
+        <v>49</v>
+      </c>
+      <c r="C232" t="s">
+        <v>50</v>
+      </c>
+      <c r="D232">
+        <v>4</v>
+      </c>
+      <c r="E232" t="s">
+        <v>76</v>
+      </c>
+      <c r="F232" t="s">
+        <v>51</v>
+      </c>
+      <c r="G232" t="s">
+        <v>26</v>
+      </c>
+      <c r="H232" t="s">
+        <v>28</v>
+      </c>
+      <c r="I232" t="s">
+        <v>15</v>
+      </c>
+      <c r="J232" t="s">
+        <v>13</v>
+      </c>
+      <c r="K232" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="233" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A233" t="s">
+        <v>75</v>
+      </c>
+      <c r="B233" t="s">
+        <v>49</v>
+      </c>
+      <c r="C233" t="s">
+        <v>50</v>
+      </c>
+      <c r="D233">
+        <v>15</v>
+      </c>
+      <c r="E233" t="s">
+        <v>76</v>
+      </c>
+      <c r="F233" t="s">
+        <v>51</v>
+      </c>
+      <c r="G233" t="s">
+        <v>26</v>
+      </c>
+      <c r="H233" t="s">
+        <v>28</v>
+      </c>
+      <c r="I233" t="s">
+        <v>15</v>
+      </c>
+      <c r="J233" t="s">
+        <v>13</v>
+      </c>
+      <c r="K233" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed control plots in Hood study not being identifiable to treatment type.  Honed the first graphs.
</commit_message>
<xml_diff>
--- a/data/web_plot_digitizer_data.xlsx
+++ b/data/web_plot_digitizer_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramR\fuels_longevity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED39F4D6-7E20-4291-B70A-41EAC31E017E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1563005-A670-40B0-ADF9-09B26031D733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{6245A06B-15CE-492B-AD18-D354A95DB25A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6245A06B-15CE-492B-AD18-D354A95DB25A}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -722,9 +722,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A8627B-2386-4DAF-99DA-19F1EA4382AF}">
   <dimension ref="A1:L917"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A883" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A918" sqref="A918"/>
+    <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A291" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I321" sqref="I321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -810,7 +810,7 @@
         <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K2" t="s">
         <v>12</v>
@@ -848,7 +848,7 @@
         <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
@@ -1266,7 +1266,7 @@
         <v>12</v>
       </c>
       <c r="J14" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K14" t="s">
         <v>12</v>
@@ -1304,7 +1304,7 @@
         <v>12</v>
       </c>
       <c r="J15" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K15" t="s">
         <v>12</v>
@@ -1722,7 +1722,7 @@
         <v>12</v>
       </c>
       <c r="J26" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K26" t="s">
         <v>12</v>
@@ -1760,7 +1760,7 @@
         <v>12</v>
       </c>
       <c r="J27" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K27" t="s">
         <v>12</v>
@@ -2178,7 +2178,7 @@
         <v>12</v>
       </c>
       <c r="J38" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K38" t="s">
         <v>12</v>
@@ -2216,7 +2216,7 @@
         <v>12</v>
       </c>
       <c r="J39" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K39" t="s">
         <v>12</v>
@@ -2634,7 +2634,7 @@
         <v>12</v>
       </c>
       <c r="J50" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K50" t="s">
         <v>12</v>
@@ -2672,7 +2672,7 @@
         <v>12</v>
       </c>
       <c r="J51" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K51" t="s">
         <v>12</v>
@@ -3090,7 +3090,7 @@
         <v>12</v>
       </c>
       <c r="J62" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K62" t="s">
         <v>12</v>
@@ -3128,7 +3128,7 @@
         <v>12</v>
       </c>
       <c r="J63" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K63" t="s">
         <v>12</v>
@@ -3546,7 +3546,7 @@
         <v>12</v>
       </c>
       <c r="J74" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K74" t="s">
         <v>12</v>
@@ -3584,7 +3584,7 @@
         <v>12</v>
       </c>
       <c r="J75" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K75" t="s">
         <v>12</v>
@@ -3622,7 +3622,7 @@
         <v>12</v>
       </c>
       <c r="J76" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K76" t="s">
         <v>12</v>
@@ -4002,7 +4002,7 @@
         <v>12</v>
       </c>
       <c r="J86" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K86" t="s">
         <v>12</v>
@@ -4040,7 +4040,7 @@
         <v>12</v>
       </c>
       <c r="J87" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K87" t="s">
         <v>12</v>
@@ -4078,7 +4078,7 @@
         <v>12</v>
       </c>
       <c r="J88" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K88" t="s">
         <v>12</v>
@@ -4458,7 +4458,7 @@
         <v>12</v>
       </c>
       <c r="J98" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K98" t="s">
         <v>12</v>
@@ -4496,7 +4496,7 @@
         <v>12</v>
       </c>
       <c r="J99" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K99" t="s">
         <v>12</v>
@@ -4534,7 +4534,7 @@
         <v>12</v>
       </c>
       <c r="J100" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K100" t="s">
         <v>12</v>
@@ -4914,7 +4914,7 @@
         <v>12</v>
       </c>
       <c r="J110" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K110" t="s">
         <v>12</v>
@@ -4952,7 +4952,7 @@
         <v>12</v>
       </c>
       <c r="J111" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K111" t="s">
         <v>12</v>
@@ -4990,7 +4990,7 @@
         <v>12</v>
       </c>
       <c r="J112" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K112" t="s">
         <v>12</v>
@@ -5370,7 +5370,7 @@
         <v>12</v>
       </c>
       <c r="J122" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K122" t="s">
         <v>12</v>
@@ -5408,7 +5408,7 @@
         <v>12</v>
       </c>
       <c r="J123" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K123" t="s">
         <v>12</v>
@@ -5446,7 +5446,7 @@
         <v>12</v>
       </c>
       <c r="J124" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K124" t="s">
         <v>12</v>
@@ -5826,7 +5826,7 @@
         <v>12</v>
       </c>
       <c r="J134" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K134" t="s">
         <v>12</v>
@@ -5864,7 +5864,7 @@
         <v>12</v>
       </c>
       <c r="J135" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K135" t="s">
         <v>12</v>
@@ -5902,7 +5902,7 @@
         <v>12</v>
       </c>
       <c r="J136" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K136" t="s">
         <v>12</v>
@@ -6282,7 +6282,7 @@
         <v>12</v>
       </c>
       <c r="J146" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K146" t="s">
         <v>12</v>
@@ -6320,7 +6320,7 @@
         <v>12</v>
       </c>
       <c r="J147" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K147" t="s">
         <v>12</v>
@@ -6358,7 +6358,7 @@
         <v>12</v>
       </c>
       <c r="J148" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K148" t="s">
         <v>12</v>
@@ -6738,7 +6738,7 @@
         <v>12</v>
       </c>
       <c r="J158" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K158" t="s">
         <v>12</v>
@@ -6776,7 +6776,7 @@
         <v>12</v>
       </c>
       <c r="J159" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K159" t="s">
         <v>12</v>
@@ -6814,7 +6814,7 @@
         <v>12</v>
       </c>
       <c r="J160" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K160" t="s">
         <v>12</v>
@@ -7194,7 +7194,7 @@
         <v>12</v>
       </c>
       <c r="J170" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K170" t="s">
         <v>12</v>
@@ -7232,7 +7232,7 @@
         <v>12</v>
       </c>
       <c r="J171" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="K171" t="s">
         <v>12</v>
@@ -7498,7 +7498,7 @@
         <v>12</v>
       </c>
       <c r="J178" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K178" t="s">
         <v>12</v>
@@ -7536,7 +7536,7 @@
         <v>12</v>
       </c>
       <c r="J179" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K179" t="s">
         <v>12</v>
@@ -7954,7 +7954,7 @@
         <v>12</v>
       </c>
       <c r="J190" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K190" t="s">
         <v>12</v>
@@ -7992,7 +7992,7 @@
         <v>12</v>
       </c>
       <c r="J191" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K191" t="s">
         <v>12</v>
@@ -8258,7 +8258,7 @@
         <v>12</v>
       </c>
       <c r="J198" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K198" t="s">
         <v>12</v>
@@ -8296,7 +8296,7 @@
         <v>12</v>
       </c>
       <c r="J199" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K199" t="s">
         <v>12</v>
@@ -8562,7 +8562,7 @@
         <v>12</v>
       </c>
       <c r="J206" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K206" t="s">
         <v>12</v>
@@ -8600,7 +8600,7 @@
         <v>12</v>
       </c>
       <c r="J207" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K207" t="s">
         <v>12</v>
@@ -8866,7 +8866,7 @@
         <v>12</v>
       </c>
       <c r="J214" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K214" t="s">
         <v>12</v>
@@ -8904,7 +8904,7 @@
         <v>12</v>
       </c>
       <c r="J215" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K215" t="s">
         <v>12</v>
@@ -9170,7 +9170,7 @@
         <v>12</v>
       </c>
       <c r="J222" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K222" t="s">
         <v>12</v>
@@ -9208,7 +9208,7 @@
         <v>12</v>
       </c>
       <c r="J223" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K223" t="s">
         <v>12</v>
@@ -9474,7 +9474,7 @@
         <v>12</v>
       </c>
       <c r="J230" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K230" t="s">
         <v>12</v>
@@ -9512,7 +9512,7 @@
         <v>12</v>
       </c>
       <c r="J231" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="K231" t="s">
         <v>12</v>
@@ -12382,7 +12382,7 @@
         <v>49</v>
       </c>
       <c r="D307">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E307" t="s">
         <v>10</v>
@@ -12420,7 +12420,7 @@
         <v>49</v>
       </c>
       <c r="D308">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E308" t="s">
         <v>10</v>
@@ -12458,7 +12458,7 @@
         <v>49</v>
       </c>
       <c r="D309">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E309" t="s">
         <v>10</v>
@@ -12496,7 +12496,7 @@
         <v>49</v>
       </c>
       <c r="D310">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E310" t="s">
         <v>10</v>
@@ -12534,7 +12534,7 @@
         <v>49</v>
       </c>
       <c r="D311">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E311" t="s">
         <v>10</v>
@@ -12572,7 +12572,7 @@
         <v>49</v>
       </c>
       <c r="D312">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E312" t="s">
         <v>10</v>
@@ -12610,7 +12610,7 @@
         <v>49</v>
       </c>
       <c r="D313">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E313" t="s">
         <v>10</v>
@@ -12648,7 +12648,7 @@
         <v>49</v>
       </c>
       <c r="D314">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E314" t="s">
         <v>10</v>
@@ -12686,7 +12686,7 @@
         <v>49</v>
       </c>
       <c r="D315">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E315" t="s">
         <v>10</v>
@@ -12838,7 +12838,7 @@
         <v>49</v>
       </c>
       <c r="D319">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E319" t="s">
         <v>10</v>
@@ -12876,7 +12876,7 @@
         <v>49</v>
       </c>
       <c r="D320">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E320" t="s">
         <v>10</v>
@@ -12914,7 +12914,7 @@
         <v>49</v>
       </c>
       <c r="D321">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E321" t="s">
         <v>10</v>
@@ -12952,7 +12952,7 @@
         <v>49</v>
       </c>
       <c r="D322">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E322" t="s">
         <v>10</v>
@@ -12990,7 +12990,7 @@
         <v>49</v>
       </c>
       <c r="D323">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E323" t="s">
         <v>10</v>
@@ -13028,7 +13028,7 @@
         <v>49</v>
       </c>
       <c r="D324">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E324" t="s">
         <v>10</v>
@@ -13066,7 +13066,7 @@
         <v>49</v>
       </c>
       <c r="D325">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E325" t="s">
         <v>10</v>
@@ -13104,7 +13104,7 @@
         <v>49</v>
       </c>
       <c r="D326">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="E326" t="s">
         <v>10</v>
@@ -13142,7 +13142,7 @@
         <v>49</v>
       </c>
       <c r="D327">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E327" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Added mission creek data
</commit_message>
<xml_diff>
--- a/data/web_plot_digitizer_data.xlsx
+++ b/data/web_plot_digitizer_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramR\fuels_longevity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0140D3-880B-4B0D-B635-33461DA99BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6205D8-7773-4925-BF5E-BE319C94A0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6245A06B-15CE-492B-AD18-D354A95DB25A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9178" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10178" uniqueCount="102">
   <si>
     <t>variable</t>
   </si>
@@ -333,6 +333,18 @@
   </si>
   <si>
     <t>shrub_cover</t>
+  </si>
+  <si>
+    <t>radcliffe_1</t>
+  </si>
+  <si>
+    <t>both</t>
+  </si>
+  <si>
+    <t>washington</t>
+  </si>
+  <si>
+    <t>wildfire</t>
   </si>
 </sst>
 </file>
@@ -717,11 +729,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A8627B-2386-4DAF-99DA-19F1EA4382AF}">
-  <dimension ref="A1:L917"/>
+  <dimension ref="A1:L1017"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A880" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J895" sqref="J895"/>
+      <pane ySplit="1" topLeftCell="A901" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H912" sqref="H912"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35583,6 +35595,3806 @@
         <v>12</v>
       </c>
       <c r="L917" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="918" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A918">
+        <v>23.907</v>
+      </c>
+      <c r="B918" t="s">
+        <v>35</v>
+      </c>
+      <c r="C918" t="s">
+        <v>36</v>
+      </c>
+      <c r="D918">
+        <v>0</v>
+      </c>
+      <c r="E918" t="s">
+        <v>8</v>
+      </c>
+      <c r="F918" t="s">
+        <v>98</v>
+      </c>
+      <c r="G918" t="s">
+        <v>99</v>
+      </c>
+      <c r="H918" t="s">
+        <v>100</v>
+      </c>
+      <c r="I918" t="s">
+        <v>13</v>
+      </c>
+      <c r="J918" t="s">
+        <v>52</v>
+      </c>
+      <c r="K918" t="s">
+        <v>12</v>
+      </c>
+      <c r="L918" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="919" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A919">
+        <v>30.423999999999999</v>
+      </c>
+      <c r="B919" t="s">
+        <v>35</v>
+      </c>
+      <c r="C919" t="s">
+        <v>36</v>
+      </c>
+      <c r="D919">
+        <v>19</v>
+      </c>
+      <c r="E919" t="s">
+        <v>8</v>
+      </c>
+      <c r="F919" t="s">
+        <v>98</v>
+      </c>
+      <c r="G919" t="s">
+        <v>99</v>
+      </c>
+      <c r="H919" t="s">
+        <v>100</v>
+      </c>
+      <c r="I919" t="s">
+        <v>13</v>
+      </c>
+      <c r="J919" t="s">
+        <v>52</v>
+      </c>
+      <c r="K919" t="s">
+        <v>12</v>
+      </c>
+      <c r="L919" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="920" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A920">
+        <v>529.16700000000003</v>
+      </c>
+      <c r="B920" t="s">
+        <v>33</v>
+      </c>
+      <c r="C920" t="s">
+        <v>34</v>
+      </c>
+      <c r="D920">
+        <v>0</v>
+      </c>
+      <c r="E920" t="s">
+        <v>8</v>
+      </c>
+      <c r="F920" t="s">
+        <v>98</v>
+      </c>
+      <c r="G920" t="s">
+        <v>99</v>
+      </c>
+      <c r="H920" t="s">
+        <v>100</v>
+      </c>
+      <c r="I920" t="s">
+        <v>13</v>
+      </c>
+      <c r="J920" t="s">
+        <v>52</v>
+      </c>
+      <c r="K920" t="s">
+        <v>12</v>
+      </c>
+      <c r="L920" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="921" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A921">
+        <v>327.596</v>
+      </c>
+      <c r="B921" t="s">
+        <v>33</v>
+      </c>
+      <c r="C921" t="s">
+        <v>34</v>
+      </c>
+      <c r="D921">
+        <v>19</v>
+      </c>
+      <c r="E921" t="s">
+        <v>8</v>
+      </c>
+      <c r="F921" t="s">
+        <v>98</v>
+      </c>
+      <c r="G921" t="s">
+        <v>99</v>
+      </c>
+      <c r="H921" t="s">
+        <v>100</v>
+      </c>
+      <c r="I921" t="s">
+        <v>13</v>
+      </c>
+      <c r="J921" t="s">
+        <v>52</v>
+      </c>
+      <c r="K921" t="s">
+        <v>12</v>
+      </c>
+      <c r="L921" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="922" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A922">
+        <v>27</v>
+      </c>
+      <c r="B922" t="s">
+        <v>37</v>
+      </c>
+      <c r="C922" t="s">
+        <v>38</v>
+      </c>
+      <c r="D922">
+        <v>0</v>
+      </c>
+      <c r="E922" t="s">
+        <v>8</v>
+      </c>
+      <c r="F922" t="s">
+        <v>98</v>
+      </c>
+      <c r="G922" t="s">
+        <v>99</v>
+      </c>
+      <c r="H922" t="s">
+        <v>100</v>
+      </c>
+      <c r="I922" t="s">
+        <v>13</v>
+      </c>
+      <c r="J922" t="s">
+        <v>52</v>
+      </c>
+      <c r="K922" t="s">
+        <v>12</v>
+      </c>
+      <c r="L922" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="923" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A923">
+        <v>39.311999999999998</v>
+      </c>
+      <c r="B923" t="s">
+        <v>37</v>
+      </c>
+      <c r="C923" t="s">
+        <v>38</v>
+      </c>
+      <c r="D923">
+        <v>19</v>
+      </c>
+      <c r="E923" t="s">
+        <v>8</v>
+      </c>
+      <c r="F923" t="s">
+        <v>98</v>
+      </c>
+      <c r="G923" t="s">
+        <v>99</v>
+      </c>
+      <c r="H923" t="s">
+        <v>100</v>
+      </c>
+      <c r="I923" t="s">
+        <v>13</v>
+      </c>
+      <c r="J923" t="s">
+        <v>52</v>
+      </c>
+      <c r="K923" t="s">
+        <v>12</v>
+      </c>
+      <c r="L923" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="924" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A924">
+        <v>1.371</v>
+      </c>
+      <c r="B924" t="s">
+        <v>74</v>
+      </c>
+      <c r="C924" t="s">
+        <v>49</v>
+      </c>
+      <c r="D924">
+        <v>0</v>
+      </c>
+      <c r="E924" t="s">
+        <v>8</v>
+      </c>
+      <c r="F924" t="s">
+        <v>98</v>
+      </c>
+      <c r="G924" t="s">
+        <v>99</v>
+      </c>
+      <c r="H924" t="s">
+        <v>100</v>
+      </c>
+      <c r="I924" t="s">
+        <v>13</v>
+      </c>
+      <c r="J924" t="s">
+        <v>52</v>
+      </c>
+      <c r="K924" t="s">
+        <v>12</v>
+      </c>
+      <c r="L924" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="925" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A925">
+        <v>1.1419999999999999</v>
+      </c>
+      <c r="B925" t="s">
+        <v>74</v>
+      </c>
+      <c r="C925" t="s">
+        <v>49</v>
+      </c>
+      <c r="D925">
+        <v>19</v>
+      </c>
+      <c r="E925" t="s">
+        <v>8</v>
+      </c>
+      <c r="F925" t="s">
+        <v>98</v>
+      </c>
+      <c r="G925" t="s">
+        <v>99</v>
+      </c>
+      <c r="H925" t="s">
+        <v>100</v>
+      </c>
+      <c r="I925" t="s">
+        <v>13</v>
+      </c>
+      <c r="J925" t="s">
+        <v>52</v>
+      </c>
+      <c r="K925" t="s">
+        <v>12</v>
+      </c>
+      <c r="L925" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="926" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A926">
+        <v>3.625</v>
+      </c>
+      <c r="B926" t="s">
+        <v>73</v>
+      </c>
+      <c r="C926" t="s">
+        <v>49</v>
+      </c>
+      <c r="D926">
+        <v>0</v>
+      </c>
+      <c r="E926" t="s">
+        <v>8</v>
+      </c>
+      <c r="F926" t="s">
+        <v>98</v>
+      </c>
+      <c r="G926" t="s">
+        <v>99</v>
+      </c>
+      <c r="H926" t="s">
+        <v>100</v>
+      </c>
+      <c r="I926" t="s">
+        <v>13</v>
+      </c>
+      <c r="J926" t="s">
+        <v>52</v>
+      </c>
+      <c r="K926" t="s">
+        <v>12</v>
+      </c>
+      <c r="L926" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="927" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A927">
+        <v>4.0830000000000002</v>
+      </c>
+      <c r="B927" t="s">
+        <v>73</v>
+      </c>
+      <c r="C927" t="s">
+        <v>49</v>
+      </c>
+      <c r="D927">
+        <v>19</v>
+      </c>
+      <c r="E927" t="s">
+        <v>8</v>
+      </c>
+      <c r="F927" t="s">
+        <v>98</v>
+      </c>
+      <c r="G927" t="s">
+        <v>99</v>
+      </c>
+      <c r="H927" t="s">
+        <v>100</v>
+      </c>
+      <c r="I927" t="s">
+        <v>13</v>
+      </c>
+      <c r="J927" t="s">
+        <v>52</v>
+      </c>
+      <c r="K927" t="s">
+        <v>12</v>
+      </c>
+      <c r="L927" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="928" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A928">
+        <v>0.52900000000000003</v>
+      </c>
+      <c r="B928" t="s">
+        <v>48</v>
+      </c>
+      <c r="C928" t="s">
+        <v>49</v>
+      </c>
+      <c r="D928">
+        <v>0</v>
+      </c>
+      <c r="E928" t="s">
+        <v>8</v>
+      </c>
+      <c r="F928" t="s">
+        <v>98</v>
+      </c>
+      <c r="G928" t="s">
+        <v>99</v>
+      </c>
+      <c r="H928" t="s">
+        <v>100</v>
+      </c>
+      <c r="I928" t="s">
+        <v>13</v>
+      </c>
+      <c r="J928" t="s">
+        <v>52</v>
+      </c>
+      <c r="K928" t="s">
+        <v>12</v>
+      </c>
+      <c r="L928" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="929" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A929">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="B929" t="s">
+        <v>48</v>
+      </c>
+      <c r="C929" t="s">
+        <v>49</v>
+      </c>
+      <c r="D929">
+        <v>19</v>
+      </c>
+      <c r="E929" t="s">
+        <v>8</v>
+      </c>
+      <c r="F929" t="s">
+        <v>98</v>
+      </c>
+      <c r="G929" t="s">
+        <v>99</v>
+      </c>
+      <c r="H929" t="s">
+        <v>100</v>
+      </c>
+      <c r="I929" t="s">
+        <v>13</v>
+      </c>
+      <c r="J929" t="s">
+        <v>52</v>
+      </c>
+      <c r="K929" t="s">
+        <v>12</v>
+      </c>
+      <c r="L929" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="930" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A930">
+        <v>1.95</v>
+      </c>
+      <c r="B930" t="s">
+        <v>47</v>
+      </c>
+      <c r="C930" t="s">
+        <v>49</v>
+      </c>
+      <c r="D930">
+        <v>0</v>
+      </c>
+      <c r="E930" t="s">
+        <v>8</v>
+      </c>
+      <c r="F930" t="s">
+        <v>98</v>
+      </c>
+      <c r="G930" t="s">
+        <v>99</v>
+      </c>
+      <c r="H930" t="s">
+        <v>100</v>
+      </c>
+      <c r="I930" t="s">
+        <v>13</v>
+      </c>
+      <c r="J930" t="s">
+        <v>52</v>
+      </c>
+      <c r="K930" t="s">
+        <v>12</v>
+      </c>
+      <c r="L930" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="931" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A931">
+        <v>4.875</v>
+      </c>
+      <c r="B931" t="s">
+        <v>47</v>
+      </c>
+      <c r="C931" t="s">
+        <v>49</v>
+      </c>
+      <c r="D931">
+        <v>19</v>
+      </c>
+      <c r="E931" t="s">
+        <v>8</v>
+      </c>
+      <c r="F931" t="s">
+        <v>98</v>
+      </c>
+      <c r="G931" t="s">
+        <v>99</v>
+      </c>
+      <c r="H931" t="s">
+        <v>100</v>
+      </c>
+      <c r="I931" t="s">
+        <v>13</v>
+      </c>
+      <c r="J931" t="s">
+        <v>52</v>
+      </c>
+      <c r="K931" t="s">
+        <v>12</v>
+      </c>
+      <c r="L931" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="932" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A932">
+        <v>2.1960000000000002</v>
+      </c>
+      <c r="B932" t="s">
+        <v>46</v>
+      </c>
+      <c r="C932" t="s">
+        <v>49</v>
+      </c>
+      <c r="D932">
+        <v>0</v>
+      </c>
+      <c r="E932" t="s">
+        <v>8</v>
+      </c>
+      <c r="F932" t="s">
+        <v>98</v>
+      </c>
+      <c r="G932" t="s">
+        <v>99</v>
+      </c>
+      <c r="H932" t="s">
+        <v>100</v>
+      </c>
+      <c r="I932" t="s">
+        <v>13</v>
+      </c>
+      <c r="J932" t="s">
+        <v>52</v>
+      </c>
+      <c r="K932" t="s">
+        <v>12</v>
+      </c>
+      <c r="L932" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="933" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A933">
+        <v>3.1890000000000001</v>
+      </c>
+      <c r="B933" t="s">
+        <v>46</v>
+      </c>
+      <c r="C933" t="s">
+        <v>49</v>
+      </c>
+      <c r="D933">
+        <v>19</v>
+      </c>
+      <c r="E933" t="s">
+        <v>8</v>
+      </c>
+      <c r="F933" t="s">
+        <v>98</v>
+      </c>
+      <c r="G933" t="s">
+        <v>99</v>
+      </c>
+      <c r="H933" t="s">
+        <v>100</v>
+      </c>
+      <c r="I933" t="s">
+        <v>13</v>
+      </c>
+      <c r="J933" t="s">
+        <v>52</v>
+      </c>
+      <c r="K933" t="s">
+        <v>12</v>
+      </c>
+      <c r="L933" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="934" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A934">
+        <v>26.262</v>
+      </c>
+      <c r="B934" t="s">
+        <v>82</v>
+      </c>
+      <c r="C934" t="s">
+        <v>49</v>
+      </c>
+      <c r="D934">
+        <v>0</v>
+      </c>
+      <c r="E934" t="s">
+        <v>8</v>
+      </c>
+      <c r="F934" t="s">
+        <v>98</v>
+      </c>
+      <c r="G934" t="s">
+        <v>99</v>
+      </c>
+      <c r="H934" t="s">
+        <v>100</v>
+      </c>
+      <c r="I934" t="s">
+        <v>13</v>
+      </c>
+      <c r="J934" t="s">
+        <v>52</v>
+      </c>
+      <c r="K934" t="s">
+        <v>12</v>
+      </c>
+      <c r="L934" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="935" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A935">
+        <v>61.503999999999998</v>
+      </c>
+      <c r="B935" t="s">
+        <v>82</v>
+      </c>
+      <c r="C935" t="s">
+        <v>49</v>
+      </c>
+      <c r="D935">
+        <v>19</v>
+      </c>
+      <c r="E935" t="s">
+        <v>8</v>
+      </c>
+      <c r="F935" t="s">
+        <v>98</v>
+      </c>
+      <c r="G935" t="s">
+        <v>99</v>
+      </c>
+      <c r="H935" t="s">
+        <v>100</v>
+      </c>
+      <c r="I935" t="s">
+        <v>13</v>
+      </c>
+      <c r="J935" t="s">
+        <v>52</v>
+      </c>
+      <c r="K935" t="s">
+        <v>12</v>
+      </c>
+      <c r="L935" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="936" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A936">
+        <v>16.516999999999999</v>
+      </c>
+      <c r="B936" t="s">
+        <v>83</v>
+      </c>
+      <c r="C936" t="s">
+        <v>49</v>
+      </c>
+      <c r="D936">
+        <v>0</v>
+      </c>
+      <c r="E936" t="s">
+        <v>8</v>
+      </c>
+      <c r="F936" t="s">
+        <v>98</v>
+      </c>
+      <c r="G936" t="s">
+        <v>99</v>
+      </c>
+      <c r="H936" t="s">
+        <v>100</v>
+      </c>
+      <c r="I936" t="s">
+        <v>13</v>
+      </c>
+      <c r="J936" t="s">
+        <v>52</v>
+      </c>
+      <c r="K936" t="s">
+        <v>12</v>
+      </c>
+      <c r="L936" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="937" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A937">
+        <v>6.2869999999999999</v>
+      </c>
+      <c r="B937" t="s">
+        <v>83</v>
+      </c>
+      <c r="C937" t="s">
+        <v>49</v>
+      </c>
+      <c r="D937">
+        <v>19</v>
+      </c>
+      <c r="E937" t="s">
+        <v>8</v>
+      </c>
+      <c r="F937" t="s">
+        <v>98</v>
+      </c>
+      <c r="G937" t="s">
+        <v>99</v>
+      </c>
+      <c r="H937" t="s">
+        <v>100</v>
+      </c>
+      <c r="I937" t="s">
+        <v>13</v>
+      </c>
+      <c r="J937" t="s">
+        <v>52</v>
+      </c>
+      <c r="K937" t="s">
+        <v>12</v>
+      </c>
+      <c r="L937" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="938" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A938">
+        <v>48.497999999999998</v>
+      </c>
+      <c r="B938" t="s">
+        <v>35</v>
+      </c>
+      <c r="C938" t="s">
+        <v>36</v>
+      </c>
+      <c r="D938">
+        <v>0</v>
+      </c>
+      <c r="E938" t="s">
+        <v>51</v>
+      </c>
+      <c r="F938" t="s">
+        <v>98</v>
+      </c>
+      <c r="G938" t="s">
+        <v>99</v>
+      </c>
+      <c r="H938" t="s">
+        <v>100</v>
+      </c>
+      <c r="I938" t="s">
+        <v>13</v>
+      </c>
+      <c r="J938" t="s">
+        <v>52</v>
+      </c>
+      <c r="K938" t="s">
+        <v>12</v>
+      </c>
+      <c r="L938" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="939" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A939">
+        <v>55.286000000000001</v>
+      </c>
+      <c r="B939" t="s">
+        <v>35</v>
+      </c>
+      <c r="C939" t="s">
+        <v>36</v>
+      </c>
+      <c r="D939">
+        <v>14</v>
+      </c>
+      <c r="E939" t="s">
+        <v>51</v>
+      </c>
+      <c r="F939" t="s">
+        <v>98</v>
+      </c>
+      <c r="G939" t="s">
+        <v>99</v>
+      </c>
+      <c r="H939" t="s">
+        <v>100</v>
+      </c>
+      <c r="I939" t="s">
+        <v>13</v>
+      </c>
+      <c r="J939" t="s">
+        <v>52</v>
+      </c>
+      <c r="K939" t="s">
+        <v>12</v>
+      </c>
+      <c r="L939" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="940" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A940">
+        <v>1597.2</v>
+      </c>
+      <c r="B940" t="s">
+        <v>33</v>
+      </c>
+      <c r="C940" t="s">
+        <v>34</v>
+      </c>
+      <c r="D940">
+        <v>0</v>
+      </c>
+      <c r="E940" t="s">
+        <v>51</v>
+      </c>
+      <c r="F940" t="s">
+        <v>98</v>
+      </c>
+      <c r="G940" t="s">
+        <v>99</v>
+      </c>
+      <c r="H940" t="s">
+        <v>100</v>
+      </c>
+      <c r="I940" t="s">
+        <v>13</v>
+      </c>
+      <c r="J940" t="s">
+        <v>52</v>
+      </c>
+      <c r="K940" t="s">
+        <v>12</v>
+      </c>
+      <c r="L940" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="941" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A941">
+        <v>705.41600000000005</v>
+      </c>
+      <c r="B941" t="s">
+        <v>33</v>
+      </c>
+      <c r="C941" t="s">
+        <v>34</v>
+      </c>
+      <c r="D941">
+        <v>14</v>
+      </c>
+      <c r="E941" t="s">
+        <v>51</v>
+      </c>
+      <c r="F941" t="s">
+        <v>98</v>
+      </c>
+      <c r="G941" t="s">
+        <v>99</v>
+      </c>
+      <c r="H941" t="s">
+        <v>100</v>
+      </c>
+      <c r="I941" t="s">
+        <v>13</v>
+      </c>
+      <c r="J941" t="s">
+        <v>52</v>
+      </c>
+      <c r="K941" t="s">
+        <v>12</v>
+      </c>
+      <c r="L941" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="942" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A942">
+        <v>45.92</v>
+      </c>
+      <c r="B942" t="s">
+        <v>37</v>
+      </c>
+      <c r="C942" t="s">
+        <v>38</v>
+      </c>
+      <c r="D942">
+        <v>0</v>
+      </c>
+      <c r="E942" t="s">
+        <v>51</v>
+      </c>
+      <c r="F942" t="s">
+        <v>98</v>
+      </c>
+      <c r="G942" t="s">
+        <v>99</v>
+      </c>
+      <c r="H942" t="s">
+        <v>100</v>
+      </c>
+      <c r="I942" t="s">
+        <v>13</v>
+      </c>
+      <c r="J942" t="s">
+        <v>52</v>
+      </c>
+      <c r="K942" t="s">
+        <v>12</v>
+      </c>
+      <c r="L942" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="943" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A943">
+        <v>70.683000000000007</v>
+      </c>
+      <c r="B943" t="s">
+        <v>37</v>
+      </c>
+      <c r="C943" t="s">
+        <v>38</v>
+      </c>
+      <c r="D943">
+        <v>14</v>
+      </c>
+      <c r="E943" t="s">
+        <v>51</v>
+      </c>
+      <c r="F943" t="s">
+        <v>98</v>
+      </c>
+      <c r="G943" t="s">
+        <v>99</v>
+      </c>
+      <c r="H943" t="s">
+        <v>100</v>
+      </c>
+      <c r="I943" t="s">
+        <v>13</v>
+      </c>
+      <c r="J943" t="s">
+        <v>52</v>
+      </c>
+      <c r="K943" t="s">
+        <v>12</v>
+      </c>
+      <c r="L943" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="944" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A944">
+        <v>4.4960000000000004</v>
+      </c>
+      <c r="B944" t="s">
+        <v>74</v>
+      </c>
+      <c r="C944" t="s">
+        <v>49</v>
+      </c>
+      <c r="D944">
+        <v>0</v>
+      </c>
+      <c r="E944" t="s">
+        <v>51</v>
+      </c>
+      <c r="F944" t="s">
+        <v>98</v>
+      </c>
+      <c r="G944" t="s">
+        <v>99</v>
+      </c>
+      <c r="H944" t="s">
+        <v>100</v>
+      </c>
+      <c r="I944" t="s">
+        <v>13</v>
+      </c>
+      <c r="J944" t="s">
+        <v>52</v>
+      </c>
+      <c r="K944" t="s">
+        <v>12</v>
+      </c>
+      <c r="L944" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="945" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A945">
+        <v>3.1240000000000001</v>
+      </c>
+      <c r="B945" t="s">
+        <v>74</v>
+      </c>
+      <c r="C945" t="s">
+        <v>49</v>
+      </c>
+      <c r="D945">
+        <v>14</v>
+      </c>
+      <c r="E945" t="s">
+        <v>51</v>
+      </c>
+      <c r="F945" t="s">
+        <v>98</v>
+      </c>
+      <c r="G945" t="s">
+        <v>99</v>
+      </c>
+      <c r="H945" t="s">
+        <v>100</v>
+      </c>
+      <c r="I945" t="s">
+        <v>13</v>
+      </c>
+      <c r="J945" t="s">
+        <v>52</v>
+      </c>
+      <c r="K945" t="s">
+        <v>12</v>
+      </c>
+      <c r="L945" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="946" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A946">
+        <v>7.3849999999999998</v>
+      </c>
+      <c r="B946" t="s">
+        <v>73</v>
+      </c>
+      <c r="C946" t="s">
+        <v>49</v>
+      </c>
+      <c r="D946">
+        <v>0</v>
+      </c>
+      <c r="E946" t="s">
+        <v>51</v>
+      </c>
+      <c r="F946" t="s">
+        <v>98</v>
+      </c>
+      <c r="G946" t="s">
+        <v>99</v>
+      </c>
+      <c r="H946" t="s">
+        <v>100</v>
+      </c>
+      <c r="I946" t="s">
+        <v>13</v>
+      </c>
+      <c r="J946" t="s">
+        <v>52</v>
+      </c>
+      <c r="K946" t="s">
+        <v>12</v>
+      </c>
+      <c r="L946" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="947" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A947">
+        <v>6.8760000000000003</v>
+      </c>
+      <c r="B947" t="s">
+        <v>73</v>
+      </c>
+      <c r="C947" t="s">
+        <v>49</v>
+      </c>
+      <c r="D947">
+        <v>14</v>
+      </c>
+      <c r="E947" t="s">
+        <v>51</v>
+      </c>
+      <c r="F947" t="s">
+        <v>98</v>
+      </c>
+      <c r="G947" t="s">
+        <v>99</v>
+      </c>
+      <c r="H947" t="s">
+        <v>100</v>
+      </c>
+      <c r="I947" t="s">
+        <v>13</v>
+      </c>
+      <c r="J947" t="s">
+        <v>52</v>
+      </c>
+      <c r="K947" t="s">
+        <v>12</v>
+      </c>
+      <c r="L947" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="948" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A948">
+        <v>1.22</v>
+      </c>
+      <c r="B948" t="s">
+        <v>48</v>
+      </c>
+      <c r="C948" t="s">
+        <v>49</v>
+      </c>
+      <c r="D948">
+        <v>0</v>
+      </c>
+      <c r="E948" t="s">
+        <v>51</v>
+      </c>
+      <c r="F948" t="s">
+        <v>98</v>
+      </c>
+      <c r="G948" t="s">
+        <v>99</v>
+      </c>
+      <c r="H948" t="s">
+        <v>100</v>
+      </c>
+      <c r="I948" t="s">
+        <v>13</v>
+      </c>
+      <c r="J948" t="s">
+        <v>52</v>
+      </c>
+      <c r="K948" t="s">
+        <v>12</v>
+      </c>
+      <c r="L948" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="949" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A949">
+        <v>2.3650000000000002</v>
+      </c>
+      <c r="B949" t="s">
+        <v>48</v>
+      </c>
+      <c r="C949" t="s">
+        <v>49</v>
+      </c>
+      <c r="D949">
+        <v>14</v>
+      </c>
+      <c r="E949" t="s">
+        <v>51</v>
+      </c>
+      <c r="F949" t="s">
+        <v>98</v>
+      </c>
+      <c r="G949" t="s">
+        <v>99</v>
+      </c>
+      <c r="H949" t="s">
+        <v>100</v>
+      </c>
+      <c r="I949" t="s">
+        <v>13</v>
+      </c>
+      <c r="J949" t="s">
+        <v>52</v>
+      </c>
+      <c r="K949" t="s">
+        <v>12</v>
+      </c>
+      <c r="L949" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="950" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A950">
+        <v>5.6609999999999996</v>
+      </c>
+      <c r="B950" t="s">
+        <v>47</v>
+      </c>
+      <c r="C950" t="s">
+        <v>49</v>
+      </c>
+      <c r="D950">
+        <v>0</v>
+      </c>
+      <c r="E950" t="s">
+        <v>51</v>
+      </c>
+      <c r="F950" t="s">
+        <v>98</v>
+      </c>
+      <c r="G950" t="s">
+        <v>99</v>
+      </c>
+      <c r="H950" t="s">
+        <v>100</v>
+      </c>
+      <c r="I950" t="s">
+        <v>13</v>
+      </c>
+      <c r="J950" t="s">
+        <v>52</v>
+      </c>
+      <c r="K950" t="s">
+        <v>12</v>
+      </c>
+      <c r="L950" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="951" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A951">
+        <v>13.491</v>
+      </c>
+      <c r="B951" t="s">
+        <v>47</v>
+      </c>
+      <c r="C951" t="s">
+        <v>49</v>
+      </c>
+      <c r="D951">
+        <v>14</v>
+      </c>
+      <c r="E951" t="s">
+        <v>51</v>
+      </c>
+      <c r="F951" t="s">
+        <v>98</v>
+      </c>
+      <c r="G951" t="s">
+        <v>99</v>
+      </c>
+      <c r="H951" t="s">
+        <v>100</v>
+      </c>
+      <c r="I951" t="s">
+        <v>13</v>
+      </c>
+      <c r="J951" t="s">
+        <v>52</v>
+      </c>
+      <c r="K951" t="s">
+        <v>12</v>
+      </c>
+      <c r="L951" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="952" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A952">
+        <v>9.9149999999999991</v>
+      </c>
+      <c r="B952" t="s">
+        <v>46</v>
+      </c>
+      <c r="C952" t="s">
+        <v>49</v>
+      </c>
+      <c r="D952">
+        <v>0</v>
+      </c>
+      <c r="E952" t="s">
+        <v>51</v>
+      </c>
+      <c r="F952" t="s">
+        <v>98</v>
+      </c>
+      <c r="G952" t="s">
+        <v>99</v>
+      </c>
+      <c r="H952" t="s">
+        <v>100</v>
+      </c>
+      <c r="I952" t="s">
+        <v>13</v>
+      </c>
+      <c r="J952" t="s">
+        <v>52</v>
+      </c>
+      <c r="K952" t="s">
+        <v>12</v>
+      </c>
+      <c r="L952" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="953" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A953">
+        <v>10.493</v>
+      </c>
+      <c r="B953" t="s">
+        <v>46</v>
+      </c>
+      <c r="C953" t="s">
+        <v>49</v>
+      </c>
+      <c r="D953">
+        <v>14</v>
+      </c>
+      <c r="E953" t="s">
+        <v>51</v>
+      </c>
+      <c r="F953" t="s">
+        <v>98</v>
+      </c>
+      <c r="G953" t="s">
+        <v>99</v>
+      </c>
+      <c r="H953" t="s">
+        <v>100</v>
+      </c>
+      <c r="I953" t="s">
+        <v>13</v>
+      </c>
+      <c r="J953" t="s">
+        <v>52</v>
+      </c>
+      <c r="K953" t="s">
+        <v>12</v>
+      </c>
+      <c r="L953" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="954" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A954">
+        <v>157.66800000000001</v>
+      </c>
+      <c r="B954" t="s">
+        <v>82</v>
+      </c>
+      <c r="C954" t="s">
+        <v>49</v>
+      </c>
+      <c r="D954">
+        <v>0</v>
+      </c>
+      <c r="E954" t="s">
+        <v>51</v>
+      </c>
+      <c r="F954" t="s">
+        <v>98</v>
+      </c>
+      <c r="G954" t="s">
+        <v>99</v>
+      </c>
+      <c r="H954" t="s">
+        <v>100</v>
+      </c>
+      <c r="I954" t="s">
+        <v>13</v>
+      </c>
+      <c r="J954" t="s">
+        <v>52</v>
+      </c>
+      <c r="K954" t="s">
+        <v>12</v>
+      </c>
+      <c r="L954" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="955" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A955">
+        <v>209.90600000000001</v>
+      </c>
+      <c r="B955" t="s">
+        <v>82</v>
+      </c>
+      <c r="C955" t="s">
+        <v>49</v>
+      </c>
+      <c r="D955">
+        <v>14</v>
+      </c>
+      <c r="E955" t="s">
+        <v>51</v>
+      </c>
+      <c r="F955" t="s">
+        <v>98</v>
+      </c>
+      <c r="G955" t="s">
+        <v>99</v>
+      </c>
+      <c r="H955" t="s">
+        <v>100</v>
+      </c>
+      <c r="I955" t="s">
+        <v>13</v>
+      </c>
+      <c r="J955" t="s">
+        <v>52</v>
+      </c>
+      <c r="K955" t="s">
+        <v>12</v>
+      </c>
+      <c r="L955" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="956" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A956">
+        <v>96.959000000000003</v>
+      </c>
+      <c r="B956" t="s">
+        <v>83</v>
+      </c>
+      <c r="C956" t="s">
+        <v>49</v>
+      </c>
+      <c r="D956">
+        <v>0</v>
+      </c>
+      <c r="E956" t="s">
+        <v>51</v>
+      </c>
+      <c r="F956" t="s">
+        <v>98</v>
+      </c>
+      <c r="G956" t="s">
+        <v>99</v>
+      </c>
+      <c r="H956" t="s">
+        <v>100</v>
+      </c>
+      <c r="I956" t="s">
+        <v>13</v>
+      </c>
+      <c r="J956" t="s">
+        <v>52</v>
+      </c>
+      <c r="K956" t="s">
+        <v>12</v>
+      </c>
+      <c r="L956" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="957" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A957">
+        <v>66.606999999999999</v>
+      </c>
+      <c r="B957" t="s">
+        <v>83</v>
+      </c>
+      <c r="C957" t="s">
+        <v>49</v>
+      </c>
+      <c r="D957">
+        <v>14</v>
+      </c>
+      <c r="E957" t="s">
+        <v>51</v>
+      </c>
+      <c r="F957" t="s">
+        <v>98</v>
+      </c>
+      <c r="G957" t="s">
+        <v>99</v>
+      </c>
+      <c r="H957" t="s">
+        <v>100</v>
+      </c>
+      <c r="I957" t="s">
+        <v>13</v>
+      </c>
+      <c r="J957" t="s">
+        <v>52</v>
+      </c>
+      <c r="K957" t="s">
+        <v>12</v>
+      </c>
+      <c r="L957" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="958" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A958">
+        <v>51.344000000000001</v>
+      </c>
+      <c r="B958" t="s">
+        <v>35</v>
+      </c>
+      <c r="C958" t="s">
+        <v>36</v>
+      </c>
+      <c r="D958">
+        <v>0</v>
+      </c>
+      <c r="E958" t="s">
+        <v>9</v>
+      </c>
+      <c r="F958" t="s">
+        <v>98</v>
+      </c>
+      <c r="G958" t="s">
+        <v>99</v>
+      </c>
+      <c r="H958" t="s">
+        <v>100</v>
+      </c>
+      <c r="I958" t="s">
+        <v>13</v>
+      </c>
+      <c r="J958" t="s">
+        <v>52</v>
+      </c>
+      <c r="K958" t="s">
+        <v>12</v>
+      </c>
+      <c r="L958" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="959" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A959">
+        <v>57.576999999999998</v>
+      </c>
+      <c r="B959" t="s">
+        <v>35</v>
+      </c>
+      <c r="C959" t="s">
+        <v>36</v>
+      </c>
+      <c r="D959">
+        <v>17</v>
+      </c>
+      <c r="E959" t="s">
+        <v>9</v>
+      </c>
+      <c r="F959" t="s">
+        <v>98</v>
+      </c>
+      <c r="G959" t="s">
+        <v>99</v>
+      </c>
+      <c r="H959" t="s">
+        <v>100</v>
+      </c>
+      <c r="I959" t="s">
+        <v>13</v>
+      </c>
+      <c r="J959" t="s">
+        <v>52</v>
+      </c>
+      <c r="K959" t="s">
+        <v>12</v>
+      </c>
+      <c r="L959" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="960" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A960">
+        <v>1133.19</v>
+      </c>
+      <c r="B960" t="s">
+        <v>33</v>
+      </c>
+      <c r="C960" t="s">
+        <v>34</v>
+      </c>
+      <c r="D960">
+        <v>0</v>
+      </c>
+      <c r="E960" t="s">
+        <v>9</v>
+      </c>
+      <c r="F960" t="s">
+        <v>98</v>
+      </c>
+      <c r="G960" t="s">
+        <v>99</v>
+      </c>
+      <c r="H960" t="s">
+        <v>100</v>
+      </c>
+      <c r="I960" t="s">
+        <v>13</v>
+      </c>
+      <c r="J960" t="s">
+        <v>52</v>
+      </c>
+      <c r="K960" t="s">
+        <v>12</v>
+      </c>
+      <c r="L960" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="961" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A961">
+        <v>1187.1679999999999</v>
+      </c>
+      <c r="B961" t="s">
+        <v>33</v>
+      </c>
+      <c r="C961" t="s">
+        <v>34</v>
+      </c>
+      <c r="D961">
+        <v>17</v>
+      </c>
+      <c r="E961" t="s">
+        <v>9</v>
+      </c>
+      <c r="F961" t="s">
+        <v>98</v>
+      </c>
+      <c r="G961" t="s">
+        <v>99</v>
+      </c>
+      <c r="H961" t="s">
+        <v>100</v>
+      </c>
+      <c r="I961" t="s">
+        <v>13</v>
+      </c>
+      <c r="J961" t="s">
+        <v>52</v>
+      </c>
+      <c r="K961" t="s">
+        <v>12</v>
+      </c>
+      <c r="L961" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="962" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A962">
+        <v>53.448999999999998</v>
+      </c>
+      <c r="B962" t="s">
+        <v>37</v>
+      </c>
+      <c r="C962" t="s">
+        <v>38</v>
+      </c>
+      <c r="D962">
+        <v>0</v>
+      </c>
+      <c r="E962" t="s">
+        <v>9</v>
+      </c>
+      <c r="F962" t="s">
+        <v>98</v>
+      </c>
+      <c r="G962" t="s">
+        <v>99</v>
+      </c>
+      <c r="H962" t="s">
+        <v>100</v>
+      </c>
+      <c r="I962" t="s">
+        <v>13</v>
+      </c>
+      <c r="J962" t="s">
+        <v>52</v>
+      </c>
+      <c r="K962" t="s">
+        <v>12</v>
+      </c>
+      <c r="L962" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="963" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A963">
+        <v>84.120999999999995</v>
+      </c>
+      <c r="B963" t="s">
+        <v>37</v>
+      </c>
+      <c r="C963" t="s">
+        <v>38</v>
+      </c>
+      <c r="D963">
+        <v>17</v>
+      </c>
+      <c r="E963" t="s">
+        <v>9</v>
+      </c>
+      <c r="F963" t="s">
+        <v>98</v>
+      </c>
+      <c r="G963" t="s">
+        <v>99</v>
+      </c>
+      <c r="H963" t="s">
+        <v>100</v>
+      </c>
+      <c r="I963" t="s">
+        <v>13</v>
+      </c>
+      <c r="J963" t="s">
+        <v>52</v>
+      </c>
+      <c r="K963" t="s">
+        <v>12</v>
+      </c>
+      <c r="L963" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="964" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A964">
+        <v>3.177</v>
+      </c>
+      <c r="B964" t="s">
+        <v>74</v>
+      </c>
+      <c r="C964" t="s">
+        <v>49</v>
+      </c>
+      <c r="D964">
+        <v>0</v>
+      </c>
+      <c r="E964" t="s">
+        <v>9</v>
+      </c>
+      <c r="F964" t="s">
+        <v>98</v>
+      </c>
+      <c r="G964" t="s">
+        <v>99</v>
+      </c>
+      <c r="H964" t="s">
+        <v>100</v>
+      </c>
+      <c r="I964" t="s">
+        <v>13</v>
+      </c>
+      <c r="J964" t="s">
+        <v>52</v>
+      </c>
+      <c r="K964" t="s">
+        <v>12</v>
+      </c>
+      <c r="L964" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="965" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A965">
+        <v>4.7830000000000004</v>
+      </c>
+      <c r="B965" t="s">
+        <v>74</v>
+      </c>
+      <c r="C965" t="s">
+        <v>49</v>
+      </c>
+      <c r="D965">
+        <v>17</v>
+      </c>
+      <c r="E965" t="s">
+        <v>9</v>
+      </c>
+      <c r="F965" t="s">
+        <v>98</v>
+      </c>
+      <c r="G965" t="s">
+        <v>99</v>
+      </c>
+      <c r="H965" t="s">
+        <v>100</v>
+      </c>
+      <c r="I965" t="s">
+        <v>13</v>
+      </c>
+      <c r="J965" t="s">
+        <v>52</v>
+      </c>
+      <c r="K965" t="s">
+        <v>12</v>
+      </c>
+      <c r="L965" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="966" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A966">
+        <v>7.125</v>
+      </c>
+      <c r="B966" t="s">
+        <v>73</v>
+      </c>
+      <c r="C966" t="s">
+        <v>49</v>
+      </c>
+      <c r="D966">
+        <v>0</v>
+      </c>
+      <c r="E966" t="s">
+        <v>9</v>
+      </c>
+      <c r="F966" t="s">
+        <v>98</v>
+      </c>
+      <c r="G966" t="s">
+        <v>99</v>
+      </c>
+      <c r="H966" t="s">
+        <v>100</v>
+      </c>
+      <c r="I966" t="s">
+        <v>13</v>
+      </c>
+      <c r="J966" t="s">
+        <v>52</v>
+      </c>
+      <c r="K966" t="s">
+        <v>12</v>
+      </c>
+      <c r="L966" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="967" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A967">
+        <v>7.391</v>
+      </c>
+      <c r="B967" t="s">
+        <v>73</v>
+      </c>
+      <c r="C967" t="s">
+        <v>49</v>
+      </c>
+      <c r="D967">
+        <v>17</v>
+      </c>
+      <c r="E967" t="s">
+        <v>9</v>
+      </c>
+      <c r="F967" t="s">
+        <v>98</v>
+      </c>
+      <c r="G967" t="s">
+        <v>99</v>
+      </c>
+      <c r="H967" t="s">
+        <v>100</v>
+      </c>
+      <c r="I967" t="s">
+        <v>13</v>
+      </c>
+      <c r="J967" t="s">
+        <v>52</v>
+      </c>
+      <c r="K967" t="s">
+        <v>12</v>
+      </c>
+      <c r="L967" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="968" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A968">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="B968" t="s">
+        <v>48</v>
+      </c>
+      <c r="C968" t="s">
+        <v>49</v>
+      </c>
+      <c r="D968">
+        <v>0</v>
+      </c>
+      <c r="E968" t="s">
+        <v>9</v>
+      </c>
+      <c r="F968" t="s">
+        <v>98</v>
+      </c>
+      <c r="G968" t="s">
+        <v>99</v>
+      </c>
+      <c r="H968" t="s">
+        <v>100</v>
+      </c>
+      <c r="I968" t="s">
+        <v>13</v>
+      </c>
+      <c r="J968" t="s">
+        <v>52</v>
+      </c>
+      <c r="K968" t="s">
+        <v>12</v>
+      </c>
+      <c r="L968" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="969" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A969">
+        <v>1.9279999999999999</v>
+      </c>
+      <c r="B969" t="s">
+        <v>48</v>
+      </c>
+      <c r="C969" t="s">
+        <v>49</v>
+      </c>
+      <c r="D969">
+        <v>17</v>
+      </c>
+      <c r="E969" t="s">
+        <v>9</v>
+      </c>
+      <c r="F969" t="s">
+        <v>98</v>
+      </c>
+      <c r="G969" t="s">
+        <v>99</v>
+      </c>
+      <c r="H969" t="s">
+        <v>100</v>
+      </c>
+      <c r="I969" t="s">
+        <v>13</v>
+      </c>
+      <c r="J969" t="s">
+        <v>52</v>
+      </c>
+      <c r="K969" t="s">
+        <v>12</v>
+      </c>
+      <c r="L969" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="970" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A970">
+        <v>3.4569999999999999</v>
+      </c>
+      <c r="B970" t="s">
+        <v>47</v>
+      </c>
+      <c r="C970" t="s">
+        <v>49</v>
+      </c>
+      <c r="D970">
+        <v>0</v>
+      </c>
+      <c r="E970" t="s">
+        <v>9</v>
+      </c>
+      <c r="F970" t="s">
+        <v>98</v>
+      </c>
+      <c r="G970" t="s">
+        <v>99</v>
+      </c>
+      <c r="H970" t="s">
+        <v>100</v>
+      </c>
+      <c r="I970" t="s">
+        <v>13</v>
+      </c>
+      <c r="J970" t="s">
+        <v>52</v>
+      </c>
+      <c r="K970" t="s">
+        <v>12</v>
+      </c>
+      <c r="L970" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="971" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A971">
+        <v>16.765999999999998</v>
+      </c>
+      <c r="B971" t="s">
+        <v>47</v>
+      </c>
+      <c r="C971" t="s">
+        <v>49</v>
+      </c>
+      <c r="D971">
+        <v>17</v>
+      </c>
+      <c r="E971" t="s">
+        <v>9</v>
+      </c>
+      <c r="F971" t="s">
+        <v>98</v>
+      </c>
+      <c r="G971" t="s">
+        <v>99</v>
+      </c>
+      <c r="H971" t="s">
+        <v>100</v>
+      </c>
+      <c r="I971" t="s">
+        <v>13</v>
+      </c>
+      <c r="J971" t="s">
+        <v>52</v>
+      </c>
+      <c r="K971" t="s">
+        <v>12</v>
+      </c>
+      <c r="L971" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="972" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A972">
+        <v>10.992000000000001</v>
+      </c>
+      <c r="B972" t="s">
+        <v>46</v>
+      </c>
+      <c r="C972" t="s">
+        <v>49</v>
+      </c>
+      <c r="D972">
+        <v>0</v>
+      </c>
+      <c r="E972" t="s">
+        <v>9</v>
+      </c>
+      <c r="F972" t="s">
+        <v>98</v>
+      </c>
+      <c r="G972" t="s">
+        <v>99</v>
+      </c>
+      <c r="H972" t="s">
+        <v>100</v>
+      </c>
+      <c r="I972" t="s">
+        <v>13</v>
+      </c>
+      <c r="J972" t="s">
+        <v>52</v>
+      </c>
+      <c r="K972" t="s">
+        <v>12</v>
+      </c>
+      <c r="L972" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="973" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A973">
+        <v>20.425000000000001</v>
+      </c>
+      <c r="B973" t="s">
+        <v>46</v>
+      </c>
+      <c r="C973" t="s">
+        <v>49</v>
+      </c>
+      <c r="D973">
+        <v>17</v>
+      </c>
+      <c r="E973" t="s">
+        <v>9</v>
+      </c>
+      <c r="F973" t="s">
+        <v>98</v>
+      </c>
+      <c r="G973" t="s">
+        <v>99</v>
+      </c>
+      <c r="H973" t="s">
+        <v>100</v>
+      </c>
+      <c r="I973" t="s">
+        <v>13</v>
+      </c>
+      <c r="J973" t="s">
+        <v>52</v>
+      </c>
+      <c r="K973" t="s">
+        <v>12</v>
+      </c>
+      <c r="L973" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="974" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A974">
+        <v>174.19399999999999</v>
+      </c>
+      <c r="B974" t="s">
+        <v>82</v>
+      </c>
+      <c r="C974" t="s">
+        <v>49</v>
+      </c>
+      <c r="D974">
+        <v>0</v>
+      </c>
+      <c r="E974" t="s">
+        <v>9</v>
+      </c>
+      <c r="F974" t="s">
+        <v>98</v>
+      </c>
+      <c r="G974" t="s">
+        <v>99</v>
+      </c>
+      <c r="H974" t="s">
+        <v>100</v>
+      </c>
+      <c r="I974" t="s">
+        <v>13</v>
+      </c>
+      <c r="J974" t="s">
+        <v>52</v>
+      </c>
+      <c r="K974" t="s">
+        <v>12</v>
+      </c>
+      <c r="L974" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="975" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A975">
+        <v>243.86</v>
+      </c>
+      <c r="B975" t="s">
+        <v>82</v>
+      </c>
+      <c r="C975" t="s">
+        <v>49</v>
+      </c>
+      <c r="D975">
+        <v>17</v>
+      </c>
+      <c r="E975" t="s">
+        <v>9</v>
+      </c>
+      <c r="F975" t="s">
+        <v>98</v>
+      </c>
+      <c r="G975" t="s">
+        <v>99</v>
+      </c>
+      <c r="H975" t="s">
+        <v>100</v>
+      </c>
+      <c r="I975" t="s">
+        <v>13</v>
+      </c>
+      <c r="J975" t="s">
+        <v>52</v>
+      </c>
+      <c r="K975" t="s">
+        <v>12</v>
+      </c>
+      <c r="L975" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="976" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A976">
+        <v>199.05500000000001</v>
+      </c>
+      <c r="B976" t="s">
+        <v>83</v>
+      </c>
+      <c r="C976" t="s">
+        <v>49</v>
+      </c>
+      <c r="D976">
+        <v>0</v>
+      </c>
+      <c r="E976" t="s">
+        <v>9</v>
+      </c>
+      <c r="F976" t="s">
+        <v>98</v>
+      </c>
+      <c r="G976" t="s">
+        <v>99</v>
+      </c>
+      <c r="H976" t="s">
+        <v>100</v>
+      </c>
+      <c r="I976" t="s">
+        <v>13</v>
+      </c>
+      <c r="J976" t="s">
+        <v>52</v>
+      </c>
+      <c r="K976" t="s">
+        <v>12</v>
+      </c>
+      <c r="L976" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="977" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A977">
+        <v>142.54900000000001</v>
+      </c>
+      <c r="B977" t="s">
+        <v>83</v>
+      </c>
+      <c r="C977" t="s">
+        <v>49</v>
+      </c>
+      <c r="D977">
+        <v>17</v>
+      </c>
+      <c r="E977" t="s">
+        <v>9</v>
+      </c>
+      <c r="F977" t="s">
+        <v>98</v>
+      </c>
+      <c r="G977" t="s">
+        <v>99</v>
+      </c>
+      <c r="H977" t="s">
+        <v>100</v>
+      </c>
+      <c r="I977" t="s">
+        <v>13</v>
+      </c>
+      <c r="J977" t="s">
+        <v>52</v>
+      </c>
+      <c r="K977" t="s">
+        <v>12</v>
+      </c>
+      <c r="L977" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="978" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A978">
+        <v>76.171000000000006</v>
+      </c>
+      <c r="B978" t="s">
+        <v>35</v>
+      </c>
+      <c r="C978" t="s">
+        <v>36</v>
+      </c>
+      <c r="D978">
+        <v>0</v>
+      </c>
+      <c r="E978" t="s">
+        <v>10</v>
+      </c>
+      <c r="F978" t="s">
+        <v>98</v>
+      </c>
+      <c r="G978" t="s">
+        <v>99</v>
+      </c>
+      <c r="H978" t="s">
+        <v>100</v>
+      </c>
+      <c r="I978" t="s">
+        <v>13</v>
+      </c>
+      <c r="J978" t="s">
+        <v>52</v>
+      </c>
+      <c r="K978" t="s">
+        <v>12</v>
+      </c>
+      <c r="L978" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="979" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A979">
+        <v>45.847999999999999</v>
+      </c>
+      <c r="B979" t="s">
+        <v>35</v>
+      </c>
+      <c r="C979" t="s">
+        <v>36</v>
+      </c>
+      <c r="D979">
+        <v>14</v>
+      </c>
+      <c r="E979" t="s">
+        <v>10</v>
+      </c>
+      <c r="F979" t="s">
+        <v>98</v>
+      </c>
+      <c r="G979" t="s">
+        <v>99</v>
+      </c>
+      <c r="H979" t="s">
+        <v>100</v>
+      </c>
+      <c r="I979" t="s">
+        <v>13</v>
+      </c>
+      <c r="J979" t="s">
+        <v>52</v>
+      </c>
+      <c r="K979" t="s">
+        <v>12</v>
+      </c>
+      <c r="L979" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="980" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A980">
+        <v>2091.8560000000002</v>
+      </c>
+      <c r="B980" t="s">
+        <v>33</v>
+      </c>
+      <c r="C980" t="s">
+        <v>34</v>
+      </c>
+      <c r="D980">
+        <v>0</v>
+      </c>
+      <c r="E980" t="s">
+        <v>10</v>
+      </c>
+      <c r="F980" t="s">
+        <v>98</v>
+      </c>
+      <c r="G980" t="s">
+        <v>99</v>
+      </c>
+      <c r="H980" t="s">
+        <v>100</v>
+      </c>
+      <c r="I980" t="s">
+        <v>13</v>
+      </c>
+      <c r="J980" t="s">
+        <v>52</v>
+      </c>
+      <c r="K980" t="s">
+        <v>12</v>
+      </c>
+      <c r="L980" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="981" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A981">
+        <v>729.74400000000003</v>
+      </c>
+      <c r="B981" t="s">
+        <v>33</v>
+      </c>
+      <c r="C981" t="s">
+        <v>34</v>
+      </c>
+      <c r="D981">
+        <v>14</v>
+      </c>
+      <c r="E981" t="s">
+        <v>10</v>
+      </c>
+      <c r="F981" t="s">
+        <v>98</v>
+      </c>
+      <c r="G981" t="s">
+        <v>99</v>
+      </c>
+      <c r="H981" t="s">
+        <v>100</v>
+      </c>
+      <c r="I981" t="s">
+        <v>13</v>
+      </c>
+      <c r="J981" t="s">
+        <v>52</v>
+      </c>
+      <c r="K981" t="s">
+        <v>12</v>
+      </c>
+      <c r="L981" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="982" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A982">
+        <v>77.56</v>
+      </c>
+      <c r="B982" t="s">
+        <v>37</v>
+      </c>
+      <c r="C982" t="s">
+        <v>38</v>
+      </c>
+      <c r="D982">
+        <v>0</v>
+      </c>
+      <c r="E982" t="s">
+        <v>10</v>
+      </c>
+      <c r="F982" t="s">
+        <v>98</v>
+      </c>
+      <c r="G982" t="s">
+        <v>99</v>
+      </c>
+      <c r="H982" t="s">
+        <v>100</v>
+      </c>
+      <c r="I982" t="s">
+        <v>13</v>
+      </c>
+      <c r="J982" t="s">
+        <v>52</v>
+      </c>
+      <c r="K982" t="s">
+        <v>12</v>
+      </c>
+      <c r="L982" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="983" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A983">
+        <v>117.86199999999999</v>
+      </c>
+      <c r="B983" t="s">
+        <v>37</v>
+      </c>
+      <c r="C983" t="s">
+        <v>38</v>
+      </c>
+      <c r="D983">
+        <v>14</v>
+      </c>
+      <c r="E983" t="s">
+        <v>10</v>
+      </c>
+      <c r="F983" t="s">
+        <v>98</v>
+      </c>
+      <c r="G983" t="s">
+        <v>99</v>
+      </c>
+      <c r="H983" t="s">
+        <v>100</v>
+      </c>
+      <c r="I983" t="s">
+        <v>13</v>
+      </c>
+      <c r="J983" t="s">
+        <v>52</v>
+      </c>
+      <c r="K983" t="s">
+        <v>12</v>
+      </c>
+      <c r="L983" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="984" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A984">
+        <v>3.044</v>
+      </c>
+      <c r="B984" t="s">
+        <v>74</v>
+      </c>
+      <c r="C984" t="s">
+        <v>49</v>
+      </c>
+      <c r="D984">
+        <v>0</v>
+      </c>
+      <c r="E984" t="s">
+        <v>10</v>
+      </c>
+      <c r="F984" t="s">
+        <v>98</v>
+      </c>
+      <c r="G984" t="s">
+        <v>99</v>
+      </c>
+      <c r="H984" t="s">
+        <v>100</v>
+      </c>
+      <c r="I984" t="s">
+        <v>13</v>
+      </c>
+      <c r="J984" t="s">
+        <v>52</v>
+      </c>
+      <c r="K984" t="s">
+        <v>12</v>
+      </c>
+      <c r="L984" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="985" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A985">
+        <v>3.4489999999999998</v>
+      </c>
+      <c r="B985" t="s">
+        <v>74</v>
+      </c>
+      <c r="C985" t="s">
+        <v>49</v>
+      </c>
+      <c r="D985">
+        <v>14</v>
+      </c>
+      <c r="E985" t="s">
+        <v>10</v>
+      </c>
+      <c r="F985" t="s">
+        <v>98</v>
+      </c>
+      <c r="G985" t="s">
+        <v>99</v>
+      </c>
+      <c r="H985" t="s">
+        <v>100</v>
+      </c>
+      <c r="I985" t="s">
+        <v>13</v>
+      </c>
+      <c r="J985" t="s">
+        <v>52</v>
+      </c>
+      <c r="K985" t="s">
+        <v>12</v>
+      </c>
+      <c r="L985" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="986" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A986">
+        <v>9.5909999999999993</v>
+      </c>
+      <c r="B986" t="s">
+        <v>73</v>
+      </c>
+      <c r="C986" t="s">
+        <v>49</v>
+      </c>
+      <c r="D986">
+        <v>0</v>
+      </c>
+      <c r="E986" t="s">
+        <v>10</v>
+      </c>
+      <c r="F986" t="s">
+        <v>98</v>
+      </c>
+      <c r="G986" t="s">
+        <v>99</v>
+      </c>
+      <c r="H986" t="s">
+        <v>100</v>
+      </c>
+      <c r="I986" t="s">
+        <v>13</v>
+      </c>
+      <c r="J986" t="s">
+        <v>52</v>
+      </c>
+      <c r="K986" t="s">
+        <v>12</v>
+      </c>
+      <c r="L986" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="987" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A987">
+        <v>9.0210000000000008</v>
+      </c>
+      <c r="B987" t="s">
+        <v>73</v>
+      </c>
+      <c r="C987" t="s">
+        <v>49</v>
+      </c>
+      <c r="D987">
+        <v>14</v>
+      </c>
+      <c r="E987" t="s">
+        <v>10</v>
+      </c>
+      <c r="F987" t="s">
+        <v>98</v>
+      </c>
+      <c r="G987" t="s">
+        <v>99</v>
+      </c>
+      <c r="H987" t="s">
+        <v>100</v>
+      </c>
+      <c r="I987" t="s">
+        <v>13</v>
+      </c>
+      <c r="J987" t="s">
+        <v>52</v>
+      </c>
+      <c r="K987" t="s">
+        <v>12</v>
+      </c>
+      <c r="L987" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="988" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A988">
+        <v>3.06</v>
+      </c>
+      <c r="B988" t="s">
+        <v>48</v>
+      </c>
+      <c r="C988" t="s">
+        <v>49</v>
+      </c>
+      <c r="D988">
+        <v>0</v>
+      </c>
+      <c r="E988" t="s">
+        <v>10</v>
+      </c>
+      <c r="F988" t="s">
+        <v>98</v>
+      </c>
+      <c r="G988" t="s">
+        <v>99</v>
+      </c>
+      <c r="H988" t="s">
+        <v>100</v>
+      </c>
+      <c r="I988" t="s">
+        <v>13</v>
+      </c>
+      <c r="J988" t="s">
+        <v>52</v>
+      </c>
+      <c r="K988" t="s">
+        <v>12</v>
+      </c>
+      <c r="L988" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="989" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A989">
+        <v>2.6970000000000001</v>
+      </c>
+      <c r="B989" t="s">
+        <v>48</v>
+      </c>
+      <c r="C989" t="s">
+        <v>49</v>
+      </c>
+      <c r="D989">
+        <v>14</v>
+      </c>
+      <c r="E989" t="s">
+        <v>10</v>
+      </c>
+      <c r="F989" t="s">
+        <v>98</v>
+      </c>
+      <c r="G989" t="s">
+        <v>99</v>
+      </c>
+      <c r="H989" t="s">
+        <v>100</v>
+      </c>
+      <c r="I989" t="s">
+        <v>13</v>
+      </c>
+      <c r="J989" t="s">
+        <v>52</v>
+      </c>
+      <c r="K989" t="s">
+        <v>12</v>
+      </c>
+      <c r="L989" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="990" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A990">
+        <v>7.4749999999999996</v>
+      </c>
+      <c r="B990" t="s">
+        <v>47</v>
+      </c>
+      <c r="C990" t="s">
+        <v>49</v>
+      </c>
+      <c r="D990">
+        <v>0</v>
+      </c>
+      <c r="E990" t="s">
+        <v>10</v>
+      </c>
+      <c r="F990" t="s">
+        <v>98</v>
+      </c>
+      <c r="G990" t="s">
+        <v>99</v>
+      </c>
+      <c r="H990" t="s">
+        <v>100</v>
+      </c>
+      <c r="I990" t="s">
+        <v>13</v>
+      </c>
+      <c r="J990" t="s">
+        <v>52</v>
+      </c>
+      <c r="K990" t="s">
+        <v>12</v>
+      </c>
+      <c r="L990" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="991" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A991">
+        <v>15.43</v>
+      </c>
+      <c r="B991" t="s">
+        <v>47</v>
+      </c>
+      <c r="C991" t="s">
+        <v>49</v>
+      </c>
+      <c r="D991">
+        <v>14</v>
+      </c>
+      <c r="E991" t="s">
+        <v>10</v>
+      </c>
+      <c r="F991" t="s">
+        <v>98</v>
+      </c>
+      <c r="G991" t="s">
+        <v>99</v>
+      </c>
+      <c r="H991" t="s">
+        <v>100</v>
+      </c>
+      <c r="I991" t="s">
+        <v>13</v>
+      </c>
+      <c r="J991" t="s">
+        <v>52</v>
+      </c>
+      <c r="K991" t="s">
+        <v>12</v>
+      </c>
+      <c r="L991" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="992" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A992">
+        <v>12.051</v>
+      </c>
+      <c r="B992" t="s">
+        <v>46</v>
+      </c>
+      <c r="C992" t="s">
+        <v>49</v>
+      </c>
+      <c r="D992">
+        <v>0</v>
+      </c>
+      <c r="E992" t="s">
+        <v>10</v>
+      </c>
+      <c r="F992" t="s">
+        <v>98</v>
+      </c>
+      <c r="G992" t="s">
+        <v>99</v>
+      </c>
+      <c r="H992" t="s">
+        <v>100</v>
+      </c>
+      <c r="I992" t="s">
+        <v>13</v>
+      </c>
+      <c r="J992" t="s">
+        <v>52</v>
+      </c>
+      <c r="K992" t="s">
+        <v>12</v>
+      </c>
+      <c r="L992" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="993" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A993">
+        <v>15.233000000000001</v>
+      </c>
+      <c r="B993" t="s">
+        <v>46</v>
+      </c>
+      <c r="C993" t="s">
+        <v>49</v>
+      </c>
+      <c r="D993">
+        <v>14</v>
+      </c>
+      <c r="E993" t="s">
+        <v>10</v>
+      </c>
+      <c r="F993" t="s">
+        <v>98</v>
+      </c>
+      <c r="G993" t="s">
+        <v>99</v>
+      </c>
+      <c r="H993" t="s">
+        <v>100</v>
+      </c>
+      <c r="I993" t="s">
+        <v>13</v>
+      </c>
+      <c r="J993" t="s">
+        <v>52</v>
+      </c>
+      <c r="K993" t="s">
+        <v>12</v>
+      </c>
+      <c r="L993" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="994" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A994">
+        <v>233.542</v>
+      </c>
+      <c r="B994" t="s">
+        <v>82</v>
+      </c>
+      <c r="C994" t="s">
+        <v>49</v>
+      </c>
+      <c r="D994">
+        <v>0</v>
+      </c>
+      <c r="E994" t="s">
+        <v>10</v>
+      </c>
+      <c r="F994" t="s">
+        <v>98</v>
+      </c>
+      <c r="G994" t="s">
+        <v>99</v>
+      </c>
+      <c r="H994" t="s">
+        <v>100</v>
+      </c>
+      <c r="I994" t="s">
+        <v>13</v>
+      </c>
+      <c r="J994" t="s">
+        <v>52</v>
+      </c>
+      <c r="K994" t="s">
+        <v>12</v>
+      </c>
+      <c r="L994" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="995" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A995">
+        <v>360.63600000000002</v>
+      </c>
+      <c r="B995" t="s">
+        <v>82</v>
+      </c>
+      <c r="C995" t="s">
+        <v>49</v>
+      </c>
+      <c r="D995">
+        <v>14</v>
+      </c>
+      <c r="E995" t="s">
+        <v>10</v>
+      </c>
+      <c r="F995" t="s">
+        <v>98</v>
+      </c>
+      <c r="G995" t="s">
+        <v>99</v>
+      </c>
+      <c r="H995" t="s">
+        <v>100</v>
+      </c>
+      <c r="I995" t="s">
+        <v>13</v>
+      </c>
+      <c r="J995" t="s">
+        <v>52</v>
+      </c>
+      <c r="K995" t="s">
+        <v>12</v>
+      </c>
+      <c r="L995" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="996" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A996">
+        <v>157.43299999999999</v>
+      </c>
+      <c r="B996" t="s">
+        <v>83</v>
+      </c>
+      <c r="C996" t="s">
+        <v>49</v>
+      </c>
+      <c r="D996">
+        <v>0</v>
+      </c>
+      <c r="E996" t="s">
+        <v>10</v>
+      </c>
+      <c r="F996" t="s">
+        <v>98</v>
+      </c>
+      <c r="G996" t="s">
+        <v>99</v>
+      </c>
+      <c r="H996" t="s">
+        <v>100</v>
+      </c>
+      <c r="I996" t="s">
+        <v>13</v>
+      </c>
+      <c r="J996" t="s">
+        <v>52</v>
+      </c>
+      <c r="K996" t="s">
+        <v>12</v>
+      </c>
+      <c r="L996" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="997" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A997">
+        <v>164.60499999999999</v>
+      </c>
+      <c r="B997" t="s">
+        <v>83</v>
+      </c>
+      <c r="C997" t="s">
+        <v>49</v>
+      </c>
+      <c r="D997">
+        <v>14</v>
+      </c>
+      <c r="E997" t="s">
+        <v>10</v>
+      </c>
+      <c r="F997" t="s">
+        <v>98</v>
+      </c>
+      <c r="G997" t="s">
+        <v>99</v>
+      </c>
+      <c r="H997" t="s">
+        <v>100</v>
+      </c>
+      <c r="I997" t="s">
+        <v>13</v>
+      </c>
+      <c r="J997" t="s">
+        <v>52</v>
+      </c>
+      <c r="K997" t="s">
+        <v>12</v>
+      </c>
+      <c r="L997" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="998" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A998">
+        <v>67.903000000000006</v>
+      </c>
+      <c r="B998" t="s">
+        <v>35</v>
+      </c>
+      <c r="C998" t="s">
+        <v>36</v>
+      </c>
+      <c r="D998">
+        <v>0</v>
+      </c>
+      <c r="E998" t="s">
+        <v>101</v>
+      </c>
+      <c r="F998" t="s">
+        <v>98</v>
+      </c>
+      <c r="G998" t="s">
+        <v>99</v>
+      </c>
+      <c r="H998" t="s">
+        <v>100</v>
+      </c>
+      <c r="I998" t="s">
+        <v>13</v>
+      </c>
+      <c r="J998" t="s">
+        <v>52</v>
+      </c>
+      <c r="K998" t="s">
+        <v>12</v>
+      </c>
+      <c r="L998" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="999" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A999">
+        <v>51.484000000000002</v>
+      </c>
+      <c r="B999" t="s">
+        <v>35</v>
+      </c>
+      <c r="C999" t="s">
+        <v>36</v>
+      </c>
+      <c r="D999">
+        <v>8</v>
+      </c>
+      <c r="E999" t="s">
+        <v>101</v>
+      </c>
+      <c r="F999" t="s">
+        <v>98</v>
+      </c>
+      <c r="G999" t="s">
+        <v>99</v>
+      </c>
+      <c r="H999" t="s">
+        <v>100</v>
+      </c>
+      <c r="I999" t="s">
+        <v>13</v>
+      </c>
+      <c r="J999" t="s">
+        <v>52</v>
+      </c>
+      <c r="K999" t="s">
+        <v>12</v>
+      </c>
+      <c r="L999" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1000">
+        <v>1169.607</v>
+      </c>
+      <c r="B1000" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1000">
+        <v>0</v>
+      </c>
+      <c r="E1000" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1000" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1000" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1000" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1000" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1000" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1000" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1000" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1001">
+        <v>509.23500000000001</v>
+      </c>
+      <c r="B1001" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1001">
+        <v>8</v>
+      </c>
+      <c r="E1001" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1001" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1001" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1001" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1001" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1001" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1001" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1001" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1002">
+        <v>64.641999999999996</v>
+      </c>
+      <c r="B1002" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1002">
+        <v>0</v>
+      </c>
+      <c r="E1002" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1002" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1002" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1002" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1002" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1002" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1002" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1002" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1003">
+        <v>83.888000000000005</v>
+      </c>
+      <c r="B1003" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1003">
+        <v>8</v>
+      </c>
+      <c r="E1003" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1003" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1003" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1003" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1003" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1003" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1003" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1003" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1004">
+        <v>1.8919999999999999</v>
+      </c>
+      <c r="B1004" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1004">
+        <v>0</v>
+      </c>
+      <c r="E1004" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1004" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1004" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1004" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1004" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1004" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1004" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1004" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1005">
+        <v>2.032</v>
+      </c>
+      <c r="B1005" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1005">
+        <v>8</v>
+      </c>
+      <c r="E1005" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1005" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1005" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1005" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1005" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1005" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1005" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1005" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1006">
+        <v>6.867</v>
+      </c>
+      <c r="B1006" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1006">
+        <v>0</v>
+      </c>
+      <c r="E1006" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1006" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1006" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1006" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1006" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1006" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1006" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1006" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1007">
+        <v>5.577</v>
+      </c>
+      <c r="B1007" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1007">
+        <v>8</v>
+      </c>
+      <c r="E1007" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1007" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1007" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1007" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1007" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1007" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1007" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1007" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1008">
+        <v>2.6680000000000001</v>
+      </c>
+      <c r="B1008" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1008">
+        <v>0</v>
+      </c>
+      <c r="E1008" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1008" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1008" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1008" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1008" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1008" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1008" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1008" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1009">
+        <v>6.0579999999999998</v>
+      </c>
+      <c r="B1009" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1009">
+        <v>8</v>
+      </c>
+      <c r="E1009" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1009" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1009" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1009" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1009" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1009" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1009" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1009" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1010">
+        <v>4.7850000000000001</v>
+      </c>
+      <c r="B1010" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1010">
+        <v>0</v>
+      </c>
+      <c r="E1010" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1010" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1010" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1010" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1010" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1010" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1010" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1010" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1011">
+        <v>10.542</v>
+      </c>
+      <c r="B1011" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1011">
+        <v>8</v>
+      </c>
+      <c r="E1011" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1011" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1011" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1011" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1011" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1011" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1011" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1011" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1012">
+        <v>5.1029999999999998</v>
+      </c>
+      <c r="B1012" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1012">
+        <v>0</v>
+      </c>
+      <c r="E1012" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1012" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1012" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1012" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1012" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1012" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1012" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1012" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1013">
+        <v>5.7229999999999999</v>
+      </c>
+      <c r="B1013" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1013">
+        <v>8</v>
+      </c>
+      <c r="E1013" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1013" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1013" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1013" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1013" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1013" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1013" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1013" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1014">
+        <v>73.822000000000003</v>
+      </c>
+      <c r="B1014" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1014">
+        <v>0</v>
+      </c>
+      <c r="E1014" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1014" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1014" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1014" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1014" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1014" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1014" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1014" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1015">
+        <v>214.227</v>
+      </c>
+      <c r="B1015" t="s">
+        <v>82</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1015">
+        <v>8</v>
+      </c>
+      <c r="E1015" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1015" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1015" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1015" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1015" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1015" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1015" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1015" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1016">
+        <v>32.137999999999998</v>
+      </c>
+      <c r="B1016" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1016" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1016">
+        <v>0</v>
+      </c>
+      <c r="E1016" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1016" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1016" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1016" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1016" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1016" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1016" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1016" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1017">
+        <v>6.29</v>
+      </c>
+      <c r="B1017" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1017">
+        <v>8</v>
+      </c>
+      <c r="E1017" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1017" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1017" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1017" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1017" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1017" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1017" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1017" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Colville surface fuels to the web plot digitizer data
</commit_message>
<xml_diff>
--- a/data/web_plot_digitizer_data.xlsx
+++ b/data/web_plot_digitizer_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramR\fuels_longevity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AC1C600-CAFA-4BA4-92DE-B5311647A136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8695DA-325A-4C67-B383-D8757E69891A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6245A06B-15CE-492B-AD18-D354A95DB25A}"/>
+    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{6245A06B-15CE-492B-AD18-D354A95DB25A}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10178" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10558" uniqueCount="105">
   <si>
     <t>variable</t>
   </si>
@@ -345,6 +345,15 @@
   </si>
   <si>
     <t>wildfire</t>
+  </si>
+  <si>
+    <t>radcliffe2</t>
+  </si>
+  <si>
+    <t>herb</t>
+  </si>
+  <si>
+    <t>shrub</t>
   </si>
 </sst>
 </file>
@@ -729,11 +738,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A8627B-2386-4DAF-99DA-19F1EA4382AF}">
-  <dimension ref="A1:L1017"/>
+  <dimension ref="A1:L1055"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A992" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1006" sqref="H1006"/>
+      <pane ySplit="1" topLeftCell="A996" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1008" sqref="E1008"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39395,6 +39404,1450 @@
         <v>12</v>
       </c>
       <c r="L1017" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1018">
+        <v>6.6079999999999997</v>
+      </c>
+      <c r="B1018" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1018">
+        <v>1</v>
+      </c>
+      <c r="E1018" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1018" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1018" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1018" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1018" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1018" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1018" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1018" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1019">
+        <v>1.2849999999999999</v>
+      </c>
+      <c r="B1019" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1019">
+        <v>1</v>
+      </c>
+      <c r="E1019" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1019" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1019" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1019" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1019" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1019" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1019" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1019" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1020">
+        <v>0.113</v>
+      </c>
+      <c r="B1020" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1020" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1020">
+        <v>1</v>
+      </c>
+      <c r="E1020" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1020" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1020" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1020" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1020" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1020" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1020" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1020" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1021">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="B1021" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1021" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1021">
+        <v>1</v>
+      </c>
+      <c r="E1021" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1021" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1021" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1021" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1021" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1021" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1021" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1021" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1022">
+        <v>3.4209999999999998</v>
+      </c>
+      <c r="B1022" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1022" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1022">
+        <v>1</v>
+      </c>
+      <c r="E1022" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1022" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1022" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1022" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1022" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1022" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1022" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1022" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1023">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="B1023" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1023" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1023">
+        <v>1</v>
+      </c>
+      <c r="E1023" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1023" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1023" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1023" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1023" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1023" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1023" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1023" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1024">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="B1024" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1024" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1024">
+        <v>1</v>
+      </c>
+      <c r="E1024" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1024" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1024" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1024" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1024" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1024" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1024" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1024" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1025" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1025">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="B1025" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1025" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1025">
+        <v>1</v>
+      </c>
+      <c r="E1025" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1025" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1025" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1025" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1025" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1025" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1025" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1025" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1026">
+        <v>11.029</v>
+      </c>
+      <c r="B1026" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1026" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1026">
+        <v>5</v>
+      </c>
+      <c r="E1026" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1026" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1026" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1026" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1026" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1026" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1026" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1026" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1027">
+        <v>1.7749999999999999</v>
+      </c>
+      <c r="B1027" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1027" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1027">
+        <v>5</v>
+      </c>
+      <c r="E1027" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1027" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1027" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1027" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1027" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1027" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1027" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1027" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1028">
+        <v>0.54</v>
+      </c>
+      <c r="B1028" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1028" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1028">
+        <v>5</v>
+      </c>
+      <c r="E1028" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1028" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1028" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1028" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1028" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1028" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1028" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1028" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1029">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="B1029" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1029" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1029">
+        <v>5</v>
+      </c>
+      <c r="E1029" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1029" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1029" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1029" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1029" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1029" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1029" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1029" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1030">
+        <v>4.2670000000000003</v>
+      </c>
+      <c r="B1030" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1030">
+        <v>5</v>
+      </c>
+      <c r="E1030" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1030" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1030" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1030" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1030" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1030" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1030" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1030" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1031">
+        <v>0.376</v>
+      </c>
+      <c r="B1031" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1031" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1031">
+        <v>5</v>
+      </c>
+      <c r="E1031" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1031" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1031" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1031" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1031" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1031" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1031" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1031" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1032">
+        <v>0.20200000000000001</v>
+      </c>
+      <c r="B1032" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1032" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1032">
+        <v>5</v>
+      </c>
+      <c r="E1032" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1032" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1032" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1032" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1032" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1032" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1032" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1032" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1033">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="B1033" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1033" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1033">
+        <v>5</v>
+      </c>
+      <c r="E1033" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1033" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1033" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1033" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1033" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1033" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1033" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1033" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1034">
+        <v>7.673</v>
+      </c>
+      <c r="B1034" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1034" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1034">
+        <v>10</v>
+      </c>
+      <c r="E1034" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1034" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1034" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1034" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1034" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1034" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1034" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1034" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1035">
+        <v>2.0179999999999998</v>
+      </c>
+      <c r="B1035" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1035" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1035">
+        <v>10</v>
+      </c>
+      <c r="E1035" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1035" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1035" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1035" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1035" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1035" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1035" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1035" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1036">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="B1036" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1036" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1036">
+        <v>10</v>
+      </c>
+      <c r="E1036" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1036" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1036" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1036" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1036" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1036" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1036" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1036" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1037">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="B1037" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1037" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1037">
+        <v>10</v>
+      </c>
+      <c r="E1037" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1037" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1037" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1037" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1037" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1037" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1037" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1037" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1038">
+        <v>4.3659999999999997</v>
+      </c>
+      <c r="B1038" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1038" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1038">
+        <v>10</v>
+      </c>
+      <c r="E1038" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1038" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1038" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1038" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1038" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1038" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1038" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1038" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1039">
+        <v>0.504</v>
+      </c>
+      <c r="B1039" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1039" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1039">
+        <v>10</v>
+      </c>
+      <c r="E1039" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1039" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1039" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1039" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1039" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1039" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1039" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1039" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1040">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="B1040" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1040" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1040">
+        <v>10</v>
+      </c>
+      <c r="E1040" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1040" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1040" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1040" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1040" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1040" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1040" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1040" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1041" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1041">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="B1041" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1041" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1041">
+        <v>10</v>
+      </c>
+      <c r="E1041" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1041" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1041" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1041" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1041" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1041" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1041" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1041" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1042" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1042">
+        <v>1.57</v>
+      </c>
+      <c r="B1042" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1042" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1042">
+        <v>15</v>
+      </c>
+      <c r="E1042" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1042" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1042" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1042" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1042" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1042" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1042" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1042" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1043">
+        <v>0.66900000000000004</v>
+      </c>
+      <c r="B1043" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1043" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1043">
+        <v>15</v>
+      </c>
+      <c r="E1043" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1043" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1043" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1043" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1043" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1043" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1043" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1043" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1044">
+        <v>0.8</v>
+      </c>
+      <c r="B1044" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1044" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1044">
+        <v>15</v>
+      </c>
+      <c r="E1044" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1044" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1044" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1044" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1044" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1044" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1044" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1044" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1045">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="B1045" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1045" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1045">
+        <v>15</v>
+      </c>
+      <c r="E1045" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1045" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1045" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1045" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1045" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1045" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1045" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1045" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1046">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="B1046" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1046" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1046">
+        <v>15</v>
+      </c>
+      <c r="E1046" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1046" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1046" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1046" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1046" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1046" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1046" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1046" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1047">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="B1047" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1047" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1047">
+        <v>15</v>
+      </c>
+      <c r="E1047" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1047" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1047" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1047" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1047" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1047" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1047" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1047" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1048">
+        <v>7.5330000000000004</v>
+      </c>
+      <c r="B1048" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1048" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1048">
+        <v>20</v>
+      </c>
+      <c r="E1048" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1048" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1048" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1048" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1048" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1048" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1048" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1048" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1049">
+        <v>2.6139999999999999</v>
+      </c>
+      <c r="B1049" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1049" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1049">
+        <v>20</v>
+      </c>
+      <c r="E1049" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1049" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1049" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1049" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1049" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1049" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1049" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1049" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1050">
+        <v>0.44700000000000001</v>
+      </c>
+      <c r="B1050" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1050" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1050">
+        <v>20</v>
+      </c>
+      <c r="E1050" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1050" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1050" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1050" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1050" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1050" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1050" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1050" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1051">
+        <v>1.431</v>
+      </c>
+      <c r="B1051" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1051" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1051">
+        <v>20</v>
+      </c>
+      <c r="E1051" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1051" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1051" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1051" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1051" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1051" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1051" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1051" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1052">
+        <v>3.5750000000000002</v>
+      </c>
+      <c r="B1052" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1052" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1052">
+        <v>20</v>
+      </c>
+      <c r="E1052" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1052" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1052" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1052" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1052" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1052" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1052" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1052" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1053">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="B1053" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1053" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1053">
+        <v>20</v>
+      </c>
+      <c r="E1053" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1053" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1053" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1053" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1053" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1053" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1053" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1053" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1054">
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="B1054" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1054" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1054">
+        <v>20</v>
+      </c>
+      <c r="E1054" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1054" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1054" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1054" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1054" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1054" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1054" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1054" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1055">
+        <v>0.626</v>
+      </c>
+      <c r="B1055" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1055" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1055">
+        <v>20</v>
+      </c>
+      <c r="E1055" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1055" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1055" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1055" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1055" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1055" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1055" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1055" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Saved colville stand structure data to webplotdigitizerdata
</commit_message>
<xml_diff>
--- a/data/web_plot_digitizer_data.xlsx
+++ b/data/web_plot_digitizer_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramR\fuels_longevity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8695DA-325A-4C67-B383-D8757E69891A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D6CB464-A4C5-4EF7-AB39-048B4942D272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{6245A06B-15CE-492B-AD18-D354A95DB25A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6245A06B-15CE-492B-AD18-D354A95DB25A}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10558" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10708" uniqueCount="105">
   <si>
     <t>variable</t>
   </si>
@@ -738,11 +738,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A8627B-2386-4DAF-99DA-19F1EA4382AF}">
-  <dimension ref="A1:L1055"/>
+  <dimension ref="A1:L1070"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A996" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1008" sqref="E1008"/>
+      <pane ySplit="1" topLeftCell="A1042" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1050" sqref="H1050"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -40848,6 +40848,576 @@
         <v>12</v>
       </c>
       <c r="L1055" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1056">
+        <v>45.753999999999998</v>
+      </c>
+      <c r="B1056" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1056" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1056">
+        <v>1</v>
+      </c>
+      <c r="E1056" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1056" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1056" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1056" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1056" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1056" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1056" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1056" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1057">
+        <v>26.837</v>
+      </c>
+      <c r="B1057" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1057" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1057">
+        <v>5</v>
+      </c>
+      <c r="E1057" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1057" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1057" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1057" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1057" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1057" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1057" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1057" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1058">
+        <v>35.634999999999998</v>
+      </c>
+      <c r="B1058" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1058" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1058">
+        <v>10</v>
+      </c>
+      <c r="E1058" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1058" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1058" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1058" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1058" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1058" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1058" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1058" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1059">
+        <v>36.520000000000003</v>
+      </c>
+      <c r="B1059" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1059" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1059">
+        <v>15</v>
+      </c>
+      <c r="E1059" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1059" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1059" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1059" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1059" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1059" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1059" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1059" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1060">
+        <v>27.59</v>
+      </c>
+      <c r="B1060" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1060" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1060">
+        <v>20</v>
+      </c>
+      <c r="E1060" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1060" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1060" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1060" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1060" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1060" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1060" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1060" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1061">
+        <v>20.210999999999999</v>
+      </c>
+      <c r="B1061" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1061" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1061">
+        <v>1</v>
+      </c>
+      <c r="E1061" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1061" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1061" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1061" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1061" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1061" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1061" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1061" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1062">
+        <v>15.531000000000001</v>
+      </c>
+      <c r="B1062" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1062" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1062">
+        <v>5</v>
+      </c>
+      <c r="E1062" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1062" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1062" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1062" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1062" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1062" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1062" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1062" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1063">
+        <v>17.89</v>
+      </c>
+      <c r="B1063" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1063" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1063">
+        <v>10</v>
+      </c>
+      <c r="E1063" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1063" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1063" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1063" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1063" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1063" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1063" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1063" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1064">
+        <v>18.228999999999999</v>
+      </c>
+      <c r="B1064" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1064" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1064">
+        <v>15</v>
+      </c>
+      <c r="E1064" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1064" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1064" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1064" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1064" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1064" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1064" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1064" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1065">
+        <v>15.946</v>
+      </c>
+      <c r="B1065" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1065" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1065">
+        <v>20</v>
+      </c>
+      <c r="E1065" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1065" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1065" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1065" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1065" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1065" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1065" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1065" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1066">
+        <v>119.383</v>
+      </c>
+      <c r="B1066" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1066" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1066">
+        <v>1</v>
+      </c>
+      <c r="E1066" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1066" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1066" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1066" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1066" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1066" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1066" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1066" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1067">
+        <v>109.32599999999999</v>
+      </c>
+      <c r="B1067" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1067" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1067">
+        <v>5</v>
+      </c>
+      <c r="E1067" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1067" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1067" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1067" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1067" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1067" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1067" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1067" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1068">
+        <v>120.03400000000001</v>
+      </c>
+      <c r="B1068" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1068" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1068">
+        <v>10</v>
+      </c>
+      <c r="E1068" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1068" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1068" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1068" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1068" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1068" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1068" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1068" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1069">
+        <v>125.571</v>
+      </c>
+      <c r="B1069" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1069" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1069">
+        <v>15</v>
+      </c>
+      <c r="E1069" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1069" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1069" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1069" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1069" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1069" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1069" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1069" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1070">
+        <v>113.831</v>
+      </c>
+      <c r="B1070" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1070" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1070">
+        <v>20</v>
+      </c>
+      <c r="E1070" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1070" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1070" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1070" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1070" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1070" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1070" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1070" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed capitalization of 'both' in the mission creek data
</commit_message>
<xml_diff>
--- a/data/web_plot_digitizer_data.xlsx
+++ b/data/web_plot_digitizer_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProgramR\fuels_longevity\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20D1458C-53AF-4AC3-A546-54A4A6847833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B63C99-A40D-4CF6-995A-A1287D4B6376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6245A06B-15CE-492B-AD18-D354A95DB25A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10708" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10708" uniqueCount="103">
   <si>
     <t>variable</t>
   </si>
@@ -348,9 +348,6 @@
   </si>
   <si>
     <t>radcliffe1</t>
-  </si>
-  <si>
-    <t>both</t>
   </si>
 </sst>
 </file>
@@ -739,7 +736,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A913" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A918" sqref="A918:L1017"/>
+      <selection pane="bottomLeft" activeCell="I931" sqref="I931"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35624,7 +35621,7 @@
         <v>102</v>
       </c>
       <c r="G918" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H918" t="s">
         <v>95</v>
@@ -35662,7 +35659,7 @@
         <v>102</v>
       </c>
       <c r="G919" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H919" t="s">
         <v>95</v>
@@ -35700,7 +35697,7 @@
         <v>102</v>
       </c>
       <c r="G920" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H920" t="s">
         <v>95</v>
@@ -35738,7 +35735,7 @@
         <v>102</v>
       </c>
       <c r="G921" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H921" t="s">
         <v>95</v>
@@ -35776,7 +35773,7 @@
         <v>102</v>
       </c>
       <c r="G922" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H922" t="s">
         <v>95</v>
@@ -35814,7 +35811,7 @@
         <v>102</v>
       </c>
       <c r="G923" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H923" t="s">
         <v>95</v>
@@ -35852,7 +35849,7 @@
         <v>102</v>
       </c>
       <c r="G924" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H924" t="s">
         <v>95</v>
@@ -35890,7 +35887,7 @@
         <v>102</v>
       </c>
       <c r="G925" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H925" t="s">
         <v>95</v>
@@ -35928,7 +35925,7 @@
         <v>102</v>
       </c>
       <c r="G926" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H926" t="s">
         <v>95</v>
@@ -35966,7 +35963,7 @@
         <v>102</v>
       </c>
       <c r="G927" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H927" t="s">
         <v>95</v>
@@ -36004,7 +36001,7 @@
         <v>102</v>
       </c>
       <c r="G928" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H928" t="s">
         <v>95</v>
@@ -36042,7 +36039,7 @@
         <v>102</v>
       </c>
       <c r="G929" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H929" t="s">
         <v>95</v>
@@ -36080,7 +36077,7 @@
         <v>102</v>
       </c>
       <c r="G930" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H930" t="s">
         <v>95</v>
@@ -36118,7 +36115,7 @@
         <v>102</v>
       </c>
       <c r="G931" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H931" t="s">
         <v>95</v>
@@ -36156,7 +36153,7 @@
         <v>102</v>
       </c>
       <c r="G932" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H932" t="s">
         <v>95</v>
@@ -36194,7 +36191,7 @@
         <v>102</v>
       </c>
       <c r="G933" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H933" t="s">
         <v>95</v>
@@ -36232,7 +36229,7 @@
         <v>102</v>
       </c>
       <c r="G934" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H934" t="s">
         <v>95</v>
@@ -36270,7 +36267,7 @@
         <v>102</v>
       </c>
       <c r="G935" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H935" t="s">
         <v>95</v>
@@ -36308,7 +36305,7 @@
         <v>102</v>
       </c>
       <c r="G936" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H936" t="s">
         <v>95</v>
@@ -36346,7 +36343,7 @@
         <v>102</v>
       </c>
       <c r="G937" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H937" t="s">
         <v>95</v>
@@ -36384,7 +36381,7 @@
         <v>102</v>
       </c>
       <c r="G938" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H938" t="s">
         <v>95</v>
@@ -36422,7 +36419,7 @@
         <v>102</v>
       </c>
       <c r="G939" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H939" t="s">
         <v>95</v>
@@ -36460,7 +36457,7 @@
         <v>102</v>
       </c>
       <c r="G940" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H940" t="s">
         <v>95</v>
@@ -36498,7 +36495,7 @@
         <v>102</v>
       </c>
       <c r="G941" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H941" t="s">
         <v>95</v>
@@ -36536,7 +36533,7 @@
         <v>102</v>
       </c>
       <c r="G942" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H942" t="s">
         <v>95</v>
@@ -36574,7 +36571,7 @@
         <v>102</v>
       </c>
       <c r="G943" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H943" t="s">
         <v>95</v>
@@ -36612,7 +36609,7 @@
         <v>102</v>
       </c>
       <c r="G944" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H944" t="s">
         <v>95</v>
@@ -36650,7 +36647,7 @@
         <v>102</v>
       </c>
       <c r="G945" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H945" t="s">
         <v>95</v>
@@ -36688,7 +36685,7 @@
         <v>102</v>
       </c>
       <c r="G946" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H946" t="s">
         <v>95</v>
@@ -36726,7 +36723,7 @@
         <v>102</v>
       </c>
       <c r="G947" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H947" t="s">
         <v>95</v>
@@ -36764,7 +36761,7 @@
         <v>102</v>
       </c>
       <c r="G948" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H948" t="s">
         <v>95</v>
@@ -36802,7 +36799,7 @@
         <v>102</v>
       </c>
       <c r="G949" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H949" t="s">
         <v>95</v>
@@ -36840,7 +36837,7 @@
         <v>102</v>
       </c>
       <c r="G950" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H950" t="s">
         <v>95</v>
@@ -36878,7 +36875,7 @@
         <v>102</v>
       </c>
       <c r="G951" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H951" t="s">
         <v>95</v>
@@ -36916,7 +36913,7 @@
         <v>102</v>
       </c>
       <c r="G952" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H952" t="s">
         <v>95</v>
@@ -36954,7 +36951,7 @@
         <v>102</v>
       </c>
       <c r="G953" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H953" t="s">
         <v>95</v>
@@ -36992,7 +36989,7 @@
         <v>102</v>
       </c>
       <c r="G954" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H954" t="s">
         <v>95</v>
@@ -37030,7 +37027,7 @@
         <v>102</v>
       </c>
       <c r="G955" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H955" t="s">
         <v>95</v>
@@ -37068,7 +37065,7 @@
         <v>102</v>
       </c>
       <c r="G956" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H956" t="s">
         <v>95</v>
@@ -37106,7 +37103,7 @@
         <v>102</v>
       </c>
       <c r="G957" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H957" t="s">
         <v>95</v>
@@ -37144,7 +37141,7 @@
         <v>102</v>
       </c>
       <c r="G958" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H958" t="s">
         <v>95</v>
@@ -37182,7 +37179,7 @@
         <v>102</v>
       </c>
       <c r="G959" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H959" t="s">
         <v>95</v>
@@ -37220,7 +37217,7 @@
         <v>102</v>
       </c>
       <c r="G960" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H960" t="s">
         <v>95</v>
@@ -37258,7 +37255,7 @@
         <v>102</v>
       </c>
       <c r="G961" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H961" t="s">
         <v>95</v>
@@ -37296,7 +37293,7 @@
         <v>102</v>
       </c>
       <c r="G962" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H962" t="s">
         <v>95</v>
@@ -37334,7 +37331,7 @@
         <v>102</v>
       </c>
       <c r="G963" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H963" t="s">
         <v>95</v>
@@ -37372,7 +37369,7 @@
         <v>102</v>
       </c>
       <c r="G964" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H964" t="s">
         <v>95</v>
@@ -37410,7 +37407,7 @@
         <v>102</v>
       </c>
       <c r="G965" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H965" t="s">
         <v>95</v>
@@ -37448,7 +37445,7 @@
         <v>102</v>
       </c>
       <c r="G966" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H966" t="s">
         <v>95</v>
@@ -37486,7 +37483,7 @@
         <v>102</v>
       </c>
       <c r="G967" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H967" t="s">
         <v>95</v>
@@ -37524,7 +37521,7 @@
         <v>102</v>
       </c>
       <c r="G968" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H968" t="s">
         <v>95</v>
@@ -37562,7 +37559,7 @@
         <v>102</v>
       </c>
       <c r="G969" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H969" t="s">
         <v>95</v>
@@ -37600,7 +37597,7 @@
         <v>102</v>
       </c>
       <c r="G970" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H970" t="s">
         <v>95</v>
@@ -37638,7 +37635,7 @@
         <v>102</v>
       </c>
       <c r="G971" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H971" t="s">
         <v>95</v>
@@ -37676,7 +37673,7 @@
         <v>102</v>
       </c>
       <c r="G972" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H972" t="s">
         <v>95</v>
@@ -37714,7 +37711,7 @@
         <v>102</v>
       </c>
       <c r="G973" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H973" t="s">
         <v>95</v>
@@ -37752,7 +37749,7 @@
         <v>102</v>
       </c>
       <c r="G974" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H974" t="s">
         <v>95</v>
@@ -37790,7 +37787,7 @@
         <v>102</v>
       </c>
       <c r="G975" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H975" t="s">
         <v>95</v>
@@ -37828,7 +37825,7 @@
         <v>102</v>
       </c>
       <c r="G976" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H976" t="s">
         <v>95</v>
@@ -37866,7 +37863,7 @@
         <v>102</v>
       </c>
       <c r="G977" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H977" t="s">
         <v>95</v>
@@ -37904,7 +37901,7 @@
         <v>102</v>
       </c>
       <c r="G978" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H978" t="s">
         <v>95</v>
@@ -37942,7 +37939,7 @@
         <v>102</v>
       </c>
       <c r="G979" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H979" t="s">
         <v>95</v>
@@ -37980,7 +37977,7 @@
         <v>102</v>
       </c>
       <c r="G980" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H980" t="s">
         <v>95</v>
@@ -38018,7 +38015,7 @@
         <v>102</v>
       </c>
       <c r="G981" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H981" t="s">
         <v>95</v>
@@ -38056,7 +38053,7 @@
         <v>102</v>
       </c>
       <c r="G982" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H982" t="s">
         <v>95</v>
@@ -38094,7 +38091,7 @@
         <v>102</v>
       </c>
       <c r="G983" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H983" t="s">
         <v>95</v>
@@ -38132,7 +38129,7 @@
         <v>102</v>
       </c>
       <c r="G984" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H984" t="s">
         <v>95</v>
@@ -38170,7 +38167,7 @@
         <v>102</v>
       </c>
       <c r="G985" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H985" t="s">
         <v>95</v>
@@ -38208,7 +38205,7 @@
         <v>102</v>
       </c>
       <c r="G986" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H986" t="s">
         <v>95</v>
@@ -38246,7 +38243,7 @@
         <v>102</v>
       </c>
       <c r="G987" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H987" t="s">
         <v>95</v>
@@ -38284,7 +38281,7 @@
         <v>102</v>
       </c>
       <c r="G988" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H988" t="s">
         <v>95</v>
@@ -38322,7 +38319,7 @@
         <v>102</v>
       </c>
       <c r="G989" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H989" t="s">
         <v>95</v>
@@ -38360,7 +38357,7 @@
         <v>102</v>
       </c>
       <c r="G990" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H990" t="s">
         <v>95</v>
@@ -38398,7 +38395,7 @@
         <v>102</v>
       </c>
       <c r="G991" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H991" t="s">
         <v>95</v>
@@ -38436,7 +38433,7 @@
         <v>102</v>
       </c>
       <c r="G992" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H992" t="s">
         <v>95</v>
@@ -38474,7 +38471,7 @@
         <v>102</v>
       </c>
       <c r="G993" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H993" t="s">
         <v>95</v>
@@ -38512,7 +38509,7 @@
         <v>102</v>
       </c>
       <c r="G994" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H994" t="s">
         <v>95</v>
@@ -38550,7 +38547,7 @@
         <v>102</v>
       </c>
       <c r="G995" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H995" t="s">
         <v>95</v>
@@ -38588,7 +38585,7 @@
         <v>102</v>
       </c>
       <c r="G996" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H996" t="s">
         <v>95</v>
@@ -38626,7 +38623,7 @@
         <v>102</v>
       </c>
       <c r="G997" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H997" t="s">
         <v>95</v>
@@ -38664,7 +38661,7 @@
         <v>102</v>
       </c>
       <c r="G998" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H998" t="s">
         <v>95</v>
@@ -38702,7 +38699,7 @@
         <v>102</v>
       </c>
       <c r="G999" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H999" t="s">
         <v>95</v>
@@ -38740,7 +38737,7 @@
         <v>102</v>
       </c>
       <c r="G1000" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1000" t="s">
         <v>95</v>
@@ -38778,7 +38775,7 @@
         <v>102</v>
       </c>
       <c r="G1001" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1001" t="s">
         <v>95</v>
@@ -38816,7 +38813,7 @@
         <v>102</v>
       </c>
       <c r="G1002" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1002" t="s">
         <v>95</v>
@@ -38854,7 +38851,7 @@
         <v>102</v>
       </c>
       <c r="G1003" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1003" t="s">
         <v>95</v>
@@ -38892,7 +38889,7 @@
         <v>102</v>
       </c>
       <c r="G1004" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1004" t="s">
         <v>95</v>
@@ -38930,7 +38927,7 @@
         <v>102</v>
       </c>
       <c r="G1005" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1005" t="s">
         <v>95</v>
@@ -38968,7 +38965,7 @@
         <v>102</v>
       </c>
       <c r="G1006" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1006" t="s">
         <v>95</v>
@@ -39006,7 +39003,7 @@
         <v>102</v>
       </c>
       <c r="G1007" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1007" t="s">
         <v>95</v>
@@ -39044,7 +39041,7 @@
         <v>102</v>
       </c>
       <c r="G1008" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1008" t="s">
         <v>95</v>
@@ -39082,7 +39079,7 @@
         <v>102</v>
       </c>
       <c r="G1009" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1009" t="s">
         <v>95</v>
@@ -39120,7 +39117,7 @@
         <v>102</v>
       </c>
       <c r="G1010" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1010" t="s">
         <v>95</v>
@@ -39158,7 +39155,7 @@
         <v>102</v>
       </c>
       <c r="G1011" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1011" t="s">
         <v>95</v>
@@ -39196,7 +39193,7 @@
         <v>102</v>
       </c>
       <c r="G1012" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1012" t="s">
         <v>95</v>
@@ -39234,7 +39231,7 @@
         <v>102</v>
       </c>
       <c r="G1013" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1013" t="s">
         <v>95</v>
@@ -39272,7 +39269,7 @@
         <v>102</v>
       </c>
       <c r="G1014" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1014" t="s">
         <v>95</v>
@@ -39310,7 +39307,7 @@
         <v>102</v>
       </c>
       <c r="G1015" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1015" t="s">
         <v>95</v>
@@ -39348,7 +39345,7 @@
         <v>102</v>
       </c>
       <c r="G1016" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1016" t="s">
         <v>95</v>
@@ -39386,7 +39383,7 @@
         <v>102</v>
       </c>
       <c r="G1017" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1017" t="s">
         <v>95</v>

</xml_diff>